<commit_message>
added two single infrastructure graphs
git-svn-id: file://localhost/tmp/svn2git/svn@6325 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="80" windowWidth="27220" windowHeight="28280" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="23160" yWindow="80" windowWidth="27220" windowHeight="28280" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="156">
   <si>
     <t>bfast</t>
   </si>
@@ -478,9 +478,6 @@
     <t>Staging</t>
   </si>
   <si>
-    <t>BJ XSEDE</t>
-  </si>
-  <si>
     <t>EGI</t>
   </si>
   <si>
@@ -488,9 +485,6 @@
   </si>
   <si>
     <t>Allocation</t>
-  </si>
-  <si>
-    <t>Mean</t>
   </si>
   <si>
     <t>Stdev</t>
@@ -506,9 +500,6 @@
   </si>
   <si>
     <t>Queuing</t>
-  </si>
-  <si>
-    <t>BJ FG</t>
   </si>
   <si>
     <t>Total (w/o Download)</t>
@@ -540,13 +531,28 @@
   <si>
     <t>Check</t>
   </si>
+  <si>
+    <t xml:space="preserve">Queuing </t>
+  </si>
+  <si>
+    <t>in min</t>
+  </si>
+  <si>
+    <t>Overhead</t>
+  </si>
+  <si>
+    <t>XSEDE</t>
+  </si>
+  <si>
+    <t>FutureGrid</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -617,7 +623,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -667,11 +673,24 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -684,11 +703,13 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -744,8 +765,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -764,6 +797,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -776,32 +828,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="67">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -829,6 +861,12 @@
     <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -856,6 +894,12 @@
     <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -1054,11 +1098,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="571649432"/>
-        <c:axId val="571645928"/>
+        <c:axId val="794179944"/>
+        <c:axId val="794188520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571649432"/>
+        <c:axId val="794179944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1112,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571645928"/>
+        <c:crossAx val="794188520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1076,7 +1120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571645928"/>
+        <c:axId val="794188520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,7 +1131,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571649432"/>
+        <c:crossAx val="794179944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1385,11 +1429,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="571624184"/>
-        <c:axId val="571618440"/>
+        <c:axId val="793663896"/>
+        <c:axId val="793669624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571624184"/>
+        <c:axId val="793663896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1423,7 +1467,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571618440"/>
+        <c:crossAx val="793669624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1431,7 +1475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571618440"/>
+        <c:axId val="793669624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1442,7 +1486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571624184"/>
+        <c:crossAx val="793663896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1755,11 +1799,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="571559400"/>
-        <c:axId val="571553672"/>
+        <c:axId val="794234312"/>
+        <c:axId val="794240024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571559400"/>
+        <c:axId val="794234312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1793,7 +1837,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571553672"/>
+        <c:crossAx val="794240024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1801,7 +1845,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571553672"/>
+        <c:axId val="794240024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1831,7 +1875,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571559400"/>
+        <c:crossAx val="794234312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1845,6 +1889,739 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="109"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="9"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>128 BFAST Match Tasks on Different Infrastructures (No Staging)</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Queueing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Total!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EGI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OSG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Total!$B$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.2861972593</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.684850489966666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.79019803333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.87222222222222</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Staging</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Total!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EGI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OSG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Total!$B$13:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.46417735</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.60000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Overhead</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Total!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EGI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OSG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Total!$B$14:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.007059797366708</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.764614890033328</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.33331592830655E-9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.00555555555555998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Bfast</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Total!$B$17:$E$17</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.107306088902948</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.459406221078215</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>23.07872113659127</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>56.38540574901877</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Total!$B$17:$E$17</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.107306088902948</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.459406221078215</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>23.07872113659127</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>56.38540574901877</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Total!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EGI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OSG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Total!$B$15:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>31.60781249999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.81484375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.48998550166667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.15555555555557</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="793041960"/>
+        <c:axId val="872448136"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="793041960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="872448136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="872448136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:t>Runtime (in min)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="793041960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="109"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="9"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>128 BFAST Match Tasks</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> on Different Infrastructures (No Staging)</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Queueing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Total!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EGI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OSG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Total!$B$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.2861972593</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.684850489966666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.79019803333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.87222222222222</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Overhead</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Total!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EGI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OSG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Total!$B$14:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.007059797366708</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.764614890033328</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.33331592830655E-9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.00555555555555998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Bfast</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Total!$B$4:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>EGI</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OSG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Total!$B$15:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>31.60781249999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.81484375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.48998550166667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.15555555555557</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="655922664"/>
+        <c:axId val="873718616"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="655922664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="873718616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="873718616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:t>Runtime (in min)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="655922664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1945,6 +2722,73 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -17701,6 +18545,108 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="I54:K65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Mittelwert - Kraken" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - Kraken2" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I4:K21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
@@ -17800,7 +18746,7 @@
     <dataField name="STABW - Kraken" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="11">
-    <format dxfId="10">
+    <format dxfId="11">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -17812,7 +18758,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="10">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -17821,7 +18767,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="9">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -17836,10 +18782,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="8">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -17848,7 +18794,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -17857,7 +18803,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -17869,7 +18815,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -17878,7 +18824,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -17890,7 +18836,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -17899,7 +18845,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -17910,108 +18856,6 @@
           </reference>
         </references>
       </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="I54:K65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="10">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Mittelwert - Kraken" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - Kraken2" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="11">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -18601,16 +19445,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
@@ -51028,30 +51872,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="G3" s="18" t="s">
-        <v>144</v>
+      <c r="G3" s="14" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -51208,7 +52052,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B11">
         <f>STDEV(B4:B8)</f>
@@ -51249,44 +52093,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16">
-      <c r="A3" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="32" t="s">
+      <c r="A3" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="32" t="s">
+      <c r="F3" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="I3" s="24" t="s">
         <v>142</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="I3" s="31" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16">
@@ -51295,27 +52140,27 @@
         <v>936.99999999999943</v>
       </c>
       <c r="B4" s="7">
+        <f>0.0924421296296296*24*60*60</f>
+        <v>7986.9999999999973</v>
+      </c>
+      <c r="C4" s="15">
+        <f>0.155601851851852*60*60*24</f>
+        <v>13444.000000000013</v>
+      </c>
+      <c r="D4" s="15">
+        <f>0.00760416666666667*60*60*24</f>
+        <v>657.00000000000023</v>
+      </c>
+      <c r="E4" s="7">
         <f>0.174039351851852*24*60*60</f>
         <v>15037.000000000015</v>
       </c>
-      <c r="C4" s="7">
-        <f>0.0924421296296296*24*60*60</f>
-        <v>7986.9999999999973</v>
-      </c>
-      <c r="D4" s="19">
-        <f>0.155601851851852*60*60*24</f>
-        <v>13444.000000000013</v>
-      </c>
-      <c r="E4" s="19">
-        <f>0.00760416666666667*60*60*24</f>
-        <v>657.00000000000023</v>
-      </c>
-      <c r="F4" s="19">
-        <f>E4+D4+A4</f>
+      <c r="F4" s="15">
+        <f>D4+C4+A4</f>
         <v>15038.000000000013</v>
       </c>
-      <c r="I4" s="31" t="s">
-        <v>146</v>
+      <c r="I4" s="24" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16">
@@ -51324,27 +52169,27 @@
         <v>916.00000000000409</v>
       </c>
       <c r="B5" s="7">
+        <f>0.0319560185185185*24*60*60</f>
+        <v>2760.9999999999982</v>
+      </c>
+      <c r="C5" s="15">
+        <f>0.0340856481481481*60*60*24</f>
+        <v>2944.9999999999964</v>
+      </c>
+      <c r="D5" s="15">
+        <f>0.00862268518518518*60*60*24</f>
+        <v>744.99999999999943</v>
+      </c>
+      <c r="E5" s="7">
         <f>0.0533101851851852*24*60*60</f>
         <v>4606.0000000000009</v>
       </c>
-      <c r="C5" s="7">
-        <f>0.0319560185185185*24*60*60</f>
-        <v>2760.9999999999982</v>
-      </c>
-      <c r="D5" s="19">
-        <f>0.0340856481481481*60*60*24</f>
-        <v>2944.9999999999964</v>
-      </c>
-      <c r="E5" s="19">
-        <f>0.00862268518518518*60*60*24</f>
-        <v>744.99999999999943</v>
-      </c>
-      <c r="F5" s="19">
-        <f t="shared" ref="F5:F6" si="0">E5+D5+A5</f>
+      <c r="F5" s="15">
+        <f>D5+C5+A5</f>
         <v>4606</v>
       </c>
-      <c r="I5" s="31" t="s">
-        <v>147</v>
+      <c r="I5" s="24" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -51353,92 +52198,92 @@
         <v>874.99999999999875</v>
       </c>
       <c r="B6" s="7">
+        <f>0.0191203703703704*24*60*60</f>
+        <v>1652.0000000000025</v>
+      </c>
+      <c r="C6" s="15">
+        <f>0.00947916666666667*60*60*24</f>
+        <v>819.00000000000034</v>
+      </c>
+      <c r="D6" s="15">
+        <f>0.00850694444444444*60*60*24</f>
+        <v>734.99999999999966</v>
+      </c>
+      <c r="E6" s="7">
         <f>0.0281134259259259*24*60*60</f>
         <v>2428.9999999999973</v>
       </c>
-      <c r="C6" s="7">
-        <f>0.0191203703703704*24*60*60</f>
-        <v>1652.0000000000025</v>
-      </c>
-      <c r="D6" s="19">
-        <f>0.00947916666666667*60*60*24</f>
-        <v>819.00000000000034</v>
-      </c>
-      <c r="E6" s="19">
-        <f>0.00850694444444444*60*60*24</f>
-        <v>734.99999999999966</v>
-      </c>
-      <c r="F6" s="19">
-        <f t="shared" si="0"/>
+      <c r="F6" s="15">
+        <f>D6+C6+A6</f>
         <v>2428.9999999999986</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16">
-      <c r="I7" s="31" t="s">
-        <v>148</v>
+      <c r="I7" s="24" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="33">
+      <c r="A8" s="26">
         <f>AVERAGE(A4:A6)</f>
         <v>909.33333333333405</v>
       </c>
-      <c r="B8" s="33">
-        <f t="shared" ref="B8:C8" si="1">AVERAGE(B4:B6)</f>
+      <c r="B8" s="26">
+        <f t="shared" ref="B8" si="0">AVERAGE(B4:B6)</f>
+        <v>4133.333333333333</v>
+      </c>
+      <c r="C8" s="16">
+        <f>AVERAGE(C4:C6)</f>
+        <v>5736.0000000000027</v>
+      </c>
+      <c r="D8" s="16">
+        <f>AVERAGE(D4:D6)</f>
+        <v>712.33333333333303</v>
+      </c>
+      <c r="E8" s="26">
+        <f>AVERAGE(E4:E6)</f>
         <v>7357.3333333333367</v>
       </c>
-      <c r="C8" s="33">
-        <f t="shared" si="1"/>
-        <v>4133.333333333333</v>
-      </c>
-      <c r="D8" s="20">
-        <f t="shared" ref="D5:D9" si="2">C8-A8</f>
-        <v>3223.9999999999991</v>
-      </c>
-      <c r="E8" s="20">
-        <f t="shared" ref="E5:E9" si="3">B8-C8</f>
-        <v>3224.0000000000036</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16">
-      <c r="A9" s="33">
+      <c r="A9" s="26">
         <f>STDEV(A4:A6)</f>
         <v>31.533051443420248</v>
       </c>
-      <c r="B9" s="33">
-        <f t="shared" ref="B9:C9" si="4">STDEV(B4:B6)</f>
+      <c r="B9" s="26">
+        <f t="shared" ref="B9" si="1">STDEV(B4:B6)</f>
+        <v>3383.1243449411259</v>
+      </c>
+      <c r="C9" s="16">
+        <f>STDEV(C4:C6)</f>
+        <v>6759.4317068818818</v>
+      </c>
+      <c r="D9" s="16">
+        <f>STDEV(D4:D6)</f>
+        <v>48.180217240412013</v>
+      </c>
+      <c r="E9" s="26">
+        <f>STDEV(E4:E6)</f>
         <v>6739.2723890145198</v>
       </c>
-      <c r="C9" s="33">
-        <f t="shared" si="4"/>
-        <v>3383.1243449411259</v>
-      </c>
-      <c r="D9" s="20">
-        <f t="shared" si="2"/>
-        <v>3351.5912934977055</v>
-      </c>
-      <c r="E9" s="20">
-        <f t="shared" si="3"/>
-        <v>3356.148044073394</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I9" s="31" t="s">
-        <v>149</v>
+        <v>136</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16">
-      <c r="I10" s="31" t="s">
-        <v>150</v>
+      <c r="I10" s="24" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16">
-      <c r="I11" s="31" t="s">
-        <v>151</v>
+      <c r="I11" s="24" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -51454,22 +52299,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R48" sqref="R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -51477,76 +52321,76 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="10"/>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="23" t="s">
+      <c r="E4" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="24" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="27">
+      <c r="A5" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="20">
         <f>BigJob!O28</f>
         <v>77.171835557999998</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="22">
         <f>BigJob!N28</f>
         <v>101.09102939799999</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="20">
         <f>Diane!B10</f>
         <v>3167.4118819999999</v>
       </c>
-      <c r="E5" s="24">
-        <f>Condor!C8-Condor!A8</f>
-        <v>3223.9999999999991</v>
+      <c r="E5" s="22">
+        <f>Condor!D8</f>
+        <v>712.33333333333303</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="32">
         <v>0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="10">
         <v>0</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="21">
         <f>Diane!C10</f>
         <v>4707.850641</v>
       </c>
-      <c r="E6" s="10">
-        <f>Condor!B8-Condor!C8</f>
-        <v>3224.0000000000036</v>
+      <c r="E6" s="23">
+        <f>Condor!C8</f>
+        <v>5736.0000000000027</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="21">
         <f>BFAST!J63*24*60*60</f>
         <v>1896.4687499999982</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="23">
         <f>BFAST!J39*60*60*24</f>
         <v>1068.8906250000002</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="21">
         <f>Diane!D10</f>
         <v>809.39913009999998</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="23">
         <f>Condor!A8</f>
         <v>909.33333333333405</v>
       </c>
@@ -51555,47 +52399,189 @@
       <c r="A8" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="21">
         <f>BigJob!R28</f>
         <v>2214.0641734000005</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="23">
         <f>BigJob!Q28</f>
         <v>1695.8585478</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="21">
         <f>Diane!F10-Diane!E10</f>
         <v>8684.6616528400009</v>
       </c>
-      <c r="E8" s="30">
-        <f>Condor!B8</f>
+      <c r="E8" s="23">
+        <f>Condor!E8</f>
         <v>7357.3333333333367</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B9" s="20">
+        <v>138</v>
+      </c>
+      <c r="B9" s="21">
         <f>BigJob!AA28</f>
         <v>66.438365334176908</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="23">
         <f>BigJob!Z28</f>
         <v>267.5643732646929</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="21">
         <f>Diane!G11</f>
         <v>1384.7232681954761</v>
       </c>
-      <c r="E9" s="20">
-        <f>Condor!C9</f>
+      <c r="E9" s="16">
+        <f>Condor!B9</f>
         <v>3383.1243449411259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" s="21"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" ht="16" thickBot="1">
+      <c r="A11" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" s="33"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:5" ht="16" thickTop="1">
+      <c r="A12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="34">
+        <f>B5/60</f>
+        <v>1.2861972593</v>
+      </c>
+      <c r="C12" s="15">
+        <f t="shared" ref="C12:E12" si="0">C5/60</f>
+        <v>1.6848504899666665</v>
+      </c>
+      <c r="D12" s="34">
+        <f t="shared" si="0"/>
+        <v>52.790198033333333</v>
+      </c>
+      <c r="E12" s="15">
+        <f t="shared" si="0"/>
+        <v>11.872222222222216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="34">
+        <f t="shared" ref="B13:E13" si="1">B6/60</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="34">
+        <f t="shared" si="1"/>
+        <v>78.46417735</v>
+      </c>
+      <c r="E13" s="15">
+        <f t="shared" si="1"/>
+        <v>95.600000000000051</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="34">
+        <f>B16-B15-B12-B13</f>
+        <v>4.0070597973667077</v>
+      </c>
+      <c r="C14" s="15">
+        <f t="shared" ref="C14:E14" si="2">C16-C15-C12-C13</f>
+        <v>8.7646148900333287</v>
+      </c>
+      <c r="D14" s="34">
+        <f t="shared" si="2"/>
+        <v>-4.333315928306547E-9</v>
+      </c>
+      <c r="E14" s="15">
+        <f t="shared" si="2"/>
+        <v>-5.5555555555599767E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" s="34">
+        <f t="shared" ref="B15:E15" si="3">B7/60</f>
+        <v>31.607812499999969</v>
+      </c>
+      <c r="C15" s="15">
+        <f t="shared" si="3"/>
+        <v>17.814843750000005</v>
+      </c>
+      <c r="D15" s="34">
+        <f t="shared" si="3"/>
+        <v>13.489985501666666</v>
+      </c>
+      <c r="E15" s="15">
+        <f t="shared" si="3"/>
+        <v>15.155555555555567</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="34">
+        <f t="shared" ref="B16:E17" si="4">B8/60</f>
+        <v>36.901069556666677</v>
+      </c>
+      <c r="C16" s="15">
+        <f t="shared" si="4"/>
+        <v>28.264309130000001</v>
+      </c>
+      <c r="D16" s="34">
+        <f t="shared" si="4"/>
+        <v>144.74436088066668</v>
+      </c>
+      <c r="E16" s="15">
+        <f t="shared" si="4"/>
+        <v>122.62222222222228</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" s="34">
+        <f t="shared" si="4"/>
+        <v>1.1073060889029485</v>
+      </c>
+      <c r="C17" s="15">
+        <f t="shared" si="4"/>
+        <v>4.4594062210782148</v>
+      </c>
+      <c r="D17" s="34">
+        <f t="shared" si="4"/>
+        <v>23.078721136591266</v>
+      </c>
+      <c r="E17" s="15">
+        <f t="shared" si="4"/>
+        <v>56.385405749018766</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
work on performance section
git-svn-id: file://localhost/tmp/svn2git/svn@6327 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="158">
   <si>
     <t>bfast</t>
   </si>
@@ -545,6 +545,12 @@
   </si>
   <si>
     <t>FutureGrid</t>
+  </si>
+  <si>
+    <t>Without Staging</t>
+  </si>
+  <si>
+    <t>With Staging</t>
   </si>
 </sst>
 </file>
@@ -1911,31 +1917,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>128 BFAST Match Tasks on Different Infrastructures (No Staging)</a:t>
-            </a:r>
-            <a:endParaRPr lang="de-DE">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2218,7 +2200,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1"/>
+              <a:defRPr sz="2000" b="1">
+                <a:latin typeface="Times"/>
+                <a:cs typeface="Times"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -2234,11 +2219,18 @@
         <c:axId val="872448136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="180.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2246,10 +2238,16 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600"/>
+                  <a:defRPr sz="2000">
+                    <a:latin typeface="Times"/>
+                    <a:cs typeface="Times"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:rPr lang="de-DE" sz="2000">
+                    <a:latin typeface="Times"/>
+                    <a:cs typeface="Times"/>
+                  </a:rPr>
                   <a:t>Runtime (in min)</a:t>
                 </a:r>
               </a:p>
@@ -2267,7 +2265,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600"/>
+              <a:defRPr sz="2000">
+                <a:latin typeface="Times"/>
+                <a:cs typeface="Times"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -2328,31 +2329,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>128 BFAST Match Tasks</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> on Different Infrastructures (No Staging)</a:t>
-            </a:r>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2539,7 +2516,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1"/>
+              <a:defRPr sz="2000" b="1">
+                <a:latin typeface="Times"/>
+                <a:cs typeface="Times"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -2559,7 +2539,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2567,10 +2546,16 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600"/>
+                  <a:defRPr sz="2000">
+                    <a:latin typeface="Times"/>
+                    <a:cs typeface="Times"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:rPr lang="de-DE" sz="2000">
+                    <a:latin typeface="Times"/>
+                    <a:cs typeface="Times"/>
+                  </a:rPr>
                   <a:t>Runtime (in min)</a:t>
                 </a:r>
               </a:p>
@@ -2588,7 +2573,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600"/>
+              <a:defRPr sz="2000">
+                <a:latin typeface="Times"/>
+                <a:cs typeface="Times"/>
+              </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -2765,15 +2753,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
+      <xdr:colOff>641350</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -52094,7 +52082,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -52299,10 +52287,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R48" sqref="R48"/>
+      <selection activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -52311,15 +52299,18 @@
     <col min="4" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="2"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G2" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="10"/>
       <c r="B4" s="18" t="s">
         <v>154</v>
@@ -52334,7 +52325,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5" s="19" t="s">
         <v>140</v>
       </c>
@@ -52355,7 +52346,7 @@
         <v>712.33333333333303</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="10" t="s">
         <v>132</v>
       </c>
@@ -52374,7 +52365,7 @@
         <v>5736.0000000000027</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>128</v>
       </c>
@@ -52395,7 +52386,7 @@
         <v>909.33333333333405</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -52416,7 +52407,7 @@
         <v>7357.3333333333367</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -52437,13 +52428,13 @@
         <v>3383.1243449411259</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="B10" s="21"/>
       <c r="C10" s="23"/>
       <c r="D10" s="21"/>
       <c r="E10" s="16"/>
     </row>
-    <row r="11" spans="1:5" ht="16" thickBot="1">
+    <row r="11" spans="1:7" ht="16" thickBot="1">
       <c r="A11" s="31" t="s">
         <v>152</v>
       </c>
@@ -52452,7 +52443,7 @@
       <c r="D11" s="33"/>
       <c r="E11" s="31"/>
     </row>
-    <row r="12" spans="1:5" ht="16" thickTop="1">
+    <row r="12" spans="1:7" ht="16" thickTop="1">
       <c r="A12" t="s">
         <v>151</v>
       </c>
@@ -52473,7 +52464,7 @@
         <v>11.872222222222216</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:7">
       <c r="A13" s="10" t="s">
         <v>132</v>
       </c>
@@ -52494,7 +52485,7 @@
         <v>95.600000000000051</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -52515,7 +52506,7 @@
         <v>-5.5555555555599767E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -52536,7 +52527,7 @@
         <v>15.155555555555567</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -52576,6 +52567,11 @@
       <c r="E17" s="15">
         <f t="shared" si="4"/>
         <v>56.385405749018766</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7">
+      <c r="G35" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added placeholder figure for interop tests
git-svn-id: file://localhost/tmp/svn2git/svn@6330 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="80" windowWidth="27220" windowHeight="28280" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="23160" yWindow="80" windowWidth="27220" windowHeight="28280" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="Raw (BJ interop)" sheetId="14" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="data_interop" localSheetId="6">'Raw (BJ interop)'!$A$1:$J$33</definedName>
     <definedName name="daten" localSheetId="1">BigJob!$A$1:$J$64</definedName>
     <definedName name="daten_1" localSheetId="5">'Raw (BJ)'!$A$1:$J$109</definedName>
   </definedNames>
@@ -25,6 +26,7 @@
     <pivotCache cacheId="1" r:id="rId9"/>
     <pivotCache cacheId="2" r:id="rId10"/>
     <pivotCache cacheId="3" r:id="rId11"/>
+    <pivotCache cacheId="8" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -36,7 +38,14 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="daten.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="1" name="data-interop.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:data-interop.csv" comma="1">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="daten.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields count="10">
         <textField/>
@@ -52,21 +61,21 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="daten.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="daten.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="daten.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="daten.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="daten.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="daten.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
@@ -77,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="195">
   <si>
     <t>bfast</t>
   </si>
@@ -552,6 +561,117 @@
   <si>
     <t>With Staging</t>
   </si>
+  <si>
+    <t>bigjob:bj-8267ba3c-442a-11e1-bedf-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-83fadb7c-442a-11e1-bedf-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-d1aa679a-442d-11e1-bedf-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-d35cf986-442d-11e1-bedf-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-90023832-4431-11e1-bedf-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-91314ec8-4431-11e1-bedf-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-e85831a0-4434-11e1-bedf-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-e9f38ab4-4434-11e1-bedf-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-367333dc-4438-11e1-bedf-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-3781b0a0-4438-11e1-bedf-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-55be3e1a-4408-11e1-a01d-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-cdcedad6-4408-11e1-a01d-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-67ecf490-4265-11e1-97c5-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-a56d1458-4265-11e1-97c5-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-b3b495b0-4268-11e1-97c5-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-b4e1875e-4268-11e1-97c5-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-ccdb55da-426b-11e1-97c5-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-d0fec1e2-426b-11e1-97c5-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-f4212cde-426e-11e1-97c5-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-f54a8b00-426e-11e1-97c5-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-10d55d98-4272-11e1-97c5-00003eb40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-11fc32b4-4272-11e1-97c5-00003eb40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-afd64bd8-421c-11e1-bbbe-00003ea40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-b19a635a-421c-11e1-bbbe-00003ea40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-4c3490cc-4220-11e1-bbbe-00003ea40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-4d36140a-4220-11e1-bbbe-00003ea40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-88c8c0fa-4223-11e1-bbbe-00003ea40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-89fe8ec8-4223-11e1-bbbe-00003ea40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-a9a184f8-4226-11e1-bbbe-00003ea40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-aaabf2fc-4226-11e1-bbbe-00003ea40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-d4c9ef3c-4229-11e1-bbbe-00003ea40000:localhost</t>
+  </si>
+  <si>
+    <t>bigjob:bj-d5d060f0-4229-11e1-bbbe-00003ea40000:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>Mittelwert - Total Runtime</t>
+  </si>
+  <si>
+    <t>STABW - Total Runtime</t>
+  </si>
+  <si>
+    <t>STABW - Queuing Time</t>
+  </si>
+  <si>
+    <t>XSEDE/FutureGrid</t>
+  </si>
+  <si>
+    <t>EGI/FutureGrid</t>
+  </si>
 </sst>
 </file>
 
@@ -629,7 +749,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -692,6 +812,17 @@
       <left/>
       <right/>
       <top style="thin">
+        <color theme="6" tint="0.79998168889431442"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="double">
@@ -715,7 +846,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -783,8 +914,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -834,12 +975,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="77">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -873,6 +1016,11 @@
     <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -906,6 +1054,11 @@
     <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -2618,6 +2771,210 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="117"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="17"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>India</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0010_XSEDE/FutureGrid</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Raw (BJ interop)'!$P$13:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>945.1709057545624</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Kraken</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>_x0010_XSEDE/FutureGrid</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Raw (BJ interop)'!$P$14:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1552.19749806875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="878731640"/>
+        <c:axId val="878768152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="878731640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000">
+                <a:latin typeface="Times"/>
+                <a:cs typeface="Times"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="878768152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="878768152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000">
+                    <a:latin typeface="Times"/>
+                    <a:cs typeface="Times"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="2000">
+                    <a:latin typeface="Times"/>
+                    <a:cs typeface="Times"/>
+                  </a:rPr>
+                  <a:t>Runtime (in sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000">
+                <a:latin typeface="Times"/>
+                <a:cs typeface="Times"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="878731640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000">
+              <a:latin typeface="Times"/>
+              <a:cs typeface="Times"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2777,6 +3134,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2971,6 +3363,54 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="40929.651928703701" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="32">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:J33" sheet="Raw (BJ interop)"/>
+  </cacheSource>
+  <cacheFields count="10">
+    <cacheField name="Run" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="4"/>
+    </cacheField>
+    <cacheField name="BJ" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="#Nodes" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="64" maxValue="264"/>
+    </cacheField>
+    <cacheField name="#cores/node" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="8" maxValue="12"/>
+    </cacheField>
+    <cacheField name="#jobs" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="64" maxValue="64"/>
+    </cacheField>
+    <cacheField name="Queuing Time" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="20.1079881191" maxValue="2293.8809878799998"/>
+    </cacheField>
+    <cacheField name="BJ Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="748.04140806199996" maxValue="3820.9009029899998"/>
+    </cacheField>
+    <cacheField name="Total Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1321.3276550800001" maxValue="3824.6060969800001"/>
+    </cacheField>
+    <cacheField name="Coordination URL" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="LRMS URL" numFmtId="0">
+      <sharedItems count="2">
+        <s v="xt5torque://localhost/"/>
+        <s v="pbs-ssh://luckow@india.futuregrid.org"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="202">
   <r>
@@ -18528,6 +18968,395 @@
     <m/>
     <x v="2"/>
     <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="32">
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-8267ba3c-442a-11e1-bedf-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="39.167788028700002"/>
+    <n v="1413.31066394"/>
+    <n v="1417.01772809"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-83fadb7c-442a-11e1-bedf-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="21.497041940700001"/>
+    <n v="947.18463110899995"/>
+    <n v="1417.01772809"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-d1aa679a-442d-11e1-bedf-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="45.065774202299998"/>
+    <n v="1600.3404600599999"/>
+    <n v="1604.0428981800001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-d35cf986-442d-11e1-bedf-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="21.5378801823"/>
+    <n v="1005.3648190500001"/>
+    <n v="1604.0428981800001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-90023832-4431-11e1-bedf-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="38.198520183600003"/>
+    <n v="1429.23286009"/>
+    <n v="1432.9367761599999"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-91314ec8-4431-11e1-bedf-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="20.537039041500002"/>
+    <n v="910.54238605499995"/>
+    <n v="1432.9367761599999"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="bigjob:bj-e85831a0-4434-11e1-bedf-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="50.490038871800003"/>
+    <n v="1412.80108595"/>
+    <n v="1416.50474381"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="bigjob:bj-e9f38ab4-4434-11e1-bedf-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="21.081934928900001"/>
+    <n v="946.83650994300001"/>
+    <n v="1416.50474381"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="bigjob:bj-367333dc-4438-11e1-bedf-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="57.089904069900001"/>
+    <n v="1396.3976569199999"/>
+    <n v="1400.0998389700001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="bigjob:bj-3781b0a0-4438-11e1-bedf-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="21.823041915899999"/>
+    <n v="954.02606391899997"/>
+    <n v="1400.0998389700001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-55be3e1a-4408-11e1-a01d-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="2293.8809878799998"/>
+    <n v="3820.9009029899998"/>
+    <n v="3824.6060969800001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-cdcedad6-4408-11e1-a01d-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="220.97108697900001"/>
+    <n v="1228.8441650899999"/>
+    <n v="3824.6060969800001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-67ecf490-4265-11e1-97c5-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="122.449388981"/>
+    <n v="1408.3830029999999"/>
+    <n v="1412.0865111400001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-a56d1458-4265-11e1-97c5-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="122.50563097"/>
+    <n v="1059.7851810499999"/>
+    <n v="1412.0865111400001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-b3b495b0-4268-11e1-97c5-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="32.246130943300003"/>
+    <n v="1323.8348290900001"/>
+    <n v="1327.5373809299999"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-b4e1875e-4268-11e1-97c5-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="20.4135661125"/>
+    <n v="951.78088307400003"/>
+    <n v="1327.5373809299999"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-ccdb55da-426b-11e1-97c5-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="31.450355052900001"/>
+    <n v="1346.9226479500001"/>
+    <n v="1350.6255128400001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-d0fec1e2-426b-11e1-97c5-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="25.5253288746"/>
+    <n v="875.02339291600003"/>
+    <n v="1350.6255128400001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="bigjob:bj-f4212cde-426e-11e1-97c5-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="32.142376899699997"/>
+    <n v="1329.398911"/>
+    <n v="1333.10122299"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="bigjob:bj-f54a8b00-426e-11e1-97c5-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="20.341579914099999"/>
+    <n v="963.28213095700005"/>
+    <n v="1333.10122299"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="bigjob:bj-10d55d98-4272-11e1-97c5-00003eb40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="32.134410858199999"/>
+    <n v="1317.6233119999999"/>
+    <n v="1321.3276550800001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="bigjob:bj-11fc32b4-4272-11e1-97c5-00003eb40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="20.338257074400001"/>
+    <n v="922.17073392899999"/>
+    <n v="1321.3276550800001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-afd64bd8-421c-11e1-bbbe-00003ea40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="62.763838052700002"/>
+    <n v="1543.42536402"/>
+    <n v="1547.13568902"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-b19a635a-421c-11e1-bbbe-00003ea40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="21.520488977399999"/>
+    <n v="748.04140806199996"/>
+    <n v="1547.13568902"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-4c3490cc-4220-11e1-bbbe-00003ea40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="37.778441190700001"/>
+    <n v="1383.16831303"/>
+    <n v="1386.8724072"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-4d36140a-4220-11e1-bbbe-00003ea40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="20.1079881191"/>
+    <n v="787.46557998699996"/>
+    <n v="1386.8724072"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-88c8c0fa-4223-11e1-bbbe-00003ea40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="26.5749640465"/>
+    <n v="1336.5342540700001"/>
+    <n v="1340.23782396"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-89fe8ec8-4223-11e1-bbbe-00003ea40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="20.647578954699998"/>
+    <n v="864.43439006799997"/>
+    <n v="1340.23782396"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="bigjob:bj-a9a184f8-4226-11e1-bbbe-00003ea40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="32.454650878899997"/>
+    <n v="1354.0647489999999"/>
+    <n v="1357.76691985"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <s v="bigjob:bj-aaabf2fc-4226-11e1-bbbe-00003ea40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="20.653827905699998"/>
+    <n v="981.99814295800002"/>
+    <n v="1357.76691985"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="bigjob:bj-d4c9ef3c-4229-11e1-bbbe-00003ea40000:localhost"/>
+    <n v="264"/>
+    <n v="12"/>
+    <n v="64"/>
+    <n v="49.602899074600003"/>
+    <n v="1418.8209559899999"/>
+    <n v="1422.5258469600001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <s v="bigjob:bj-d5d060f0-4229-11e1-bbbe-00003ea40000:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="20.167595863300001"/>
+    <n v="975.95407390599996"/>
+    <n v="1422.5258469600001"/>
+    <s v="redis://cyder.cct.lsu.edu:2525"/>
+    <x v="1"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -19079,12 +19908,91 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="O6:U10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="9"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="6">
+    <dataField name="Mittelwert - Queuing Time" fld="5" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Mittelwert - BJ Runtime" fld="6" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="Mittelwert - Total Runtime" fld="7" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - Queuing Time" fld="5" subtotal="stdDev" baseField="0" baseItem="0"/>
+    <dataField name="STABW - BJ Runtime" fld="6" subtotal="stdDev" baseField="0" baseItem="0"/>
+    <dataField name="STABW - Total Runtime" fld="7" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten_1" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten_1" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data-interop" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -51850,20 +52758,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G4" sqref="G4:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="14" t="s">
         <v>16</v>
       </c>
@@ -51883,10 +52791,13 @@
         <v>130</v>
       </c>
       <c r="G3" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="13">
         <v>1</v>
       </c>
@@ -51905,12 +52816,16 @@
       <c r="F4" s="13">
         <v>8373.6170280000006</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="13">
+        <f>B4+C4+D4+E4</f>
+        <v>8373.6170287900004</v>
+      </c>
+      <c r="H4">
         <f>F4-E4</f>
         <v>8319.2837661100002</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="13">
         <v>2</v>
       </c>
@@ -51929,12 +52844,16 @@
       <c r="F5" s="13">
         <v>10659.133680000001</v>
       </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G11" si="0">F5-E5</f>
+      <c r="G5" s="13">
+        <f t="shared" ref="G5:G8" si="0">B5+C5+D5+E5</f>
+        <v>10659.133677379999</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H11" si="1">F5-E5</f>
         <v>10596.611719620001</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="13">
         <v>3</v>
       </c>
@@ -51953,12 +52872,16 @@
       <c r="F6" s="13">
         <v>8295.7415490000003</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="13">
         <f t="shared" si="0"/>
+        <v>8295.7415485399997</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
         <v>8199.7927942599999</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="13">
         <v>4</v>
       </c>
@@ -51977,12 +52900,16 @@
       <c r="F7" s="13">
         <v>9524.4176769999995</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="13">
         <f t="shared" si="0"/>
+        <v>9524.4176774900006</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
         <v>9447.7057570099987</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="13">
         <v>5</v>
       </c>
@@ -52001,20 +52928,25 @@
       <c r="F8" s="13">
         <v>6943.7142320000003</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="13">
         <f t="shared" si="0"/>
+        <v>6943.71423228</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
         <v>6859.91422822</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="13" t="s">
         <v>131</v>
       </c>
@@ -52033,12 +52965,13 @@
       <c r="F10" s="13">
         <v>8759.3248330000006</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
+      <c r="G10" s="13"/>
+      <c r="H10">
+        <f t="shared" si="1"/>
         <v>8684.6616528400009</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>138</v>
       </c>
@@ -52047,23 +52980,23 @@
         <v>2616.6997684639559</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:F11" si="1">STDEV(C4:C8)</f>
+        <f t="shared" ref="C11:F11" si="2">STDEV(C4:C8)</f>
         <v>1511.1894494054065</v>
       </c>
       <c r="D11">
+        <f t="shared" si="2"/>
+        <v>12.086796340131176</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>16.594195977554207</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>1401.3174641730302</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="1"/>
-        <v>12.086796340131176</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>16.594195977554207</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>1401.3174641730302</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
         <v>1384.7232681954761</v>
       </c>
     </row>
@@ -52289,7 +53222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
@@ -52350,7 +53283,7 @@
       <c r="A6" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="33">
         <v>0</v>
       </c>
       <c r="C6" s="10">
@@ -52420,7 +53353,7 @@
         <v>267.5643732646929</v>
       </c>
       <c r="D9" s="21">
-        <f>Diane!G11</f>
+        <f>Diane!H11</f>
         <v>1384.7232681954761</v>
       </c>
       <c r="E9" s="16">
@@ -52435,19 +53368,19 @@
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:7" ht="16" thickBot="1">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="31"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:7" ht="16" thickTop="1">
       <c r="A12" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="34">
+      <c r="B12" s="35">
         <f>B5/60</f>
         <v>1.2861972593</v>
       </c>
@@ -52455,7 +53388,7 @@
         <f t="shared" ref="C12:E12" si="0">C5/60</f>
         <v>1.6848504899666665</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="35">
         <f t="shared" si="0"/>
         <v>52.790198033333333</v>
       </c>
@@ -52468,7 +53401,7 @@
       <c r="A13" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="34">
+      <c r="B13" s="35">
         <f t="shared" ref="B13:E13" si="1">B6/60</f>
         <v>0</v>
       </c>
@@ -52476,7 +53409,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="35">
         <f t="shared" si="1"/>
         <v>78.46417735</v>
       </c>
@@ -52489,7 +53422,7 @@
       <c r="A14" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="35">
         <f>B16-B15-B12-B13</f>
         <v>4.0070597973667077</v>
       </c>
@@ -52497,7 +53430,7 @@
         <f t="shared" ref="C14:E14" si="2">C16-C15-C12-C13</f>
         <v>8.7646148900333287</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="35">
         <f t="shared" si="2"/>
         <v>-4.333315928306547E-9</v>
       </c>
@@ -52510,7 +53443,7 @@
       <c r="A15" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="34">
+      <c r="B15" s="35">
         <f t="shared" ref="B15:E15" si="3">B7/60</f>
         <v>31.607812499999969</v>
       </c>
@@ -52518,7 +53451,7 @@
         <f t="shared" si="3"/>
         <v>17.814843750000005</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="35">
         <f t="shared" si="3"/>
         <v>13.489985501666666</v>
       </c>
@@ -52531,7 +53464,7 @@
       <c r="A16" t="s">
         <v>130</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="35">
         <f t="shared" ref="B16:E17" si="4">B8/60</f>
         <v>36.901069556666677</v>
       </c>
@@ -52539,7 +53472,7 @@
         <f t="shared" si="4"/>
         <v>28.264309130000001</v>
       </c>
-      <c r="D16" s="34">
+      <c r="D16" s="35">
         <f t="shared" si="4"/>
         <v>144.74436088066668</v>
       </c>
@@ -52552,7 +53485,7 @@
       <c r="A17" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="34">
+      <c r="B17" s="35">
         <f t="shared" si="4"/>
         <v>1.1073060889029485</v>
       </c>
@@ -52560,7 +53493,7 @@
         <f t="shared" si="4"/>
         <v>4.4594062210782148</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="35">
         <f t="shared" si="4"/>
         <v>23.078721136591266</v>
       </c>
@@ -55501,13 +56434,1204 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S54" sqref="S54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.83203125" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="17.83203125" customWidth="1"/>
+    <col min="21" max="21" width="20.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2">
+        <v>264</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>64</v>
+      </c>
+      <c r="F2">
+        <v>39.167788028700002</v>
+      </c>
+      <c r="G2">
+        <v>1413.31066394</v>
+      </c>
+      <c r="H2">
+        <v>1417.01772809</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3">
+        <v>64</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+      <c r="F3">
+        <v>21.497041940700001</v>
+      </c>
+      <c r="G3">
+        <v>947.18463110899995</v>
+      </c>
+      <c r="H3">
+        <v>1417.01772809</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4">
+        <v>264</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>64</v>
+      </c>
+      <c r="F4">
+        <v>45.065774202299998</v>
+      </c>
+      <c r="G4">
+        <v>1600.3404600599999</v>
+      </c>
+      <c r="H4">
+        <v>1604.0428981800001</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5">
+        <v>64</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>64</v>
+      </c>
+      <c r="F5">
+        <v>21.5378801823</v>
+      </c>
+      <c r="G5">
+        <v>1005.3648190500001</v>
+      </c>
+      <c r="H5">
+        <v>1604.0428981800001</v>
+      </c>
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6">
+        <v>264</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>64</v>
+      </c>
+      <c r="F6">
+        <v>38.198520183600003</v>
+      </c>
+      <c r="G6">
+        <v>1429.23286009</v>
+      </c>
+      <c r="H6">
+        <v>1432.9367761599999</v>
+      </c>
+      <c r="I6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7">
+        <v>64</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>64</v>
+      </c>
+      <c r="F7">
+        <v>20.537039041500002</v>
+      </c>
+      <c r="G7">
+        <v>910.54238605499995</v>
+      </c>
+      <c r="H7">
+        <v>1432.9367761599999</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>76</v>
+      </c>
+      <c r="R7" t="s">
+        <v>190</v>
+      </c>
+      <c r="S7" t="s">
+        <v>192</v>
+      </c>
+      <c r="T7" t="s">
+        <v>117</v>
+      </c>
+      <c r="U7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8">
+        <v>264</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>64</v>
+      </c>
+      <c r="F8">
+        <v>50.490038871800003</v>
+      </c>
+      <c r="G8">
+        <v>1412.80108595</v>
+      </c>
+      <c r="H8">
+        <v>1416.50474381</v>
+      </c>
+      <c r="I8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P8" s="7">
+        <v>39.979366734631249</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>945.17090575456245</v>
+      </c>
+      <c r="R8" s="7">
+        <v>1555.9015657600003</v>
+      </c>
+      <c r="S8" s="7">
+        <v>54.499846619321666</v>
+      </c>
+      <c r="T8" s="7">
+        <v>108.59382028879376</v>
+      </c>
+      <c r="U8" s="7">
+        <v>609.87942292746834</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9">
+        <v>64</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>64</v>
+      </c>
+      <c r="F9">
+        <v>21.081934928900001</v>
+      </c>
+      <c r="G9">
+        <v>946.83650994300001</v>
+      </c>
+      <c r="H9">
+        <v>1416.50474381</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="7">
+        <v>186.46815432592501</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>1552.1974980687498</v>
+      </c>
+      <c r="R9" s="7">
+        <v>1555.9015657600003</v>
+      </c>
+      <c r="S9" s="7">
+        <v>562.43943242055707</v>
+      </c>
+      <c r="T9" s="7">
+        <v>609.87901363033779</v>
+      </c>
+      <c r="U9" s="7">
+        <v>609.87942292746834</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10">
+        <v>264</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10">
+        <v>64</v>
+      </c>
+      <c r="F10">
+        <v>57.089904069900001</v>
+      </c>
+      <c r="G10">
+        <v>1396.3976569199999</v>
+      </c>
+      <c r="H10">
+        <v>1400.0998389700001</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P10" s="7">
+        <v>113.22376053027813</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>1248.6842019116559</v>
+      </c>
+      <c r="R10" s="7">
+        <v>1555.90156576</v>
+      </c>
+      <c r="S10" s="7">
+        <v>400.05229276998023</v>
+      </c>
+      <c r="T10" s="7">
+        <v>529.88208384833388</v>
+      </c>
+      <c r="U10" s="7">
+        <v>599.96202340326283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>64</v>
+      </c>
+      <c r="F11">
+        <v>21.823041915899999</v>
+      </c>
+      <c r="G11">
+        <v>954.02606391899997</v>
+      </c>
+      <c r="H11">
+        <v>1400.0998389700001</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12">
+        <v>264</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>64</v>
+      </c>
+      <c r="F12">
+        <v>2293.8809878799998</v>
+      </c>
+      <c r="G12">
+        <v>3820.9009029899998</v>
+      </c>
+      <c r="H12">
+        <v>3824.6060969800001</v>
+      </c>
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13">
+        <v>64</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>64</v>
+      </c>
+      <c r="F13">
+        <v>220.97108697900001</v>
+      </c>
+      <c r="G13">
+        <v>1228.8441650899999</v>
+      </c>
+      <c r="H13">
+        <v>3824.6060969800001</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" t="s">
+        <v>47</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="P13" s="31">
+        <v>945.17090575456245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14">
+        <v>264</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>64</v>
+      </c>
+      <c r="F14">
+        <v>122.449388981</v>
+      </c>
+      <c r="G14">
+        <v>1408.3830029999999</v>
+      </c>
+      <c r="H14">
+        <v>1412.0865111400001</v>
+      </c>
+      <c r="I14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="P14" s="31">
+        <v>1552.1974980687498</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15">
+        <v>64</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>64</v>
+      </c>
+      <c r="F15">
+        <v>122.50563097</v>
+      </c>
+      <c r="G15">
+        <v>1059.7851810499999</v>
+      </c>
+      <c r="H15">
+        <v>1412.0865111400001</v>
+      </c>
+      <c r="I15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" t="s">
+        <v>47</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="P15" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16">
+        <v>264</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <v>32.246130943300003</v>
+      </c>
+      <c r="G16">
+        <v>1323.8348290900001</v>
+      </c>
+      <c r="H16">
+        <v>1327.5373809299999</v>
+      </c>
+      <c r="I16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17">
+        <v>64</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>64</v>
+      </c>
+      <c r="F17">
+        <v>20.4135661125</v>
+      </c>
+      <c r="G17">
+        <v>951.78088307400003</v>
+      </c>
+      <c r="H17">
+        <v>1327.5373809299999</v>
+      </c>
+      <c r="I17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18">
+        <v>264</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <v>64</v>
+      </c>
+      <c r="F18">
+        <v>31.450355052900001</v>
+      </c>
+      <c r="G18">
+        <v>1346.9226479500001</v>
+      </c>
+      <c r="H18">
+        <v>1350.6255128400001</v>
+      </c>
+      <c r="I18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C19">
+        <v>64</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>64</v>
+      </c>
+      <c r="F19">
+        <v>25.5253288746</v>
+      </c>
+      <c r="G19">
+        <v>875.02339291600003</v>
+      </c>
+      <c r="H19">
+        <v>1350.6255128400001</v>
+      </c>
+      <c r="I19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20">
+        <v>264</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+      <c r="E20">
+        <v>64</v>
+      </c>
+      <c r="F20">
+        <v>32.142376899699997</v>
+      </c>
+      <c r="G20">
+        <v>1329.398911</v>
+      </c>
+      <c r="H20">
+        <v>1333.10122299</v>
+      </c>
+      <c r="I20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21">
+        <v>64</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>64</v>
+      </c>
+      <c r="F21">
+        <v>20.341579914099999</v>
+      </c>
+      <c r="G21">
+        <v>963.28213095700005</v>
+      </c>
+      <c r="H21">
+        <v>1333.10122299</v>
+      </c>
+      <c r="I21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22">
+        <v>264</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22">
+        <v>64</v>
+      </c>
+      <c r="F22">
+        <v>32.134410858199999</v>
+      </c>
+      <c r="G22">
+        <v>1317.6233119999999</v>
+      </c>
+      <c r="H22">
+        <v>1321.3276550800001</v>
+      </c>
+      <c r="I22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23">
+        <v>64</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>64</v>
+      </c>
+      <c r="F23">
+        <v>20.338257074400001</v>
+      </c>
+      <c r="G23">
+        <v>922.17073392899999</v>
+      </c>
+      <c r="H23">
+        <v>1321.3276550800001</v>
+      </c>
+      <c r="I23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24">
+        <v>264</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <v>64</v>
+      </c>
+      <c r="F24">
+        <v>62.763838052700002</v>
+      </c>
+      <c r="G24">
+        <v>1543.42536402</v>
+      </c>
+      <c r="H24">
+        <v>1547.13568902</v>
+      </c>
+      <c r="I24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25">
+        <v>64</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>64</v>
+      </c>
+      <c r="F25">
+        <v>21.520488977399999</v>
+      </c>
+      <c r="G25">
+        <v>748.04140806199996</v>
+      </c>
+      <c r="H25">
+        <v>1547.13568902</v>
+      </c>
+      <c r="I25" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26">
+        <v>264</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>64</v>
+      </c>
+      <c r="F26">
+        <v>37.778441190700001</v>
+      </c>
+      <c r="G26">
+        <v>1383.16831303</v>
+      </c>
+      <c r="H26">
+        <v>1386.8724072</v>
+      </c>
+      <c r="I26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>183</v>
+      </c>
+      <c r="C27">
+        <v>64</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>64</v>
+      </c>
+      <c r="F27">
+        <v>20.1079881191</v>
+      </c>
+      <c r="G27">
+        <v>787.46557998699996</v>
+      </c>
+      <c r="H27">
+        <v>1386.8724072</v>
+      </c>
+      <c r="I27" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28">
+        <v>264</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <v>64</v>
+      </c>
+      <c r="F28">
+        <v>26.5749640465</v>
+      </c>
+      <c r="G28">
+        <v>1336.5342540700001</v>
+      </c>
+      <c r="H28">
+        <v>1340.23782396</v>
+      </c>
+      <c r="I28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>185</v>
+      </c>
+      <c r="C29">
+        <v>64</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>64</v>
+      </c>
+      <c r="F29">
+        <v>20.647578954699998</v>
+      </c>
+      <c r="G29">
+        <v>864.43439006799997</v>
+      </c>
+      <c r="H29">
+        <v>1340.23782396</v>
+      </c>
+      <c r="I29" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>186</v>
+      </c>
+      <c r="C30">
+        <v>264</v>
+      </c>
+      <c r="D30">
+        <v>12</v>
+      </c>
+      <c r="E30">
+        <v>64</v>
+      </c>
+      <c r="F30">
+        <v>32.454650878899997</v>
+      </c>
+      <c r="G30">
+        <v>1354.0647489999999</v>
+      </c>
+      <c r="H30">
+        <v>1357.76691985</v>
+      </c>
+      <c r="I30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>187</v>
+      </c>
+      <c r="C31">
+        <v>64</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>64</v>
+      </c>
+      <c r="F31">
+        <v>20.653827905699998</v>
+      </c>
+      <c r="G31">
+        <v>981.99814295800002</v>
+      </c>
+      <c r="H31">
+        <v>1357.76691985</v>
+      </c>
+      <c r="I31" t="s">
+        <v>27</v>
+      </c>
+      <c r="J31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C32">
+        <v>264</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32">
+        <v>64</v>
+      </c>
+      <c r="F32">
+        <v>49.602899074600003</v>
+      </c>
+      <c r="G32">
+        <v>1418.8209559899999</v>
+      </c>
+      <c r="H32">
+        <v>1422.5258469600001</v>
+      </c>
+      <c r="I32" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>15</v>
+      </c>
+      <c r="B33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33">
+        <v>64</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>64</v>
+      </c>
+      <c r="F33">
+        <v>20.167595863300001</v>
+      </c>
+      <c r="G33">
+        <v>975.95407390599996</v>
+      </c>
+      <c r="H33">
+        <v>1422.5258469600001</v>
+      </c>
+      <c r="I33" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
work on section V.B
git-svn-id: file://localhost/tmp/svn2git/svn@6337 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23160" yWindow="80" windowWidth="27220" windowHeight="28280" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31740" windowHeight="23100" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <pivotCache cacheId="1" r:id="rId9"/>
     <pivotCache cacheId="2" r:id="rId10"/>
     <pivotCache cacheId="3" r:id="rId11"/>
-    <pivotCache cacheId="8" r:id="rId12"/>
+    <pivotCache cacheId="4" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="197">
   <si>
     <t>bfast</t>
   </si>
@@ -541,13 +541,7 @@
     <t>Check</t>
   </si>
   <si>
-    <t xml:space="preserve">Queuing </t>
-  </si>
-  <si>
     <t>in min</t>
-  </si>
-  <si>
-    <t>Overhead</t>
   </si>
   <si>
     <t>XSEDE</t>
@@ -671,6 +665,18 @@
   </si>
   <si>
     <t>EGI/FutureGrid</t>
+  </si>
+  <si>
+    <t>Queuing Pilot</t>
+  </si>
+  <si>
+    <t>Queuing LRMS</t>
+  </si>
+  <si>
+    <t>Factor (Total)</t>
+  </si>
+  <si>
+    <t>Factor (BFAST)</t>
   </si>
 </sst>
 </file>
@@ -925,7 +931,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -963,6 +969,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -975,12 +991,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="77">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -1257,11 +1267,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="794179944"/>
-        <c:axId val="794188520"/>
+        <c:axId val="652661544"/>
+        <c:axId val="652662760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="794179944"/>
+        <c:axId val="652661544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1271,7 +1281,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="794188520"/>
+        <c:crossAx val="652662760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1279,7 +1289,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="794188520"/>
+        <c:axId val="652662760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,7 +1300,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="794179944"/>
+        <c:crossAx val="652661544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1588,11 +1598,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="793663896"/>
-        <c:axId val="793669624"/>
+        <c:axId val="650016888"/>
+        <c:axId val="650022616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="793663896"/>
+        <c:axId val="650016888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,7 +1636,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="793669624"/>
+        <c:crossAx val="650022616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1634,7 +1644,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="793669624"/>
+        <c:axId val="650022616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1645,7 +1655,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="793663896"/>
+        <c:crossAx val="650016888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1697,7 +1707,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1958,11 +1967,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="794234312"/>
-        <c:axId val="794240024"/>
+        <c:axId val="650064456"/>
+        <c:axId val="650070184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="794234312"/>
+        <c:axId val="650064456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1989,14 +1998,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="794240024"/>
+        <c:crossAx val="650070184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2004,7 +2012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="794240024"/>
+        <c:axId val="650070184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2027,21 +2035,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="794234312"/>
+        <c:crossAx val="650064456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2111,21 +2117,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Total!$B$12:$E$12</c:f>
+              <c:f>Total!$B$15:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.2861972593</c:v>
+                  <c:v>5.293257056666707</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.684850489966666</c:v>
+                  <c:v>10.44946538</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.79019803333333</c:v>
+                  <c:v>52.79019802900001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.87222222222222</c:v>
+                  <c:v>11.86666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2135,8 +2141,16 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Staging</c:v>
+            <c:v>Data Staging</c:v>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
@@ -2181,60 +2195,18 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Overhead</c:v>
+            <c:v>BFAST Runtime</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Total!$B$4:$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>XSEDE</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>FutureGrid</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>EGI</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>OSG</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Total!$B$14:$E$14</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>4.007059797366708</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.764614890033328</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-4.33331592830655E-9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.00555555555555998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Bfast</c:v>
-          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
@@ -2242,7 +2214,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Total!$B$17:$E$17</c:f>
+                <c:f>Total!$B$18:$E$18</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -2263,7 +2235,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Total!$B$17:$E$17</c:f>
+                <c:f>Total!$B$18:$E$18</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -2305,7 +2277,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Total!$B$15:$E$15</c:f>
+              <c:f>Total!$B$16:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2335,11 +2307,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="793041960"/>
-        <c:axId val="872448136"/>
+        <c:axId val="652738632"/>
+        <c:axId val="652741608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="793041960"/>
+        <c:axId val="652738632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2353,7 +2325,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="1">
+              <a:defRPr sz="2800" b="1">
                 <a:latin typeface="Times"/>
                 <a:cs typeface="Times"/>
               </a:defRPr>
@@ -2361,7 +2333,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="872448136"/>
+        <c:crossAx val="652741608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2369,7 +2341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="872448136"/>
+        <c:axId val="652741608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -2391,13 +2363,13 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000">
+                  <a:defRPr sz="2800">
                     <a:latin typeface="Times"/>
                     <a:cs typeface="Times"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="2000">
+                  <a:rPr lang="de-DE" sz="2800">
                     <a:latin typeface="Times"/>
                     <a:cs typeface="Times"/>
                   </a:rPr>
@@ -2418,7 +2390,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000">
+              <a:defRPr sz="2800">
                 <a:latin typeface="Times"/>
                 <a:cs typeface="Times"/>
               </a:defRPr>
@@ -2426,7 +2398,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="793041960"/>
+        <c:crossAx val="652738632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2437,7 +2409,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
@@ -2445,7 +2417,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400"/>
+            <a:defRPr sz="2800">
+              <a:latin typeface="Times"/>
+              <a:cs typeface="Times"/>
+            </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="de-DE"/>
         </a:p>
@@ -2621,7 +2596,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Total!$B$15:$E$15</c:f>
+              <c:f>Total!$B$16:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2651,11 +2626,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="655922664"/>
-        <c:axId val="873718616"/>
+        <c:axId val="649480200"/>
+        <c:axId val="649477144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="655922664"/>
+        <c:axId val="649480200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2677,7 +2652,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="873718616"/>
+        <c:crossAx val="649477144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2685,7 +2660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="873718616"/>
+        <c:axId val="649477144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2734,7 +2709,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="655922664"/>
+        <c:crossAx val="649480200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2857,11 +2832,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="878731640"/>
-        <c:axId val="878768152"/>
+        <c:axId val="649423368"/>
+        <c:axId val="649420312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="878731640"/>
+        <c:axId val="649423368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2883,7 +2858,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="878768152"/>
+        <c:crossAx val="649420312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2891,13 +2866,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="878768152"/>
+        <c:axId val="649420312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2920,7 +2894,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2940,14 +2913,13 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="878731640"/>
+        <c:crossAx val="649423368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2967,6 +2939,11 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -3080,15 +3057,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>69850</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3110,14 +3087,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>641350</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -19464,6 +19441,92 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="47" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I4:K21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
@@ -19563,7 +19626,7 @@
     <dataField name="STABW - Kraken" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="11">
-    <format dxfId="11">
+    <format dxfId="12">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -19575,7 +19638,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="11">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -19584,7 +19647,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="10">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -19599,10 +19662,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="9">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="8">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -19611,7 +19674,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -19620,7 +19683,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -19632,7 +19695,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -19641,7 +19704,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -19653,7 +19716,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -19662,7 +19725,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -19673,92 +19736,6 @@
           </reference>
         </references>
       </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="47" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="12">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -19909,7 +19886,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="O6:U10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -20341,16 +20318,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
@@ -52761,7 +52738,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -52845,11 +52822,11 @@
         <v>10659.133680000001</v>
       </c>
       <c r="G5" s="13">
-        <f t="shared" ref="G5:G8" si="0">B5+C5+D5+E5</f>
+        <f>B5+C5+D5+E5</f>
         <v>10659.133677379999</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H11" si="1">F5-E5</f>
+        <f t="shared" ref="H5:H11" si="0">F5-E5</f>
         <v>10596.611719620001</v>
       </c>
     </row>
@@ -52873,11 +52850,11 @@
         <v>8295.7415490000003</v>
       </c>
       <c r="G6" s="13">
+        <f>B6+C6+D6+E6</f>
+        <v>8295.7415485399997</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="0"/>
-        <v>8295.7415485399997</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
         <v>8199.7927942599999</v>
       </c>
     </row>
@@ -52901,11 +52878,11 @@
         <v>9524.4176769999995</v>
       </c>
       <c r="G7" s="13">
+        <f>B7+C7+D7+E7</f>
+        <v>9524.4176774900006</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>9524.4176774900006</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
         <v>9447.7057570099987</v>
       </c>
     </row>
@@ -52929,11 +52906,11 @@
         <v>6943.7142320000003</v>
       </c>
       <c r="G8" s="13">
+        <f>B8+C8+D8+E8</f>
+        <v>6943.71423228</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
-        <v>6943.71423228</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
         <v>6859.91422822</v>
       </c>
     </row>
@@ -52967,7 +52944,7 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8684.6616528400009</v>
       </c>
     </row>
@@ -52980,23 +52957,23 @@
         <v>2616.6997684639559</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:F11" si="2">STDEV(C4:C8)</f>
+        <f>STDEV(C4:C8)</f>
         <v>1511.1894494054065</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
+        <f>STDEV(D4:D8)</f>
         <v>12.086796340131176</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f>STDEV(E4:E8)</f>
         <v>16.594195977554207</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f>STDEV(F4:F8)</f>
         <v>1401.3174641730302</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1384.7232681954761</v>
       </c>
     </row>
@@ -53150,7 +53127,7 @@
         <v>909.33333333333405</v>
       </c>
       <c r="B8" s="26">
-        <f t="shared" ref="B8" si="0">AVERAGE(B4:B6)</f>
+        <f>AVERAGE(B4:B6)</f>
         <v>4133.333333333333</v>
       </c>
       <c r="C8" s="16">
@@ -53175,7 +53152,7 @@
         <v>31.533051443420248</v>
       </c>
       <c r="B9" s="26">
-        <f t="shared" ref="B9" si="1">STDEV(B4:B6)</f>
+        <f>STDEV(B4:B6)</f>
         <v>3383.1243449411259</v>
       </c>
       <c r="C9" s="16">
@@ -53220,14 +53197,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K69" sqref="K69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
@@ -53240,16 +53218,16 @@
     <row r="2" spans="1:7">
       <c r="A2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="10"/>
       <c r="B4" s="18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>133</v>
@@ -53283,17 +53261,17 @@
       <c r="A6" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="29">
         <v>0</v>
       </c>
       <c r="C6" s="10">
         <v>0</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="33">
         <f>Diane!C10</f>
         <v>4707.850641</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="34">
         <f>Condor!C8</f>
         <v>5736.0000000000027</v>
       </c>
@@ -53368,27 +53346,27 @@
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:7" ht="16" thickBot="1">
-      <c r="A11" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="32"/>
+      <c r="A11" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:7" ht="16" thickTop="1">
       <c r="A12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12" s="35">
-        <f>B5/60</f>
+        <v>194</v>
+      </c>
+      <c r="B12" s="31">
+        <f t="shared" ref="B12:E13" si="0">B5/60</f>
         <v>1.2861972593</v>
       </c>
       <c r="C12" s="15">
-        <f t="shared" ref="C12:E12" si="0">C5/60</f>
+        <f t="shared" si="0"/>
         <v>1.6848504899666665</v>
       </c>
-      <c r="D12" s="35">
+      <c r="D12" s="31">
         <f t="shared" si="0"/>
         <v>52.790198033333333</v>
       </c>
@@ -53401,110 +53379,180 @@
       <c r="A13" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="35">
-        <f t="shared" ref="B13:E13" si="1">B6/60</f>
+      <c r="B13" s="31">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C13" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D13" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>78.46417735</v>
       </c>
-      <c r="E13" s="15">
-        <f t="shared" si="1"/>
+      <c r="E13" s="36">
+        <f t="shared" si="0"/>
         <v>95.600000000000051</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" s="35">
-        <f>B16-B15-B12-B13</f>
+        <v>193</v>
+      </c>
+      <c r="B14" s="31">
+        <f>B17-B16-B12-B13</f>
         <v>4.0070597973667077</v>
       </c>
       <c r="C14" s="15">
-        <f t="shared" ref="C14:E14" si="2">C16-C15-C12-C13</f>
+        <f>C17-C16-C12-C13</f>
         <v>8.7646148900333287</v>
       </c>
-      <c r="D14" s="35">
-        <f t="shared" si="2"/>
+      <c r="D14" s="31">
+        <f>D17-D16-D12-D13</f>
         <v>-4.333315928306547E-9</v>
       </c>
       <c r="E14" s="15">
-        <f t="shared" si="2"/>
+        <f>E17-E16-E12-E13</f>
         <v>-5.5555555555599767E-3</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="35">
-        <f t="shared" ref="B15:E15" si="3">B7/60</f>
-        <v>31.607812499999969</v>
-      </c>
-      <c r="C15" s="15">
-        <f t="shared" si="3"/>
-        <v>17.814843750000005</v>
-      </c>
-      <c r="D15" s="35">
-        <f t="shared" si="3"/>
-        <v>13.489985501666666</v>
-      </c>
-      <c r="E15" s="15">
-        <f t="shared" si="3"/>
-        <v>15.155555555555567</v>
+        <v>140</v>
+      </c>
+      <c r="B15" s="31">
+        <f>B12+B14</f>
+        <v>5.2932570566667074</v>
+      </c>
+      <c r="C15" s="31">
+        <f>C12+C14</f>
+        <v>10.449465379999996</v>
+      </c>
+      <c r="D15" s="31">
+        <f>D12+D14</f>
+        <v>52.790198029000017</v>
+      </c>
+      <c r="E15" s="31">
+        <f>E12+E14</f>
+        <v>11.866666666666656</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16" s="35">
-        <f t="shared" ref="B16:E17" si="4">B8/60</f>
-        <v>36.901069556666677</v>
+        <v>128</v>
+      </c>
+      <c r="B16" s="31">
+        <f>B7/60</f>
+        <v>31.607812499999969</v>
       </c>
       <c r="C16" s="15">
-        <f t="shared" si="4"/>
-        <v>28.264309130000001</v>
-      </c>
-      <c r="D16" s="35">
-        <f t="shared" si="4"/>
-        <v>144.74436088066668</v>
+        <f>C7/60</f>
+        <v>17.814843750000005</v>
+      </c>
+      <c r="D16" s="31">
+        <f>D7/60</f>
+        <v>13.489985501666666</v>
       </c>
       <c r="E16" s="15">
-        <f t="shared" si="4"/>
-        <v>122.62222222222228</v>
+        <f>E7/60</f>
+        <v>15.155555555555567</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="31">
+        <f t="shared" ref="B17:E18" si="1">B8/60</f>
+        <v>36.901069556666677</v>
+      </c>
+      <c r="C17" s="15">
+        <f t="shared" si="1"/>
+        <v>28.264309130000001</v>
+      </c>
+      <c r="D17" s="31">
+        <f t="shared" si="1"/>
+        <v>144.74436088066668</v>
+      </c>
+      <c r="E17" s="15">
+        <f t="shared" si="1"/>
+        <v>122.62222222222228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="35">
-        <f t="shared" si="4"/>
+      <c r="B18" s="31">
+        <f t="shared" si="1"/>
         <v>1.1073060889029485</v>
       </c>
-      <c r="C17" s="15">
-        <f t="shared" si="4"/>
+      <c r="C18" s="15">
+        <f t="shared" si="1"/>
         <v>4.4594062210782148</v>
       </c>
-      <c r="D17" s="35">
-        <f t="shared" si="4"/>
+      <c r="D18" s="31">
+        <f t="shared" si="1"/>
         <v>23.078721136591266</v>
       </c>
-      <c r="E17" s="15">
-        <f t="shared" si="4"/>
+      <c r="E18" s="15">
+        <f t="shared" si="1"/>
         <v>56.385405749018766</v>
       </c>
     </row>
-    <row r="35" spans="7:7">
-      <c r="G35" s="2" t="s">
-        <v>156</v>
+    <row r="19" spans="1:5" ht="16" thickBot="1">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:5" ht="16" thickTop="1">
+      <c r="A20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B20">
+        <f>B8/$C$8</f>
+        <v>1.3055712554990258</v>
+      </c>
+      <c r="C20">
+        <f>C8/$C$8</f>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>D8/$C$8</f>
+        <v>5.1211002616382251</v>
+      </c>
+      <c r="E20">
+        <f>E8/$C$8</f>
+        <v>4.3384121528755113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21">
+        <f>B7/$D$7</f>
+        <v>2.3430575589643796</v>
+      </c>
+      <c r="C21">
+        <f>C7/$D$7</f>
+        <v>1.3205976943265809</v>
+      </c>
+      <c r="D21">
+        <f>D7/$D$7</f>
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <f>E7/$D$7</f>
+        <v>1.1234671492925714</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7">
+      <c r="G36" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -56436,8 +56484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S54" sqref="S54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -56498,7 +56546,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C2">
         <v>264</v>
@@ -56530,7 +56578,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C3">
         <v>64</v>
@@ -56562,7 +56610,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C4">
         <v>264</v>
@@ -56594,7 +56642,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C5">
         <v>64</v>
@@ -56626,7 +56674,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C6">
         <v>264</v>
@@ -56661,7 +56709,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C7">
         <v>64</v>
@@ -56697,16 +56745,16 @@
         <v>76</v>
       </c>
       <c r="R7" t="s">
+        <v>188</v>
+      </c>
+      <c r="S7" t="s">
         <v>190</v>
-      </c>
-      <c r="S7" t="s">
-        <v>192</v>
       </c>
       <c r="T7" t="s">
         <v>117</v>
       </c>
       <c r="U7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -56714,7 +56762,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C8">
         <v>264</v>
@@ -56767,7 +56815,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C9">
         <v>64</v>
@@ -56820,7 +56868,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C10">
         <v>264</v>
@@ -56873,7 +56921,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C11">
         <v>64</v>
@@ -56905,7 +56953,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C12">
         <v>264</v>
@@ -56937,7 +56985,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C13">
         <v>64</v>
@@ -56964,9 +57012,9 @@
         <v>47</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="P13" s="31">
+        <v>191</v>
+      </c>
+      <c r="P13" s="27">
         <v>945.17090575456245</v>
       </c>
     </row>
@@ -56975,7 +57023,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C14">
         <v>264</v>
@@ -57002,9 +57050,9 @@
         <v>28</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="P14" s="31">
+        <v>191</v>
+      </c>
+      <c r="P14" s="27">
         <v>1552.1974980687498</v>
       </c>
     </row>
@@ -57013,7 +57061,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C15">
         <v>64</v>
@@ -57040,9 +57088,9 @@
         <v>47</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="P15" s="36">
+        <v>192</v>
+      </c>
+      <c r="P15" s="32">
         <v>0</v>
       </c>
     </row>
@@ -57051,7 +57099,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C16">
         <v>264</v>
@@ -57078,7 +57126,7 @@
         <v>28</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -57089,7 +57137,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C17">
         <v>64</v>
@@ -57121,7 +57169,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C18">
         <v>264</v>
@@ -57153,7 +57201,7 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C19">
         <v>64</v>
@@ -57185,7 +57233,7 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C20">
         <v>264</v>
@@ -57217,7 +57265,7 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C21">
         <v>64</v>
@@ -57249,7 +57297,7 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C22">
         <v>264</v>
@@ -57281,7 +57329,7 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C23">
         <v>64</v>
@@ -57313,7 +57361,7 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C24">
         <v>264</v>
@@ -57345,7 +57393,7 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C25">
         <v>64</v>
@@ -57377,7 +57425,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C26">
         <v>264</v>
@@ -57409,7 +57457,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C27">
         <v>64</v>
@@ -57441,7 +57489,7 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C28">
         <v>264</v>
@@ -57473,7 +57521,7 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C29">
         <v>64</v>
@@ -57505,7 +57553,7 @@
         <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C30">
         <v>264</v>
@@ -57537,7 +57585,7 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C31">
         <v>64</v>
@@ -57569,7 +57617,7 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C32">
         <v>264</v>
@@ -57601,7 +57649,7 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C33">
         <v>64</v>

</xml_diff>

<commit_message>
updated motivation in Pilot-Data section VI
git-svn-id: file://localhost/tmp/svn2git/svn@6349 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31740" windowHeight="23100" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31740" windowHeight="23100" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="199">
   <si>
     <t>bfast</t>
   </si>
@@ -678,6 +678,12 @@
   <si>
     <t>Factor (BFAST)</t>
   </si>
+  <si>
+    <t>Total (w/o staging)</t>
+  </si>
+  <si>
+    <t>Factor (Total w/o Staging)</t>
+  </si>
 </sst>
 </file>
 
@@ -755,7 +761,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -851,6 +857,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -931,7 +961,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -976,9 +1006,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -991,6 +1019,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="77">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -2894,6 +2932,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2920,6 +2959,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3064,7 +3104,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3088,13 +3128,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -20318,16 +20358,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
@@ -53197,10 +53237,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -53229,10 +53269,10 @@
       <c r="C4" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="18" t="s">
         <v>134</v>
       </c>
     </row>
@@ -53248,11 +53288,11 @@
         <f>BigJob!N28</f>
         <v>101.09102939799999</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="43">
         <f>Diane!B10</f>
         <v>3167.4118819999999</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="20">
         <f>Condor!D8</f>
         <v>712.33333333333303</v>
       </c>
@@ -53267,11 +53307,11 @@
       <c r="C6" s="10">
         <v>0</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="44">
         <f>Diane!C10</f>
         <v>4707.850641</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="33">
         <f>Condor!C8</f>
         <v>5736.0000000000027</v>
       </c>
@@ -53288,11 +53328,11 @@
         <f>BFAST!J39*60*60*24</f>
         <v>1068.8906250000002</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="45">
         <f>Diane!D10</f>
         <v>809.39913009999998</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <f>Condor!A8</f>
         <v>909.33333333333405</v>
       </c>
@@ -53309,11 +53349,11 @@
         <f>BigJob!Q28</f>
         <v>1695.8585478</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="45">
         <f>Diane!F10-Diane!E10</f>
         <v>8684.6616528400009</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <f>Condor!E8</f>
         <v>7357.3333333333367</v>
       </c>
@@ -53330,11 +53370,11 @@
         <f>BigJob!Z28</f>
         <v>267.5643732646929</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="45">
         <f>Diane!H11</f>
         <v>1384.7232681954761</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="21">
         <f>Condor!B9</f>
         <v>3383.1243449411259</v>
       </c>
@@ -53342,8 +53382,8 @@
     <row r="10" spans="1:7">
       <c r="B10" s="21"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="16"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:7" ht="16" thickBot="1">
       <c r="A11" s="28" t="s">
@@ -53351,8 +53391,8 @@
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="28"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="28"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:7" ht="16" thickTop="1">
       <c r="A12" t="s">
@@ -53366,11 +53406,11 @@
         <f t="shared" si="0"/>
         <v>1.6848504899666665</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="40">
         <f t="shared" si="0"/>
         <v>52.790198033333333</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="31">
         <f t="shared" si="0"/>
         <v>11.872222222222216</v>
       </c>
@@ -53387,11 +53427,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="46">
         <f t="shared" si="0"/>
         <v>78.46417735</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="34">
         <f t="shared" si="0"/>
         <v>95.600000000000051</v>
       </c>
@@ -53408,11 +53448,11 @@
         <f>C17-C16-C12-C13</f>
         <v>8.7646148900333287</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="40">
         <f>D17-D16-D12-D13</f>
         <v>-4.333315928306547E-9</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="31">
         <f>E17-E16-E12-E13</f>
         <v>-5.5555555555599767E-3</v>
       </c>
@@ -53429,7 +53469,7 @@
         <f>C12+C14</f>
         <v>10.449465379999996</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="40">
         <f>D12+D14</f>
         <v>52.790198029000017</v>
       </c>
@@ -53450,11 +53490,11 @@
         <f>C7/60</f>
         <v>17.814843750000005</v>
       </c>
-      <c r="D16" s="31">
+      <c r="D16" s="40">
         <f>D7/60</f>
         <v>13.489985501666666</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="31">
         <f>E7/60</f>
         <v>15.155555555555567</v>
       </c>
@@ -53471,11 +53511,11 @@
         <f t="shared" si="1"/>
         <v>28.264309130000001</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="40">
         <f t="shared" si="1"/>
         <v>144.74436088066668</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="31">
         <f t="shared" si="1"/>
         <v>122.62222222222228</v>
       </c>
@@ -53488,70 +53528,118 @@
         <f t="shared" si="1"/>
         <v>1.1073060889029485</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="39">
         <f t="shared" si="1"/>
         <v>4.4594062210782148</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="40">
         <f t="shared" si="1"/>
         <v>23.078721136591266</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="31">
         <f t="shared" si="1"/>
         <v>56.385405749018766</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16" thickBot="1">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-    </row>
-    <row r="20" spans="1:5" ht="16" thickTop="1">
-      <c r="A20" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>197</v>
+      </c>
+      <c r="B19" s="40">
+        <f>B15+B16</f>
+        <v>36.901069556666677</v>
+      </c>
+      <c r="C19" s="40">
+        <f t="shared" ref="C19:E19" si="2">C15+C16</f>
+        <v>28.264309130000001</v>
+      </c>
+      <c r="D19" s="40">
+        <f t="shared" si="2"/>
+        <v>66.280183530666676</v>
+      </c>
+      <c r="E19" s="40">
+        <f t="shared" si="2"/>
+        <v>27.022222222222226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" thickBot="1">
+      <c r="A20" s="28"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="30"/>
+    </row>
+    <row r="21" spans="1:5" ht="16" thickTop="1">
+      <c r="A21" t="s">
         <v>195</v>
       </c>
-      <c r="B20">
+      <c r="B21" s="3">
         <f>B8/$C$8</f>
         <v>1.3055712554990258</v>
       </c>
-      <c r="C20">
+      <c r="C21" s="29">
         <f>C8/$C$8</f>
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="D21" s="10">
         <f>D8/$C$8</f>
         <v>5.1211002616382251</v>
       </c>
-      <c r="E20">
+      <c r="E21" s="29">
         <f>E8/$C$8</f>
         <v>4.3384121528755113</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
         <v>196</v>
       </c>
-      <c r="B21">
+      <c r="B22" s="3">
         <f>B7/$D$7</f>
         <v>2.3430575589643796</v>
       </c>
-      <c r="C21">
+      <c r="C22" s="29">
         <f>C7/$D$7</f>
         <v>1.3205976943265809</v>
       </c>
-      <c r="D21">
+      <c r="D22" s="10">
         <f>D7/$D$7</f>
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="E22" s="29">
         <f>E7/$D$7</f>
         <v>1.1234671492925714</v>
       </c>
     </row>
-    <row r="36" spans="7:7">
-      <c r="G36" s="2" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>198</v>
+      </c>
+      <c r="B23" s="29">
+        <f>B19/$C$19</f>
+        <v>1.3055712554990258</v>
+      </c>
+      <c r="C23" s="29">
+        <f>C19/$C$19</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="29">
+        <f t="shared" ref="D23:E23" si="3">D19/$C$19</f>
+        <v>2.3450133957216126</v>
+      </c>
+      <c r="E23" s="29">
+        <f t="shared" si="3"/>
+        <v>0.95605458098887641</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="D25">
+        <f>D19/B19</f>
+        <v>1.7961588736305956</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7">
+      <c r="G37" s="2" t="s">
         <v>154</v>
       </c>
     </row>
@@ -56484,8 +56572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S46" sqref="S46"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updated figure 3 (DIANE in caps) updated figure 8 w/ EGI/FG numbers
git-svn-id: file://localhost/tmp/svn2git/svn@6370 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31740" windowHeight="23100" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35560" windowHeight="27840" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -13,20 +13,21 @@
     <sheet name="Condor" sheetId="11" r:id="rId4"/>
     <sheet name="Total" sheetId="12" r:id="rId5"/>
     <sheet name="Raw (BJ)" sheetId="8" r:id="rId6"/>
-    <sheet name="Raw (BJ interop)" sheetId="14" r:id="rId7"/>
+    <sheet name="Interop " sheetId="14" r:id="rId7"/>
+    <sheet name="Interop EGI-FG" sheetId="15" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="data_interop" localSheetId="6">'Raw (BJ interop)'!$A$1:$J$33</definedName>
+    <definedName name="data_interop" localSheetId="6">'Interop '!$A$1:$J$33</definedName>
     <definedName name="daten" localSheetId="1">BigJob!$A$1:$J$64</definedName>
     <definedName name="daten_1" localSheetId="5">'Raw (BJ)'!$A$1:$J$109</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="1" r:id="rId9"/>
-    <pivotCache cacheId="2" r:id="rId10"/>
-    <pivotCache cacheId="3" r:id="rId11"/>
-    <pivotCache cacheId="4" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId10"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
+    <pivotCache cacheId="3" r:id="rId12"/>
+    <pivotCache cacheId="4" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="200">
   <si>
     <t>bfast</t>
   </si>
@@ -684,6 +685,9 @@
   <si>
     <t>Factor (Total w/o Staging)</t>
   </si>
+  <si>
+    <t>Total (no Staging)</t>
+  </si>
 </sst>
 </file>
 
@@ -882,7 +886,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -960,8 +964,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -999,7 +1009,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1007,6 +1016,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1019,18 +1038,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="83">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1069,6 +1084,9 @@
     <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1107,6 +1125,9 @@
     <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -1305,11 +1326,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="652661544"/>
-        <c:axId val="652662760"/>
+        <c:axId val="624674104"/>
+        <c:axId val="624677128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="652661544"/>
+        <c:axId val="624674104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1319,7 +1340,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="652662760"/>
+        <c:crossAx val="624677128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1327,7 +1348,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="652662760"/>
+        <c:axId val="624677128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,7 +1359,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="652661544"/>
+        <c:crossAx val="624674104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1636,11 +1657,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="650016888"/>
-        <c:axId val="650022616"/>
+        <c:axId val="624723400"/>
+        <c:axId val="624729128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="650016888"/>
+        <c:axId val="624723400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,7 +1695,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="650022616"/>
+        <c:crossAx val="624729128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1682,7 +1703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="650022616"/>
+        <c:axId val="624729128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,7 +1714,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="650016888"/>
+        <c:crossAx val="624723400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2005,11 +2026,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="650064456"/>
-        <c:axId val="650070184"/>
+        <c:axId val="624750168"/>
+        <c:axId val="624755880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="650064456"/>
+        <c:axId val="624750168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2042,7 +2063,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="650070184"/>
+        <c:crossAx val="624755880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2050,7 +2071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="650070184"/>
+        <c:axId val="624755880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2079,7 +2100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="650064456"/>
+        <c:crossAx val="624750168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2345,11 +2366,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="652738632"/>
-        <c:axId val="652741608"/>
+        <c:axId val="600089592"/>
+        <c:axId val="600086536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="652738632"/>
+        <c:axId val="600089592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2371,7 +2392,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652741608"/>
+        <c:crossAx val="600086536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2379,7 +2400,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="652741608"/>
+        <c:axId val="600086536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -2416,7 +2437,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -2436,7 +2456,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="652738632"/>
+        <c:crossAx val="600089592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2448,7 +2468,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2664,11 +2683,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="649480200"/>
-        <c:axId val="649477144"/>
+        <c:axId val="624820744"/>
+        <c:axId val="624823784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="649480200"/>
+        <c:axId val="624820744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2690,7 +2709,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649477144"/>
+        <c:crossAx val="624823784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2698,7 +2717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="649477144"/>
+        <c:axId val="624823784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2727,7 +2746,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -2747,14 +2765,13 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649480200"/>
+        <c:crossAx val="624820744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2798,64 +2815,142 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>India</c:v>
+            <c:v>FutureGrid</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0010_XSEDE/FutureGrid</c:v>
-              </c:pt>
-            </c:strLit>
+            <c:strRef>
+              <c:f>'Interop '!$O$13:$O$14</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE/FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EGI/FutureGrid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Raw (BJ interop)'!$P$13:$P$13</c:f>
+              <c:f>'Interop '!$P$13:$P$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>945.1709057545624</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>15.75284842924271</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Kraken</c:v>
+            <c:strRef>
+              <c:f>'Interop '!$Q$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strLit>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>_x0010_XSEDE/FutureGrid</c:v>
-              </c:pt>
-            </c:strLit>
-          </c:cat>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Interop '!$S$13:$T$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>10.1646502271723</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Interop '!$S$13:$T$13</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>10.1646502271723</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>'Raw (BJ interop)'!$P$14:$P$14</c:f>
+              <c:f>'Interop '!$Q$13:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>10.11710987190312</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Interop '!$R$12</c:f>
+              <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1552.19749806875</c:v>
+                  <c:v>EGI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Interop '!$R$13:$R$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.59764122603281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2870,11 +2965,12 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="649423368"/>
-        <c:axId val="649420312"/>
+        <c:overlap val="100"/>
+        <c:axId val="624886280"/>
+        <c:axId val="624889320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="649423368"/>
+        <c:axId val="624886280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2888,7 +2984,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000">
+              <a:defRPr sz="2000" b="1">
                 <a:latin typeface="Times"/>
                 <a:cs typeface="Times"/>
               </a:defRPr>
@@ -2896,7 +2992,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649420312"/>
+        <c:crossAx val="624889320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2904,7 +3000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="649420312"/>
+        <c:axId val="624889320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2917,25 +3013,32 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000">
+                  <a:defRPr sz="2800">
                     <a:latin typeface="Times"/>
                     <a:cs typeface="Times"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="2000">
+                  <a:rPr lang="de-DE" sz="2800">
                     <a:latin typeface="Times"/>
                     <a:cs typeface="Times"/>
                   </a:rPr>
-                  <a:t>Runtime (in sec)</a:t>
+                  <a:t>Runtime (in min)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00649772579597141"/>
+              <c:y val="0.233224622260055"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2944,7 +3047,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000">
+              <a:defRPr sz="2000" b="0">
                 <a:latin typeface="Times"/>
                 <a:cs typeface="Times"/>
               </a:defRPr>
@@ -2952,7 +3055,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649423368"/>
+        <c:crossAx val="624886280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3169,10 +3272,10 @@
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3383,7 +3486,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="40929.651928703701" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="32">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J33" sheet="Raw (BJ interop)"/>
+    <worksheetSource ref="A1:J33" sheet="Interop "/>
   </cacheSource>
   <cacheFields count="10">
     <cacheField name="Run" numFmtId="0">
@@ -19379,6 +19482,92 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="47" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I54:K65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
@@ -19465,92 +19654,6 @@
   <dataFields count="2">
     <dataField name="Mittelwert - Kraken" fld="2" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Kraken2" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="47" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
     <format dxfId="1">
@@ -20358,16 +20461,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
@@ -52778,7 +52881,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -53019,6 +53122,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -53269,7 +53373,7 @@
       <c r="C4" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="37" t="s">
         <v>133</v>
       </c>
       <c r="E4" s="18" t="s">
@@ -53288,7 +53392,7 @@
         <f>BigJob!N28</f>
         <v>101.09102939799999</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="38">
         <f>Diane!B10</f>
         <v>3167.4118819999999</v>
       </c>
@@ -53301,17 +53405,17 @@
       <c r="A6" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="28">
         <v>0</v>
       </c>
       <c r="C6" s="10">
         <v>0</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="39">
         <f>Diane!C10</f>
         <v>4707.850641</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="32">
         <f>Condor!C8</f>
         <v>5736.0000000000027</v>
       </c>
@@ -53328,7 +53432,7 @@
         <f>BFAST!J39*60*60*24</f>
         <v>1068.8906250000002</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="40">
         <f>Diane!D10</f>
         <v>809.39913009999998</v>
       </c>
@@ -53349,7 +53453,7 @@
         <f>BigJob!Q28</f>
         <v>1695.8585478</v>
       </c>
-      <c r="D8" s="45">
+      <c r="D8" s="40">
         <f>Diane!F10-Diane!E10</f>
         <v>8684.6616528400009</v>
       </c>
@@ -53370,7 +53474,7 @@
         <f>BigJob!Z28</f>
         <v>267.5643732646929</v>
       </c>
-      <c r="D9" s="45">
+      <c r="D9" s="40">
         <f>Diane!H11</f>
         <v>1384.7232681954761</v>
       </c>
@@ -53382,23 +53486,23 @@
     <row r="10" spans="1:7">
       <c r="B10" s="21"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="45"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:7" ht="16" thickBot="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="30"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="12" spans="1:7" ht="16" thickTop="1">
       <c r="A12" t="s">
         <v>194</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="30">
         <f t="shared" ref="B12:E13" si="0">B5/60</f>
         <v>1.2861972593</v>
       </c>
@@ -53406,11 +53510,11 @@
         <f t="shared" si="0"/>
         <v>1.6848504899666665</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="35">
         <f t="shared" si="0"/>
         <v>52.790198033333333</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="30">
         <f t="shared" si="0"/>
         <v>11.872222222222216</v>
       </c>
@@ -53419,7 +53523,7 @@
       <c r="A13" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -53427,11 +53531,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D13" s="46">
+      <c r="D13" s="41">
         <f t="shared" si="0"/>
         <v>78.46417735</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="33">
         <f t="shared" si="0"/>
         <v>95.600000000000051</v>
       </c>
@@ -53440,7 +53544,7 @@
       <c r="A14" t="s">
         <v>193</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="30">
         <f>B17-B16-B12-B13</f>
         <v>4.0070597973667077</v>
       </c>
@@ -53448,11 +53552,11 @@
         <f>C17-C16-C12-C13</f>
         <v>8.7646148900333287</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="35">
         <f>D17-D16-D12-D13</f>
         <v>-4.333315928306547E-9</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="30">
         <f>E17-E16-E12-E13</f>
         <v>-5.5555555555599767E-3</v>
       </c>
@@ -53461,19 +53565,19 @@
       <c r="A15" t="s">
         <v>140</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="30">
         <f>B12+B14</f>
         <v>5.2932570566667074</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="30">
         <f>C12+C14</f>
         <v>10.449465379999996</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="35">
         <f>D12+D14</f>
         <v>52.790198029000017</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="30">
         <f>E12+E14</f>
         <v>11.866666666666656</v>
       </c>
@@ -53482,7 +53586,7 @@
       <c r="A16" t="s">
         <v>128</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="30">
         <f>B7/60</f>
         <v>31.607812499999969</v>
       </c>
@@ -53490,11 +53594,11 @@
         <f>C7/60</f>
         <v>17.814843750000005</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="35">
         <f>D7/60</f>
         <v>13.489985501666666</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="30">
         <f>E7/60</f>
         <v>15.155555555555567</v>
       </c>
@@ -53503,7 +53607,7 @@
       <c r="A17" t="s">
         <v>130</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="30">
         <f t="shared" ref="B17:E18" si="1">B8/60</f>
         <v>36.901069556666677</v>
       </c>
@@ -53511,11 +53615,11 @@
         <f t="shared" si="1"/>
         <v>28.264309130000001</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="35">
         <f t="shared" si="1"/>
         <v>144.74436088066668</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="30">
         <f t="shared" si="1"/>
         <v>122.62222222222228</v>
       </c>
@@ -53524,19 +53628,19 @@
       <c r="A18" t="s">
         <v>138</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="30">
         <f t="shared" si="1"/>
         <v>1.1073060889029485</v>
       </c>
-      <c r="C18" s="39">
+      <c r="C18" s="34">
         <f t="shared" si="1"/>
         <v>4.4594062210782148</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="35">
         <f t="shared" si="1"/>
         <v>23.078721136591266</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="30">
         <f t="shared" si="1"/>
         <v>56.385405749018766</v>
       </c>
@@ -53545,29 +53649,29 @@
       <c r="A19" t="s">
         <v>197</v>
       </c>
-      <c r="B19" s="40">
+      <c r="B19" s="35">
         <f>B15+B16</f>
         <v>36.901069556666677</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="35">
         <f t="shared" ref="C19:E19" si="2">C15+C16</f>
         <v>28.264309130000001</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="35">
         <f t="shared" si="2"/>
         <v>66.280183530666676</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="35">
         <f t="shared" si="2"/>
         <v>27.022222222222226</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16" thickBot="1">
-      <c r="A20" s="28"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="30"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="29"/>
     </row>
     <row r="21" spans="1:5" ht="16" thickTop="1">
       <c r="A21" t="s">
@@ -53577,7 +53681,7 @@
         <f>B8/$C$8</f>
         <v>1.3055712554990258</v>
       </c>
-      <c r="C21" s="29">
+      <c r="C21" s="28">
         <f>C8/$C$8</f>
         <v>1</v>
       </c>
@@ -53585,7 +53689,7 @@
         <f>D8/$C$8</f>
         <v>5.1211002616382251</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="28">
         <f>E8/$C$8</f>
         <v>4.3384121528755113</v>
       </c>
@@ -53598,7 +53702,7 @@
         <f>B7/$D$7</f>
         <v>2.3430575589643796</v>
       </c>
-      <c r="C22" s="29">
+      <c r="C22" s="28">
         <f>C7/$D$7</f>
         <v>1.3205976943265809</v>
       </c>
@@ -53606,7 +53710,7 @@
         <f>D7/$D$7</f>
         <v>1</v>
       </c>
-      <c r="E22" s="29">
+      <c r="E22" s="28">
         <f>E7/$D$7</f>
         <v>1.1234671492925714</v>
       </c>
@@ -53615,19 +53719,19 @@
       <c r="A23" t="s">
         <v>198</v>
       </c>
-      <c r="B23" s="29">
+      <c r="B23" s="28">
         <f>B19/$C$19</f>
         <v>1.3055712554990258</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="28">
         <f>C19/$C$19</f>
         <v>1</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="28">
         <f t="shared" ref="D23:E23" si="3">D19/$C$19</f>
         <v>2.3450133957216126</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="28">
         <f t="shared" si="3"/>
         <v>0.95605458098887641</v>
       </c>
@@ -56572,8 +56676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8:Q9"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -56591,7 +56695,7 @@
     <col min="15" max="15" width="32.83203125" customWidth="1"/>
     <col min="16" max="16" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.6640625" customWidth="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20" customWidth="1"/>
     <col min="20" max="20" width="17.83203125" customWidth="1"/>
     <col min="21" max="21" width="20.1640625" customWidth="1"/>
@@ -57067,6 +57171,18 @@
       <c r="J12" t="s">
         <v>28</v>
       </c>
+      <c r="P12" s="46" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q12" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="R12" t="s">
+        <v>133</v>
+      </c>
+      <c r="S12" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13">
@@ -57102,8 +57218,23 @@
       <c r="O13" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="P13" s="27">
-        <v>945.17090575456245</v>
+      <c r="P13" s="48">
+        <f>Q8/60</f>
+        <v>15.752848429242707</v>
+      </c>
+      <c r="Q13" s="48">
+        <f>Q9/60-P13</f>
+        <v>10.117109871903125</v>
+      </c>
+      <c r="R13" s="49">
+        <v>0</v>
+      </c>
+      <c r="S13" s="49">
+        <f>T9/60</f>
+        <v>10.164650227172297</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -57138,10 +57269,23 @@
         <v>28</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="P14" s="27">
-        <v>1552.1974980687498</v>
+        <v>192</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14" s="47">
+        <f>'Interop EGI-FG'!I8/60</f>
+        <v>20.597641226032813</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -57175,12 +57319,7 @@
       <c r="J15" t="s">
         <v>47</v>
       </c>
-      <c r="O15" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="P15" s="32">
-        <v>0</v>
-      </c>
+      <c r="P15" s="31"/>
     </row>
     <row r="16" spans="1:21">
       <c r="A16">
@@ -57213,12 +57352,7 @@
       <c r="J16" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
+      <c r="O16" s="8"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
@@ -57774,4 +57908,135 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>421.76157190086724</v>
+      </c>
+      <c r="C2">
+        <v>1350.2136189248276</v>
+      </c>
+      <c r="D2">
+        <v>814.09690166110136</v>
+      </c>
+      <c r="E2">
+        <v>2.2251180018750141</v>
+      </c>
+      <c r="F2">
+        <v>2588.2972104886717</v>
+      </c>
+      <c r="H2">
+        <f>F2-E2</f>
+        <v>2586.0720924867965</v>
+      </c>
+      <c r="I2">
+        <f>F2-E2-C2</f>
+        <v>1235.8584735619688</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8">
+        <f>AVERAGE(B2:B6)</f>
+        <v>421.76157190086724</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:I8" si="0">AVERAGE(C2:C6)</f>
+        <v>1350.2136189248276</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>814.09690166110136</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2.2251180018750141</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2588.2972104886717</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>2586.0720924867965</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1235.8584735619688</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refinements to figure 8 consistent spelling \pilot, \pilotjob, \pilots... (didn't do entire document to avoid conflict). Please try to use the macro. update to section II
git-svn-id: file://localhost/tmp/svn2git/svn@6372 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -2808,10 +2808,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="117"/>
+      <c14:style val="109"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="17"/>
+      <c:style val="9"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -3013,13 +3013,13 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2800">
+                  <a:defRPr sz="2400">
                     <a:latin typeface="Times"/>
                     <a:cs typeface="Times"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="2800">
+                  <a:rPr lang="de-DE" sz="2400">
                     <a:latin typeface="Times"/>
                     <a:cs typeface="Times"/>
                   </a:rPr>
@@ -3032,8 +3032,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.00649772579597141"/>
-              <c:y val="0.233224622260055"/>
+              <c:x val="0.00389863547758284"/>
+              <c:y val="0.309801198836632"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3047,7 +3047,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0">
+              <a:defRPr sz="2000">
                 <a:latin typeface="Times"/>
                 <a:cs typeface="Times"/>
               </a:defRPr>
@@ -3061,7 +3061,7 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
@@ -3069,10 +3069,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000">
-              <a:latin typeface="Times"/>
-              <a:cs typeface="Times"/>
-            </a:defRPr>
+            <a:defRPr sz="2400"/>
           </a:pPr>
           <a:endParaRPr lang="de-DE"/>
         </a:p>
@@ -3082,11 +3079,6 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -56677,7 +56669,7 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V38" sqref="V38"/>
+      <selection activeCell="U66" sqref="U66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updated graphs with new EGI and OSG data
git-svn-id: file://localhost/tmp/svn2git/svn@6435 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="47000" windowHeight="28240" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="14780" yWindow="0" windowWidth="47000" windowHeight="28240" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -14,23 +14,24 @@
     <sheet name="Total" sheetId="12" r:id="rId5"/>
     <sheet name="Raw (BJ)" sheetId="8" r:id="rId6"/>
     <sheet name="Interop EGI-FG" sheetId="15" r:id="rId7"/>
-    <sheet name="Interop " sheetId="14" r:id="rId8"/>
+    <sheet name="Interop OSG-XSEDE" sheetId="16" r:id="rId8"/>
+    <sheet name="Interop " sheetId="14" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
-    <definedName name="data_interop" localSheetId="7">'Interop '!$A$1:$J$32</definedName>
+    <definedName name="data_interop" localSheetId="8">'Interop '!$A$1:$J$32</definedName>
     <definedName name="daten" localSheetId="1">BigJob!$A$1:$J$64</definedName>
     <definedName name="daten_1" localSheetId="5">'Raw (BJ)'!$A$1:$J$109</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId10"/>
-    <pivotCache cacheId="1" r:id="rId11"/>
-    <pivotCache cacheId="2" r:id="rId12"/>
-    <pivotCache cacheId="3" r:id="rId13"/>
-    <pivotCache cacheId="7" r:id="rId14"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
+    <pivotCache cacheId="2" r:id="rId13"/>
+    <pivotCache cacheId="3" r:id="rId14"/>
+    <pivotCache cacheId="4" r:id="rId15"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="207">
   <si>
     <t>bfast</t>
   </si>
@@ -683,15 +684,37 @@
     <t>Total (no Staging)</t>
   </si>
   <si>
-    <t>XSEDE/
-FutureGrid</t>
-  </si>
-  <si>
     <t>EGI/
 FutureGrid</t>
   </si>
   <si>
     <t>Future Grid</t>
+  </si>
+  <si>
+    <t>CPU Time</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Allocation/Runtime</t>
+  </si>
+  <si>
+    <t>Condor</t>
+  </si>
+  <si>
+    <t>OSG-XSEDE</t>
+  </si>
+  <si>
+    <t>stddev</t>
+  </si>
+  <si>
+    <t>FutureGrid/
+XSEDE:Kraken</t>
+  </si>
+  <si>
+    <t>OSG/
+XSEDE:QB</t>
   </si>
 </sst>
 </file>
@@ -891,7 +914,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -981,8 +1004,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1036,6 +1081,13 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1048,18 +1100,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="111">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1104,6 +1156,17 @@
     <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1148,6 +1211,17 @@
     <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -1346,11 +1420,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="624674104"/>
-        <c:axId val="624677128"/>
+        <c:axId val="861616728"/>
+        <c:axId val="861619704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="624674104"/>
+        <c:axId val="861616728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1360,7 +1434,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="624677128"/>
+        <c:crossAx val="861619704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1368,7 +1442,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="624677128"/>
+        <c:axId val="861619704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,7 +1453,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="624674104"/>
+        <c:crossAx val="861616728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1677,11 +1751,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="624723400"/>
-        <c:axId val="624729128"/>
+        <c:axId val="861662584"/>
+        <c:axId val="861668312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="624723400"/>
+        <c:axId val="861662584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,7 +1789,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="624729128"/>
+        <c:crossAx val="861668312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1723,7 +1797,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="624729128"/>
+        <c:axId val="861668312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1734,7 +1808,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="624723400"/>
+        <c:crossAx val="861662584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1786,7 +1860,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2047,11 +2120,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="624750168"/>
-        <c:axId val="624755880"/>
+        <c:axId val="861728504"/>
+        <c:axId val="861734216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="624750168"/>
+        <c:axId val="861728504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2078,14 +2151,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="624755880"/>
+        <c:crossAx val="861734216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2093,7 +2165,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="624755880"/>
+        <c:axId val="861734216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2116,21 +2188,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="624750168"/>
+        <c:crossAx val="861728504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2390,11 +2460,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="600089592"/>
-        <c:axId val="600086536"/>
+        <c:axId val="861805960"/>
+        <c:axId val="861809000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="600089592"/>
+        <c:axId val="861805960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2416,7 +2486,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600086536"/>
+        <c:crossAx val="861809000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2424,7 +2494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="600086536"/>
+        <c:axId val="861809000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -2481,7 +2551,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="600089592"/>
+        <c:crossAx val="861805960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2709,11 +2779,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="624820744"/>
-        <c:axId val="624823784"/>
+        <c:axId val="861843688"/>
+        <c:axId val="861846728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="624820744"/>
+        <c:axId val="861843688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2735,7 +2805,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="624823784"/>
+        <c:crossAx val="861846728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2743,7 +2813,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="624823784"/>
+        <c:axId val="861846728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2792,7 +2862,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="624820744"/>
+        <c:crossAx val="861843688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2864,29 +2934,69 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Interop '!$O$15:$O$16</c:f>
+              <c:f>'Interop '!$O$15:$O$17</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>XSEDE/_x000d_FutureGrid</c:v>
+                  <c:v>FutureGrid/_x000d_XSEDE:Kraken</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>EGI/_x000d_FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OSG/_x000d_XSEDE:QB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Interop '!$P$15:$P$16</c:f>
+              <c:f>'Interop '!$P$15:$P$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="0.00">
                   <c:v>15.75284842924271</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.55944666223809</c:v>
+                  <c:v>23.00641267479796</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>OSG</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Interop '!$S$15:$S$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0">
+                  <c:v>40.61111111111111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2894,7 +3004,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>'Interop '!$Q$14</c:f>
@@ -2920,40 +3030,66 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Interop '!$S$15:$T$15</c:f>
+                <c:f>'Interop '!$T$15:$V$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
                     <c:v>1.329881595054672</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.291502622129181</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Interop '!$S$15:$T$15</c:f>
+                <c:f>'Interop '!$T$15:$V$15</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="3"/>
                   <c:pt idx="0">
                     <c:v>1.329881595054672</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.291502622129181</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
           </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Interop '!$O$15:$O$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FutureGrid/_x000d_XSEDE:Kraken</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EGI/_x000d_FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OSG/_x000d_XSEDE:QB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Interop '!$Q$15:$Q$16</c:f>
+              <c:f>'Interop '!$Q$15:$Q$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="0.00">
                   <c:v>7.596328310879517</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0">
+                  <c:v>50.3888888888889</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2961,7 +3097,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>'Interop '!$R$14</c:f>
@@ -2976,8 +3112,8 @@
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
@@ -2988,40 +3124,60 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Interop '!$S$16:$T$16</c:f>
+                <c:f>'Interop '!$T$16:$U$16</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="1">
-                    <c:v>6.338517354918173</c:v>
+                    <c:v>5.887279534302993</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Interop '!$S$16:$T$16</c:f>
+                <c:f>'Interop '!$T$16:$U$16</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="2"/>
                   <c:pt idx="1">
-                    <c:v>6.338517354918173</c:v>
+                    <c:v>5.887279534302993</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
           </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Interop '!$O$15:$O$17</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FutureGrid/_x000d_XSEDE:Kraken</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EGI/_x000d_FutureGrid</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OSG/_x000d_XSEDE:QB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Interop '!$R$15:$R$16</c:f>
+              <c:f>'Interop '!$R$15:$R$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0" formatCode="0.00">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.94222290801475</c:v>
+                  <c:v>72.86479822088748</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3037,11 +3193,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="624886280"/>
-        <c:axId val="624889320"/>
+        <c:axId val="861356040"/>
+        <c:axId val="861352968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="624886280"/>
+        <c:axId val="861356040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3055,7 +3211,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2800" b="1">
+              <a:defRPr sz="2400" b="1">
                 <a:latin typeface="Times"/>
                 <a:cs typeface="Times"/>
               </a:defRPr>
@@ -3063,7 +3219,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="624889320"/>
+        <c:crossAx val="861352968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3071,7 +3227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="624889320"/>
+        <c:axId val="861352968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3126,7 +3282,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="624886280"/>
+        <c:crossAx val="861356040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3377,7 +3533,9 @@
       <sheetName val="summary"/>
       <sheetName val="run1"/>
       <sheetName val="run2"/>
-      <sheetName val="run2 (2)"/>
+      <sheetName val="run3"/>
+      <sheetName val="run4"/>
+      <sheetName val="run5"/>
       <sheetName val="run1 (3) old"/>
       <sheetName val="run1 old"/>
       <sheetName val="run1 (2) old"/>
@@ -3387,7 +3545,7 @@
       <sheetName val="run5 old"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="72">
           <cell r="O72">
@@ -3396,7 +3554,7 @@
         </row>
         <row r="131">
           <cell r="O131">
-            <v>4248.3777595267238</v>
+            <v>4243.4671542812066</v>
           </cell>
         </row>
       </sheetData>
@@ -3408,18 +3566,53 @@
         </row>
         <row r="131">
           <cell r="O131">
-            <v>4744.688989435047</v>
+            <v>4707.8597792293331</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="3">
+        <row r="61">
+          <cell r="O61">
+            <v>2148.8040556623728</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="O131">
+            <v>3879.476980005943</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="62">
+          <cell r="O62">
+            <v>1091.8222408393551</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="O127">
+            <v>4722.518188808127</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="68">
+          <cell r="O68">
+            <v>1194.1639064690908</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="O131">
+            <v>4306.1173639416338</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -19598,92 +19791,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="47" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I54:K65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
@@ -19770,6 +19877,92 @@
   <dataFields count="2">
     <dataField name="Mittelwert - Kraken" fld="2" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Kraken2" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="47" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
     <format dxfId="1">
@@ -20145,7 +20338,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="O6:U10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -20577,16 +20770,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
@@ -53253,19 +53446,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -53381,71 +53571,163 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="16">
+      <c r="A7">
+        <v>962</v>
+      </c>
+      <c r="B7" s="50">
+        <v>2830</v>
+      </c>
+      <c r="C7">
+        <v>872</v>
+      </c>
+      <c r="D7" s="50">
+        <v>2711</v>
+      </c>
+      <c r="E7" s="50">
+        <v>4697</v>
+      </c>
+      <c r="F7" s="15">
+        <f t="shared" ref="F7:F8" si="0">D7+C7+A7</f>
+        <v>4545</v>
+      </c>
       <c r="I7" s="24" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="26">
+    <row r="8" spans="1:9" ht="16">
+      <c r="A8">
+        <v>826</v>
+      </c>
+      <c r="B8" s="50">
+        <v>1978</v>
+      </c>
+      <c r="C8">
+        <v>190</v>
+      </c>
+      <c r="D8" s="50">
+        <v>1994</v>
+      </c>
+      <c r="E8" s="50">
+        <v>3129</v>
+      </c>
+      <c r="F8" s="15">
+        <f t="shared" si="0"/>
+        <v>3010</v>
+      </c>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="26">
         <f>AVERAGE(A4:A6)</f>
         <v>909.33333333333405</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B9" s="26">
         <f>AVERAGE(B4:B6)</f>
         <v>4133.333333333333</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C9" s="16">
         <f>AVERAGE(C4:C6)</f>
         <v>5736.0000000000027</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D9" s="16">
         <f>AVERAGE(D4:D6)</f>
         <v>712.33333333333303</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E9" s="26">
         <f>AVERAGE(E4:E6)</f>
         <v>7357.3333333333367</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16">
-      <c r="A9" s="26">
+    <row r="10" spans="1:9" ht="16">
+      <c r="A10" s="26">
         <f>STDEV(A4:A6)</f>
         <v>31.533051443420248</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B10" s="26">
         <f>STDEV(B4:B6)</f>
         <v>3383.1243449411259</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C10" s="16">
         <f>STDEV(C4:C6)</f>
         <v>6759.4317068818818</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D10" s="16">
         <f>STDEV(D4:D6)</f>
         <v>48.180217240412013</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E10" s="26">
         <f>STDEV(E4:E6)</f>
         <v>6739.2723890145198</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I10" s="24" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16">
-      <c r="I10" s="24" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="16">
       <c r="I11" s="24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16">
+      <c r="I12" s="24" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>962</v>
+      </c>
+      <c r="B18" s="50">
+        <v>4697</v>
+      </c>
+      <c r="C18" s="50">
+        <v>2830</v>
+      </c>
+      <c r="D18" s="50">
+        <v>2711</v>
+      </c>
+      <c r="E18">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>826</v>
+      </c>
+      <c r="B19" s="50">
+        <v>3129</v>
+      </c>
+      <c r="C19" s="50">
+        <v>1978</v>
+      </c>
+      <c r="D19" s="50">
+        <v>1994</v>
+      </c>
+      <c r="E19">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -53463,8 +53745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -53517,7 +53799,7 @@
         <v>3167.4118819999999</v>
       </c>
       <c r="E5" s="20">
-        <f>Condor!D8</f>
+        <f>Condor!D9</f>
         <v>712.33333333333303</v>
       </c>
     </row>
@@ -53536,7 +53818,7 @@
         <v>4707.850641</v>
       </c>
       <c r="E6" s="31">
-        <f>Condor!C8</f>
+        <f>Condor!C9</f>
         <v>5736.0000000000027</v>
       </c>
     </row>
@@ -53557,7 +53839,7 @@
         <v>809.39913009999998</v>
       </c>
       <c r="E7" s="21">
-        <f>Condor!A8</f>
+        <f>Condor!A9</f>
         <v>909.33333333333405</v>
       </c>
     </row>
@@ -53578,7 +53860,7 @@
         <v>8684.6616528400009</v>
       </c>
       <c r="E8" s="21">
-        <f>Condor!E8</f>
+        <f>Condor!E9</f>
         <v>7357.3333333333367</v>
       </c>
     </row>
@@ -53599,7 +53881,7 @@
         <v>1384.7232681954761</v>
       </c>
       <c r="E9" s="21">
-        <f>Condor!B9</f>
+        <f>Condor!B10</f>
         <v>3383.1243449411259</v>
       </c>
     </row>
@@ -56802,10 +57084,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9:R9"/>
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -56814,7 +57096,7 @@
     <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:17">
       <c r="A1" s="14" t="s">
         <v>16</v>
       </c>
@@ -56849,13 +57131,10 @@
         <v>133</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1</v>
       </c>
@@ -56887,18 +57166,14 @@
       </c>
       <c r="P2">
         <f>[1]run1!$O$131</f>
-        <v>4248.3777595267238</v>
+        <v>4243.4671542812066</v>
       </c>
       <c r="Q2">
         <f>[1]run1!$O$72</f>
         <v>1212.8018984285716</v>
       </c>
-      <c r="R2">
-        <f>SUM(P2:Q2)</f>
-        <v>5461.1796579552956</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>2</v>
       </c>
@@ -56907,42 +57182,62 @@
       </c>
       <c r="P3">
         <f>[1]run2!$O$131</f>
-        <v>4744.688989435047</v>
+        <v>4707.8597792293331</v>
       </c>
       <c r="Q3">
         <f>[1]run2!$O$67</f>
         <v>1254.3317010400001</v>
       </c>
-      <c r="R3">
-        <f>SUM(P3:Q3)</f>
-        <v>5999.0206904750466</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="O4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="P4">
+        <f>[1]run3!$O$131</f>
+        <v>3879.476980005943</v>
+      </c>
+      <c r="Q4">
+        <f>[1]run3!$O$61</f>
+        <v>2148.8040556623728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="O5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="P5">
+        <f>[1]run4!$O$127</f>
+        <v>4722.518188808127</v>
+      </c>
+      <c r="Q5">
+        <f>[1]run4!$O$62</f>
+        <v>1091.8222408393551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="O6">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="P6">
+        <f>[1]run5!$O$131</f>
+        <v>4306.1173639416338</v>
+      </c>
+      <c r="Q6">
+        <f>[1]run5!$O$68</f>
+        <v>1194.1639064690908</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="B8">
         <f>AVERAGE(B2:B6)</f>
         <v>421.76157190086724</v>
@@ -56971,37 +57266,29 @@
         <f t="shared" si="0"/>
         <v>1235.8584735619688</v>
       </c>
-      <c r="O8" s="50" t="s">
+      <c r="O8" s="45" t="s">
         <v>131</v>
       </c>
       <c r="P8">
         <f>AVERAGE(P2:P7)</f>
-        <v>4496.533374480885</v>
+        <v>4371.8878932532489</v>
       </c>
       <c r="Q8">
         <f>AVERAGE(Q2:Q7)</f>
-        <v>1233.5667997342857</v>
-      </c>
-      <c r="R8">
-        <f>SUM(P8:Q8)</f>
-        <v>5730.1001742151711</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
+        <v>1380.3847604878779</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="O9" t="s">
         <v>138</v>
       </c>
       <c r="P9">
         <f>STDEV(P2:P6)</f>
-        <v>350.94503624721096</v>
+        <v>353.23677205817961</v>
       </c>
       <c r="Q9">
-        <f t="shared" ref="Q9:R9" si="1">STDEV(Q2:Q6)</f>
-        <v>29.366005047879899</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="1"/>
-        <v>380.31104129509038</v>
+        <f t="shared" ref="Q9" si="1">STDEV(Q2:Q6)</f>
+        <v>433.70154970498379</v>
       </c>
     </row>
   </sheetData>
@@ -57017,10 +57304,199 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="51" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>748</v>
+      </c>
+      <c r="B5" s="50">
+        <v>4202</v>
+      </c>
+      <c r="C5" s="50">
+        <v>2475</v>
+      </c>
+      <c r="D5" s="50">
+        <v>2991</v>
+      </c>
+      <c r="E5">
+        <v>463</v>
+      </c>
+      <c r="F5">
+        <f>(60+37)*60</f>
+        <v>5820</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>854</v>
+      </c>
+      <c r="B6" s="50">
+        <v>1582</v>
+      </c>
+      <c r="C6" s="50">
+        <v>1218</v>
+      </c>
+      <c r="D6">
+        <v>385</v>
+      </c>
+      <c r="E6">
+        <v>269</v>
+      </c>
+      <c r="F6">
+        <f>89*60</f>
+        <v>5340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>880</v>
+      </c>
+      <c r="B7" s="50">
+        <v>1526</v>
+      </c>
+      <c r="C7" s="50">
+        <v>1203</v>
+      </c>
+      <c r="D7">
+        <v>383</v>
+      </c>
+      <c r="E7">
+        <v>273</v>
+      </c>
+      <c r="F7">
+        <f>87*60</f>
+        <v>5220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="16">
+        <f>AVERAGE(A5:A9)</f>
+        <v>827.33333333333337</v>
+      </c>
+      <c r="B11" s="16">
+        <f t="shared" ref="B11:F11" si="0">AVERAGE(B5:B9)</f>
+        <v>2436.6666666666665</v>
+      </c>
+      <c r="C11" s="16">
+        <f t="shared" si="0"/>
+        <v>1632</v>
+      </c>
+      <c r="D11" s="16">
+        <f t="shared" si="0"/>
+        <v>1253</v>
+      </c>
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>335</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" si="0"/>
+        <v>5460</v>
+      </c>
+      <c r="G11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="16">
+        <f>STDEV(A5:A9)</f>
+        <v>69.92376801441219</v>
+      </c>
+      <c r="B12" s="16">
+        <f t="shared" ref="B12:F12" si="1">STDEV(B5:B9)</f>
+        <v>1529.0798976290723</v>
+      </c>
+      <c r="C12" s="16">
+        <f t="shared" si="1"/>
+        <v>730.09793863563266</v>
+      </c>
+      <c r="D12" s="16">
+        <f t="shared" si="1"/>
+        <v>1505.1524839696476</v>
+      </c>
+      <c r="E12" s="16">
+        <f t="shared" si="1"/>
+        <v>110.8692924122816</v>
+      </c>
+      <c r="F12" s="16">
+        <f t="shared" si="1"/>
+        <v>317.49015732775086</v>
+      </c>
+      <c r="G12" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
+      <selection activeCell="U53" sqref="U53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -57044,7 +57520,7 @@
     <col min="21" max="21" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -57076,7 +57552,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:22">
       <c r="A2">
         <v>0</v>
       </c>
@@ -57108,7 +57584,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="A3">
         <v>0</v>
       </c>
@@ -57140,7 +57616,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4">
         <v>1</v>
       </c>
@@ -57172,7 +57648,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22">
       <c r="A5">
         <v>1</v>
       </c>
@@ -57204,7 +57680,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="A6">
         <v>2</v>
       </c>
@@ -57239,7 +57715,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22">
       <c r="A7">
         <v>2</v>
       </c>
@@ -57292,7 +57768,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:22">
       <c r="A8">
         <v>3</v>
       </c>
@@ -57345,7 +57821,7 @@
         <v>609.87942292746834</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9">
         <v>3</v>
       </c>
@@ -57398,7 +57874,7 @@
         <v>79.793807647801373</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:22">
       <c r="A10">
         <v>4</v>
       </c>
@@ -57451,7 +57927,7 @@
         <v>441.41945864232554</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:22">
       <c r="A11">
         <v>4</v>
       </c>
@@ -57483,7 +57959,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:22">
       <c r="A12">
         <v>5</v>
       </c>
@@ -57515,7 +57991,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:22">
       <c r="A13">
         <v>6</v>
       </c>
@@ -57547,7 +58023,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:22">
       <c r="A14">
         <v>6</v>
       </c>
@@ -57578,20 +58054,25 @@
       <c r="J14" t="s">
         <v>47</v>
       </c>
-      <c r="P14" s="45" t="s">
+      <c r="P14" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="Q14" s="45" t="s">
+      <c r="Q14" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="S14" t="s">
+      <c r="S14" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="T14" s="51" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="30">
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+    </row>
+    <row r="15" spans="1:22" ht="30">
       <c r="A15">
         <v>7</v>
       </c>
@@ -57622,26 +58103,33 @@
       <c r="J15" t="s">
         <v>28</v>
       </c>
-      <c r="O15" s="49" t="s">
-        <v>197</v>
-      </c>
-      <c r="P15" s="47">
+      <c r="O15" s="44" t="s">
+        <v>205</v>
+      </c>
+      <c r="P15" s="42">
         <f>Q8/60</f>
         <v>15.752848429242707</v>
       </c>
-      <c r="Q15" s="47">
+      <c r="Q15" s="42">
         <f>Q9/60-P15</f>
         <v>7.5963283108795174</v>
       </c>
-      <c r="R15" s="48">
+      <c r="R15" s="43">
         <v>0</v>
       </c>
-      <c r="S15" s="48">
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" s="43">
         <f>T9/60</f>
         <v>1.3298815950546723</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="30">
+      <c r="V15" s="16">
+        <f>'Interop OSG-XSEDE'!F12/60</f>
+        <v>5.2915026221291814</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="30">
       <c r="A16">
         <v>7</v>
       </c>
@@ -57672,27 +58160,30 @@
       <c r="J16" t="s">
         <v>47</v>
       </c>
-      <c r="O16" s="49" t="s">
-        <v>198</v>
+      <c r="O16" s="44" t="s">
+        <v>197</v>
       </c>
       <c r="P16" s="15">
         <f>'Interop EGI-FG'!Q8/60</f>
-        <v>20.559446662238095</v>
+        <v>23.006412674797964</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
-      <c r="R16" s="46">
+      <c r="R16" s="41">
         <f>'Interop EGI-FG'!P8/60</f>
-        <v>74.942222908014756</v>
-      </c>
-      <c r="S16" s="48"/>
-      <c r="T16">
-        <f>'Interop EGI-FG'!R9/60</f>
-        <v>6.3385173549181726</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+        <v>72.864798220887479</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16" s="43"/>
+      <c r="U16">
+        <f>'Interop EGI-FG'!P9/60</f>
+        <v>5.8872795343029933</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="30">
       <c r="A17">
         <v>8</v>
       </c>
@@ -57723,12 +58214,25 @@
       <c r="J17" t="s">
         <v>28</v>
       </c>
+      <c r="O17" s="52" t="s">
+        <v>206</v>
+      </c>
       <c r="P17">
-        <f>P16/P15*100</f>
-        <v>130.51256574063575</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="16">
+        <f>'Interop OSG-XSEDE'!F11/60-S17</f>
+        <v>50.388888888888893</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" s="16">
+        <f>'Interop OSG-XSEDE'!B11/60</f>
+        <v>40.611111111111107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18">
         <v>8</v>
       </c>
@@ -57760,7 +58264,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:19">
       <c r="A19">
         <v>9</v>
       </c>
@@ -57792,7 +58296,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:19">
       <c r="A20">
         <v>9</v>
       </c>
@@ -57824,7 +58328,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:19">
       <c r="A21">
         <v>10</v>
       </c>
@@ -57856,7 +58360,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:19">
       <c r="A22">
         <v>10</v>
       </c>
@@ -57888,7 +58392,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:19">
       <c r="A23">
         <v>11</v>
       </c>
@@ -57920,7 +58424,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:19">
       <c r="A24">
         <v>11</v>
       </c>
@@ -57952,7 +58456,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:19">
       <c r="A25">
         <v>12</v>
       </c>
@@ -57984,7 +58488,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:19">
       <c r="A26">
         <v>12</v>
       </c>
@@ -58016,7 +58520,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:19">
       <c r="A27">
         <v>13</v>
       </c>
@@ -58048,7 +58552,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:19">
       <c r="A28">
         <v>13</v>
       </c>
@@ -58080,7 +58584,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:19">
       <c r="A29">
         <v>14</v>
       </c>
@@ -58112,7 +58616,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:19">
       <c r="A30">
         <v>14</v>
       </c>
@@ -58144,7 +58648,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:19">
       <c r="A31">
         <v>15</v>
       </c>
@@ -58176,7 +58680,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:19">
       <c r="A32">
         <v>15</v>
       </c>
@@ -58209,6 +58713,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="T14:V14"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
4. OSG run considered
git-svn-id: file://localhost/tmp/svn2git/svn@6436 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="0" windowWidth="47000" windowHeight="28240" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="14780" yWindow="0" windowWidth="47000" windowHeight="28240" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -2996,7 +2996,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0">
-                  <c:v>40.61111111111111</c:v>
+                  <c:v>37.30416666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3038,7 +3038,7 @@
                     <c:v>1.329881595054672</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.291502622129181</c:v>
+                    <c:v>9.983319421247957</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3053,7 +3053,7 @@
                     <c:v>1.329881595054672</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>5.291502622129181</c:v>
+                    <c:v>9.983319421247957</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3089,7 +3089,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0">
-                  <c:v>50.3888888888889</c:v>
+                  <c:v>49.19583333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -57306,8 +57306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -57420,30 +57420,51 @@
         <v>5220</v>
       </c>
     </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>763</v>
+      </c>
+      <c r="B8" s="50">
+        <v>1643</v>
+      </c>
+      <c r="C8" s="50">
+        <v>1203</v>
+      </c>
+      <c r="D8">
+        <v>96</v>
+      </c>
+      <c r="E8">
+        <v>782</v>
+      </c>
+      <c r="F8">
+        <f>73*60</f>
+        <v>4380</v>
+      </c>
+    </row>
     <row r="11" spans="1:7">
       <c r="A11" s="16">
         <f>AVERAGE(A5:A9)</f>
-        <v>827.33333333333337</v>
+        <v>811.25</v>
       </c>
       <c r="B11" s="16">
         <f t="shared" ref="B11:F11" si="0">AVERAGE(B5:B9)</f>
-        <v>2436.6666666666665</v>
+        <v>2238.25</v>
       </c>
       <c r="C11" s="16">
         <f t="shared" si="0"/>
-        <v>1632</v>
+        <v>1524.75</v>
       </c>
       <c r="D11" s="16">
         <f t="shared" si="0"/>
-        <v>1253</v>
+        <v>963.75</v>
       </c>
       <c r="E11" s="16">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>446.75</v>
       </c>
       <c r="F11" s="16">
         <f t="shared" si="0"/>
-        <v>5460</v>
+        <v>5190</v>
       </c>
       <c r="G11" t="s">
         <v>131</v>
@@ -57452,27 +57473,27 @@
     <row r="12" spans="1:7">
       <c r="A12" s="16">
         <f>STDEV(A5:A9)</f>
-        <v>69.92376801441219</v>
+        <v>65.530527237311318</v>
       </c>
       <c r="B12" s="16">
         <f t="shared" ref="B12:F12" si="1">STDEV(B5:B9)</f>
-        <v>1529.0798976290723</v>
+        <v>1310.0382627999841</v>
       </c>
       <c r="C12" s="16">
         <f t="shared" si="1"/>
-        <v>730.09793863563266</v>
+        <v>633.53946207004344</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="1"/>
-        <v>1505.1524839696476</v>
+        <v>1358.302218457537</v>
       </c>
       <c r="E12" s="16">
         <f t="shared" si="1"/>
-        <v>110.8692924122816</v>
+        <v>241.13671779027487</v>
       </c>
       <c r="F12" s="16">
         <f t="shared" si="1"/>
-        <v>317.49015732775086</v>
+        <v>598.99916527487744</v>
       </c>
       <c r="G12" t="s">
         <v>204</v>
@@ -57495,7 +57516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
+    <sheetView topLeftCell="J2" workbookViewId="0">
       <selection activeCell="U53" sqref="U53"/>
     </sheetView>
   </sheetViews>
@@ -58126,7 +58147,7 @@
       </c>
       <c r="V15" s="16">
         <f>'Interop OSG-XSEDE'!F12/60</f>
-        <v>5.2915026221291814</v>
+        <v>9.9833194212479572</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="30">
@@ -58222,14 +58243,14 @@
       </c>
       <c r="Q17" s="16">
         <f>'Interop OSG-XSEDE'!F11/60-S17</f>
-        <v>50.388888888888893</v>
+        <v>49.195833333333333</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
       <c r="S17" s="16">
         <f>'Interop OSG-XSEDE'!B11/60</f>
-        <v>40.611111111111107</v>
+        <v>37.304166666666667</v>
       </c>
     </row>
     <row r="18" spans="1:19">

</xml_diff>

<commit_message>
condensed Swift to 1 paragraph
git-svn-id: file://localhost/tmp/svn2git/svn@6451 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="0" windowWidth="47000" windowHeight="28240" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="14780" yWindow="0" windowWidth="47000" windowHeight="28240" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -709,12 +709,12 @@
     <t>stddev</t>
   </si>
   <si>
-    <t>FutureGrid/
-XSEDE:Kraken</t>
+    <t>XSEDE::Kraken/
+FutureGrid</t>
   </si>
   <si>
-    <t>OSG/
-XSEDE:QB</t>
+    <t>XSEDE::QB/
+OSG</t>
   </si>
 </sst>
 </file>
@@ -1027,7 +1027,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1110,6 +1110,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="111">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -2938,13 +2939,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>FutureGrid/_x000d_XSEDE:Kraken</c:v>
+                  <c:v>XSEDE::Kraken/_x000d_FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>EGI/_x000d_FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>OSG/_x000d_XSEDE:QB</c:v>
+                  <c:v>XSEDE::QB/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3065,13 +3066,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>FutureGrid/_x000d_XSEDE:Kraken</c:v>
+                  <c:v>XSEDE::Kraken/_x000d_FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>EGI/_x000d_FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>OSG/_x000d_XSEDE:QB</c:v>
+                  <c:v>XSEDE::QB/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3153,13 +3154,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>FutureGrid/_x000d_XSEDE:Kraken</c:v>
+                  <c:v>XSEDE::Kraken/_x000d_FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>EGI/_x000d_FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>OSG/_x000d_XSEDE:QB</c:v>
+                  <c:v>XSEDE::QB/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -57306,8 +57307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -57446,7 +57447,7 @@
         <f>AVERAGE(A5:A9)</f>
         <v>811.25</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="54">
         <f t="shared" ref="B11:F11" si="0">AVERAGE(B5:B9)</f>
         <v>2238.25</v>
       </c>
@@ -57462,7 +57463,7 @@
         <f t="shared" si="0"/>
         <v>446.75</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="54">
         <f t="shared" si="0"/>
         <v>5190</v>
       </c>
@@ -57516,8 +57517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView topLeftCell="J2" workbookViewId="0">
-      <selection activeCell="U53" sqref="U53"/>
+    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
working on performance with pilot data section
git-svn-id: file://localhost/tmp/svn2git/svn@7092 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="0" windowWidth="47000" windowHeight="28240" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30440" windowHeight="28360" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -1088,6 +1088,14 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1100,17 +1108,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="111">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -1421,11 +1421,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="861616728"/>
-        <c:axId val="861619704"/>
+        <c:axId val="2122957096"/>
+        <c:axId val="2122995384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="861616728"/>
+        <c:axId val="2122957096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1435,7 +1435,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="861619704"/>
+        <c:crossAx val="2122995384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1443,7 +1443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="861619704"/>
+        <c:axId val="2122995384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,7 +1454,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="861616728"/>
+        <c:crossAx val="2122957096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1752,11 +1752,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="861662584"/>
-        <c:axId val="861668312"/>
+        <c:axId val="2120739624"/>
+        <c:axId val="2120745352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="861662584"/>
+        <c:axId val="2120739624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1790,7 +1790,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="861668312"/>
+        <c:crossAx val="2120745352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1798,7 +1798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="861668312"/>
+        <c:axId val="2120745352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1809,7 +1809,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="861662584"/>
+        <c:crossAx val="2120739624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2121,11 +2121,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="861728504"/>
-        <c:axId val="861734216"/>
+        <c:axId val="2123066440"/>
+        <c:axId val="2123072152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="861728504"/>
+        <c:axId val="2123066440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,7 +2158,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="861734216"/>
+        <c:crossAx val="2123072152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2166,7 +2166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="861734216"/>
+        <c:axId val="2123072152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2195,7 +2195,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="861728504"/>
+        <c:crossAx val="2123066440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2461,11 +2461,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="861805960"/>
-        <c:axId val="861809000"/>
+        <c:axId val="2123522568"/>
+        <c:axId val="2117901464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="861805960"/>
+        <c:axId val="2123522568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2487,7 +2487,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="861809000"/>
+        <c:crossAx val="2117901464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2495,7 +2495,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="861809000"/>
+        <c:axId val="2117901464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -2552,7 +2552,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="861805960"/>
+        <c:crossAx val="2123522568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2780,11 +2780,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="861843688"/>
-        <c:axId val="861846728"/>
+        <c:axId val="2121986600"/>
+        <c:axId val="2121989640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="861843688"/>
+        <c:axId val="2121986600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2806,7 +2806,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="861846728"/>
+        <c:crossAx val="2121989640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2814,7 +2814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="861846728"/>
+        <c:axId val="2121989640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2863,7 +2863,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="861843688"/>
+        <c:crossAx val="2121986600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3194,11 +3194,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="861356040"/>
-        <c:axId val="861352968"/>
+        <c:axId val="2123173064"/>
+        <c:axId val="2123176328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="861356040"/>
+        <c:axId val="2123173064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3220,7 +3220,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="861352968"/>
+        <c:crossAx val="2123176328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3228,7 +3228,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="861352968"/>
+        <c:axId val="2123176328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3283,7 +3283,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="861356040"/>
+        <c:crossAx val="2123173064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3546,7 +3546,7 @@
       <sheetName val="run5 old"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="72">
           <cell r="O72">
@@ -3607,13 +3607,13 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -19792,6 +19792,92 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="47" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I54:K65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
@@ -19878,92 +19964,6 @@
   <dataFields count="2">
     <dataField name="Mittelwert - Kraken" fld="2" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Kraken2" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="47" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
     <format dxfId="1">
@@ -20771,16 +20771,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
@@ -53575,16 +53575,16 @@
       <c r="A7">
         <v>962</v>
       </c>
-      <c r="B7" s="50">
+      <c r="B7" s="46">
         <v>2830</v>
       </c>
       <c r="C7">
         <v>872</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="46">
         <v>2711</v>
       </c>
-      <c r="E7" s="50">
+      <c r="E7" s="46">
         <v>4697</v>
       </c>
       <c r="F7" s="15">
@@ -53599,16 +53599,16 @@
       <c r="A8">
         <v>826</v>
       </c>
-      <c r="B8" s="50">
+      <c r="B8" s="46">
         <v>1978</v>
       </c>
       <c r="C8">
         <v>190</v>
       </c>
-      <c r="D8" s="50">
+      <c r="D8" s="46">
         <v>1994</v>
       </c>
-      <c r="E8" s="50">
+      <c r="E8" s="46">
         <v>3129</v>
       </c>
       <c r="F8" s="15">
@@ -53701,13 +53701,13 @@
       <c r="A18">
         <v>962</v>
       </c>
-      <c r="B18" s="50">
+      <c r="B18" s="46">
         <v>4697</v>
       </c>
-      <c r="C18" s="50">
+      <c r="C18" s="46">
         <v>2830</v>
       </c>
-      <c r="D18" s="50">
+      <c r="D18" s="46">
         <v>2711</v>
       </c>
       <c r="E18">
@@ -53718,13 +53718,13 @@
       <c r="A19">
         <v>826</v>
       </c>
-      <c r="B19" s="50">
+      <c r="B19" s="46">
         <v>3129</v>
       </c>
-      <c r="C19" s="50">
+      <c r="C19" s="46">
         <v>1978</v>
       </c>
-      <c r="D19" s="50">
+      <c r="D19" s="46">
         <v>1994</v>
       </c>
       <c r="E19">
@@ -53746,7 +53746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
@@ -57327,13 +57327,13 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="2" t="s">
         <v>152</v>
       </c>
@@ -57362,13 +57362,13 @@
       <c r="A5">
         <v>748</v>
       </c>
-      <c r="B5" s="50">
+      <c r="B5" s="46">
         <v>4202</v>
       </c>
-      <c r="C5" s="50">
+      <c r="C5" s="46">
         <v>2475</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D5" s="46">
         <v>2991</v>
       </c>
       <c r="E5">
@@ -57383,10 +57383,10 @@
       <c r="A6">
         <v>854</v>
       </c>
-      <c r="B6" s="50">
+      <c r="B6" s="46">
         <v>1582</v>
       </c>
-      <c r="C6" s="50">
+      <c r="C6" s="46">
         <v>1218</v>
       </c>
       <c r="D6">
@@ -57404,10 +57404,10 @@
       <c r="A7">
         <v>880</v>
       </c>
-      <c r="B7" s="50">
+      <c r="B7" s="46">
         <v>1526</v>
       </c>
-      <c r="C7" s="50">
+      <c r="C7" s="46">
         <v>1203</v>
       </c>
       <c r="D7">
@@ -57425,10 +57425,10 @@
       <c r="A8">
         <v>763</v>
       </c>
-      <c r="B8" s="50">
+      <c r="B8" s="46">
         <v>1643</v>
       </c>
-      <c r="C8" s="50">
+      <c r="C8" s="46">
         <v>1203</v>
       </c>
       <c r="D8">
@@ -57447,7 +57447,7 @@
         <f>AVERAGE(A5:A9)</f>
         <v>811.25</v>
       </c>
-      <c r="B11" s="54">
+      <c r="B11" s="49">
         <f t="shared" ref="B11:F11" si="0">AVERAGE(B5:B9)</f>
         <v>2238.25</v>
       </c>
@@ -57463,7 +57463,7 @@
         <f t="shared" si="0"/>
         <v>446.75</v>
       </c>
-      <c r="F11" s="54">
+      <c r="F11" s="49">
         <f t="shared" si="0"/>
         <v>5190</v>
       </c>
@@ -57517,7 +57517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" workbookViewId="0">
+    <sheetView topLeftCell="J2" workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
@@ -58076,10 +58076,10 @@
       <c r="J14" t="s">
         <v>47</v>
       </c>
-      <c r="P14" s="53" t="s">
+      <c r="P14" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="Q14" s="53" t="s">
+      <c r="Q14" s="48" t="s">
         <v>152</v>
       </c>
       <c r="R14" s="2" t="s">
@@ -58088,11 +58088,11 @@
       <c r="S14" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="T14" s="51" t="s">
+      <c r="T14" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
+      <c r="U14" s="54"/>
+      <c r="V14" s="54"/>
     </row>
     <row r="15" spans="1:22" ht="30">
       <c r="A15">
@@ -58236,7 +58236,7 @@
       <c r="J17" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="52" t="s">
+      <c r="O17" s="47" t="s">
         <v>206</v>
       </c>
       <c r="P17">

</xml_diff>

<commit_message>
some more work on performance data added Mark's SRM data
git-svn-id: file://localhost/tmp/svn2git/svn@7151 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
+  <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21060" yWindow="0" windowWidth="29160" windowHeight="28360" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="19940" yWindow="0" windowWidth="29160" windowHeight="28360" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -23,20 +23,21 @@
     <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_1bj_results" localSheetId="2">'BJ w Staging'!$A$20:$J$21</definedName>
     <definedName name="_2bj_results" localSheetId="3">'BJ (FG multi)'!$A$1:$J$13</definedName>
-    <definedName name="bj_singleresource" localSheetId="2">'BJ w Staging'!$A$1:$J$31</definedName>
+    <definedName name="bj_singleresource" localSheetId="2">'BJ w Staging'!$A$1:$J$35</definedName>
     <definedName name="data_interop" localSheetId="10">'Interop '!$A$1:$J$32</definedName>
     <definedName name="daten" localSheetId="1">BigJob!$A$1:$J$64</definedName>
     <definedName name="daten_1" localSheetId="7">'Raw (BJ)'!$A$1:$J$109</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId13"/>
-    <pivotCache cacheId="1" r:id="rId14"/>
-    <pivotCache cacheId="2" r:id="rId15"/>
-    <pivotCache cacheId="3" r:id="rId16"/>
-    <pivotCache cacheId="4" r:id="rId17"/>
-    <pivotCache cacheId="24" r:id="rId18"/>
+    <pivotCache cacheId="21" r:id="rId13"/>
+    <pivotCache cacheId="22" r:id="rId14"/>
+    <pivotCache cacheId="23" r:id="rId15"/>
+    <pivotCache cacheId="24" r:id="rId16"/>
+    <pivotCache cacheId="25" r:id="rId17"/>
+    <pivotCache cacheId="26" r:id="rId18"/>
     <pivotCache cacheId="31" r:id="rId19"/>
   </pivotCaches>
   <extLst>
@@ -49,7 +50,23 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="2bj-results.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="1" name="1bj_results.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:experiments-SC12:results:1bj_results.txt" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="2bj-results.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:experiments-SC12:results:2bj-results.txt" comma="1">
       <textFields count="10">
         <textField/>
@@ -65,7 +82,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="bj-singleresource.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="bj-singleresource.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:Dropbox:SAGA:papers:troy:pstar:perf:sc:bj-singleresource.txt" comma="1">
       <textFields count="10">
         <textField/>
@@ -81,14 +98,14 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="data-interop.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="data-interop.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:data-interop.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="daten.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="daten.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields count="10">
         <textField/>
@@ -104,21 +121,21 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="daten.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" name="daten.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="daten.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="7" name="daten.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="daten.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="8" name="daten.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
@@ -129,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="275">
   <si>
     <t>bfast</t>
   </si>
@@ -934,6 +951,30 @@
   <si>
     <t>Runtime</t>
   </si>
+  <si>
+    <t>bigjob:bj-ca2a8246-92c7-11e1-83ec-bc305b7ee8dc:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-e99b42c6-92fb-11e1-83ec-bc305b7ee8dc:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pilot Overhead </t>
+  </si>
+  <si>
+    <t>bigjob:bj-3ff74b52-935f-11e1-ac66-00259019a084:trestles.sdsc.edu</t>
+  </si>
+  <si>
+    <t>bigjob:bj-3f8cbd32-93a0-11e1-bbde-bc305b7ee8dc:trestles.sdsc.edu</t>
+  </si>
+  <si>
+    <t>pbs-ssh://pmantha@trestles.sdsc.edu</t>
+  </si>
+  <si>
+    <t>(from pilot-data-exp.xlsx)</t>
+  </si>
+  <si>
+    <t>Overhead</t>
+  </si>
 </sst>
 </file>
 
@@ -1192,8 +1233,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1391,6 +1440,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1406,20 +1467,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="139">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1485,6 +1534,10 @@
     <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1550,35 +1603,15 @@
     <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="14">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="29" formatCode="mm:ss.0"/>
@@ -1775,11 +1808,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2082388200"/>
-        <c:axId val="2082389448"/>
+        <c:axId val="2141954728"/>
+        <c:axId val="2141957704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2082388200"/>
+        <c:axId val="2141954728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1789,7 +1822,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082389448"/>
+        <c:crossAx val="2141957704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1797,7 +1830,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082389448"/>
+        <c:axId val="2141957704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1808,7 +1841,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082388200"/>
+        <c:crossAx val="2141954728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2106,11 +2139,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2081920440"/>
-        <c:axId val="2081914696"/>
+        <c:axId val="2141913640"/>
+        <c:axId val="2141895688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2081920440"/>
+        <c:axId val="2141913640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2144,7 +2177,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081914696"/>
+        <c:crossAx val="2141895688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2152,7 +2185,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081914696"/>
+        <c:axId val="2141895688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2163,7 +2196,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081920440"/>
+        <c:crossAx val="2141913640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2215,7 +2248,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2476,11 +2508,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2078476200"/>
-        <c:axId val="2078470472"/>
+        <c:axId val="2142818376"/>
+        <c:axId val="2142824088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2078476200"/>
+        <c:axId val="2142818376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2507,14 +2539,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078470472"/>
+        <c:crossAx val="2142824088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2522,7 +2553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2078470472"/>
+        <c:axId val="2142824088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2545,21 +2576,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078476200"/>
+        <c:crossAx val="2142818376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2726,7 +2755,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Total!$B$19:$E$19</c:f>
+                <c:f>Total!$B$20:$E$20</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -2747,7 +2776,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Total!$B$19:$E$19</c:f>
+                <c:f>Total!$B$20:$E$20</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="4"/>
@@ -2819,11 +2848,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2078489992"/>
-        <c:axId val="2078492792"/>
+        <c:axId val="2144770296"/>
+        <c:axId val="2144764920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2078489992"/>
+        <c:axId val="2144770296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2845,7 +2874,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078492792"/>
+        <c:crossAx val="2144764920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2853,7 +2882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2078492792"/>
+        <c:axId val="2144764920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -2910,7 +2939,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078489992"/>
+        <c:crossAx val="2144770296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3138,11 +3167,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2078414264"/>
-        <c:axId val="2078411208"/>
+        <c:axId val="2141847192"/>
+        <c:axId val="2141825800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2078414264"/>
+        <c:axId val="2141847192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3164,7 +3193,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078411208"/>
+        <c:crossAx val="2141825800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3172,7 +3201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2078411208"/>
+        <c:axId val="2141825800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3221,7 +3250,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2078414264"/>
+        <c:crossAx val="2141847192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3325,10 +3354,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>224.4480902777783</c:v>
+                  <c:v>191.0096412556054</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>245.45</c:v>
+                  <c:v>319.8666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>115.4936172222222</c:v>
@@ -3357,6 +3386,59 @@
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(Total!$F$20,Total!$G$20,Total!$H$20,Total!$D$20,Total!$E$20)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>35.03971545</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>294.4423239772857</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20.84980258491097</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23.07872113659127</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>56.38540574901877</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(Total!$F$20,Total!$G$20,Total!$H$20,Total!$D$20,Total!$E$20)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>35.03971545</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>294.4423239772857</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20.84980258491097</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23.07872113659127</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>56.38540574901877</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>(Total!$F$4,Total!$G$4,Total!$H$4,Total!$D$4,Total!$E$4)</c:f>
@@ -3387,10 +3469,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18.29373737222161</c:v>
+                  <c:v>26.9553659860612</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>169.3827795500001</c:v>
+                  <c:v>16.62462746549255</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24.56504025566889</c:v>
@@ -3415,11 +3497,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2142638296"/>
-        <c:axId val="2142615928"/>
+        <c:axId val="2142950248"/>
+        <c:axId val="2142953224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142638296"/>
+        <c:axId val="2142950248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3441,7 +3523,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142615928"/>
+        <c:crossAx val="2142953224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3449,7 +3531,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142615928"/>
+        <c:axId val="2142953224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3494,7 +3576,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142638296"/>
+        <c:crossAx val="2142950248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3828,11 +3910,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2081796568"/>
-        <c:axId val="2081793288"/>
+        <c:axId val="2144653800"/>
+        <c:axId val="2144639000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2081796568"/>
+        <c:axId val="2144653800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3854,7 +3936,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081793288"/>
+        <c:crossAx val="2144639000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3862,7 +3944,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081793288"/>
+        <c:axId val="2144639000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3917,7 +3999,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081796568"/>
+        <c:crossAx val="2144653800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3929,7 +4011,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4071,7 +4152,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4095,13 +4176,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>615950</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4127,13 +4208,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>102</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4518,63 +4599,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41030.486125115742" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="30">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J31" sheet="BJ w Staging"/>
-  </cacheSource>
-  <cacheFields count="10">
-    <cacheField name="Run" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2"/>
-    </cacheField>
-    <cacheField name="BJ" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="#Nodes" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="128"/>
-    </cacheField>
-    <cacheField name="#cores/node" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="8" maxValue="16"/>
-    </cacheField>
-    <cacheField name="#jobs" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="128" count="7">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="4"/>
-        <n v="8"/>
-        <n v="16"/>
-        <n v="32"/>
-        <n v="128"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Queuing Time" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="23.373319864300001" maxValue="22768.135295200002"/>
-    </cacheField>
-    <cacheField name="BJ Runtime" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="727.22062802300002" maxValue="47417.862745999999"/>
-    </cacheField>
-    <cacheField name="Total Runtime" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="728.41032099699999" maxValue="47419.311981899999"/>
-    </cacheField>
-    <cacheField name="Coordination URL" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="LRMS URL" numFmtId="0">
-      <sharedItems count="3">
-        <s v="pbs-ssh://luckow@trestles.sdsc.edu"/>
-        <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
-        <s v="sge-ssh://login2.ls4.tacc.utexas.edu"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41030.557750578701" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="12">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:J13" sheet="BJ (FG multi)"/>
@@ -4623,6 +4647,64 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41030.902490740744" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="34">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:J35" sheet="BJ w Staging"/>
+  </cacheSource>
+  <cacheFields count="10">
+    <cacheField name="Run" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2"/>
+    </cacheField>
+    <cacheField name="BJ" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="#Nodes" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="128"/>
+    </cacheField>
+    <cacheField name="#cores/node" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="8" maxValue="32"/>
+    </cacheField>
+    <cacheField name="#jobs" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="128" count="7">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="4"/>
+        <n v="8"/>
+        <n v="16"/>
+        <n v="32"/>
+        <n v="128"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Queuing Time" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.6857481002799997" maxValue="25158.968379999998"/>
+    </cacheField>
+    <cacheField name="BJ Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="727.22062802300002" maxValue="47417.862745999999"/>
+    </cacheField>
+    <cacheField name="Total Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="728.41032099699999" maxValue="47419.311981899999"/>
+    </cacheField>
+    <cacheField name="Coordination URL" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="LRMS URL" numFmtId="0">
+      <sharedItems count="4">
+        <s v="pbs-ssh://luckow@trestles.sdsc.edu"/>
+        <s v="pbs-ssh://pmantha@trestles.sdsc.edu"/>
+        <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
+        <s v="sge-ssh://login2.ls4.tacc.utexas.edu"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="202">
   <r>
@@ -20562,7 +20644,156 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="30">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="12">
+  <r>
+    <x v="0"/>
+    <s v="bigjob:bj-aff746cc-917b-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="30.872246026999999"/>
+    <n v="9624.9724540700008"/>
+    <n v="10142.329308"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="bigjob:bj-b5f29158-917b-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="35.5793919563"/>
+    <n v="9724.9150030599994"/>
+    <n v="10142.329308"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="bigjob:bj-bbaf26a6-917b-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="37.014262914699998"/>
+    <n v="10108.4680591"/>
+    <n v="10142.329308"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="bigjob:bj-bda24fa6-917b-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="38.351100921600001"/>
+    <n v="10140.9886279"/>
+    <n v="10142.329308"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="bigjob:bj-5553695e-9193-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="30.8952770233"/>
+    <n v="7480.1843180699998"/>
+    <n v="8313.7364161000005"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="bigjob:bj-5b809c7a-9193-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="35.605715990100002"/>
+    <n v="7641.5092239400001"/>
+    <n v="8313.7364161000005"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="bigjob:bj-614cd920-9193-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="832.90166497200005"/>
+    <n v="8310.0284941200007"/>
+    <n v="8313.7364161000005"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="bigjob:bj-6327ea6e-9193-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="800.63245511100001"/>
+    <n v="8312.4067189699999"/>
+    <n v="8313.7364161000005"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="bigjob:bj-b8726e32-91a6-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="30.460361003900001"/>
+    <n v="7255.1056170499996"/>
+    <n v="7749.2488341300004"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="bigjob:bj-be8f4b0a-91a6-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="35.1687569618"/>
+    <n v="7421.4965550899997"/>
+    <n v="7749.2488341300004"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="bigjob:bj-c45aee54-91a6-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="52.7022640705"/>
+    <n v="7684.46806216"/>
+    <n v="7749.2488341300004"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="bigjob:bj-c625fd3c-91a6-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="32"/>
+    <n v="8"/>
+    <n v="32"/>
+    <n v="119.38696813599999"/>
+    <n v="7747.8027331800004"/>
+    <n v="7749.2488341300004"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="34">
   <r>
     <n v="0"/>
     <s v="bigjob:bj-887db1c6-910d-11e1-b0d6-00259019a082:trestles.sdsc.edu"/>
@@ -20745,6 +20976,30 @@
   </r>
   <r>
     <n v="0"/>
+    <s v="bigjob:bj-3ff74b52-935f-11e1-ac66-00259019a084:trestles.sdsc.edu"/>
+    <n v="128"/>
+    <n v="16"/>
+    <x v="6"/>
+    <n v="25158.968379999998"/>
+    <n v="36750.259590000001"/>
+    <n v="36750.694069999998"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-3f8cbd32-93a0-11e1-bbde-bc305b7ee8dc:trestles.sdsc.edu"/>
+    <n v="128"/>
+    <n v="32"/>
+    <x v="6"/>
+    <n v="2217.9745159099998"/>
+    <n v="13175.735358"/>
+    <n v="13178.010752"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="0"/>
     <s v="bigjob:bj-5c9ed678-9259-11e1-83ec-bc305b7ee8dc:india.futuregrid.org"/>
     <n v="128"/>
     <n v="8"/>
@@ -20753,7 +21008,31 @@
     <n v="47417.862745999999"/>
     <n v="47419.311981899999"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-ca2a8246-92c7-11e1-83ec-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="128"/>
+    <n v="8"/>
+    <x v="6"/>
+    <n v="5.7084000110600002"/>
+    <n v="22380.652238800001"/>
+    <n v="22382.094851999998"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-e99b42c6-92fb-11e1-83ec-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="128"/>
+    <n v="8"/>
+    <x v="6"/>
+    <n v="4.6857481002799997"/>
+    <n v="13308.208080099999"/>
+    <n v="13309.640333200001"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
   </r>
   <r>
     <n v="0"/>
@@ -20765,7 +21044,7 @@
     <n v="934.00202012099999"/>
     <n v="935.09974002800004"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="1"/>
@@ -20777,7 +21056,7 @@
     <n v="756.88640379900005"/>
     <n v="758.091012955"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="2"/>
@@ -20789,7 +21068,7 @@
     <n v="727.96860408800001"/>
     <n v="729.173197985"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="0"/>
@@ -20801,7 +21080,7 @@
     <n v="927.508314133"/>
     <n v="928.868350029"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="1"/>
@@ -20813,7 +21092,7 @@
     <n v="912.68654990200002"/>
     <n v="913.90338492399997"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="2"/>
@@ -20825,7 +21104,7 @@
     <n v="727.22062802300002"/>
     <n v="728.41032099699999"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="0"/>
@@ -20837,7 +21116,7 @@
     <n v="2510.5651390600001"/>
     <n v="2511.7870490599998"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="1"/>
@@ -20849,7 +21128,7 @@
     <n v="1207.55374312"/>
     <n v="1208.7523281599999"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="2"/>
@@ -20861,7 +21140,7 @@
     <n v="866.61979699100004"/>
     <n v="867.81867504100001"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="0"/>
@@ -20873,7 +21152,7 @@
     <n v="1318.27436304"/>
     <n v="1319.4774529900001"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="1"/>
@@ -20885,7 +21164,7 @@
     <n v="1207.09737587"/>
     <n v="1208.20039296"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="2"/>
@@ -20897,7 +21176,7 @@
     <n v="4049.5441341400001"/>
     <n v="4050.7455921199999"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="0"/>
@@ -20909,7 +21188,7 @@
     <n v="2503.21842599"/>
     <n v="2504.4764480600002"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="1"/>
@@ -20921,162 +21200,99 @@
     <n v="1988.56460881"/>
     <n v="1989.9456028899999"/>
     <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="12">
-  <r>
-    <x v="0"/>
-    <s v="bigjob:bj-aff746cc-917b-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="30.872246026999999"/>
-    <n v="9624.9724540700008"/>
-    <n v="10142.329308"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="bigjob:bj-b5f29158-917b-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="35.5793919563"/>
-    <n v="9724.9150030599994"/>
-    <n v="10142.329308"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="bigjob:bj-bbaf26a6-917b-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="37.014262914699998"/>
-    <n v="10108.4680591"/>
-    <n v="10142.329308"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="bigjob:bj-bda24fa6-917b-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="38.351100921600001"/>
-    <n v="10140.9886279"/>
-    <n v="10142.329308"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <s v="bigjob:bj-5553695e-9193-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="30.8952770233"/>
-    <n v="7480.1843180699998"/>
-    <n v="8313.7364161000005"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <s v="bigjob:bj-5b809c7a-9193-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="35.605715990100002"/>
-    <n v="7641.5092239400001"/>
-    <n v="8313.7364161000005"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <s v="bigjob:bj-614cd920-9193-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="832.90166497200005"/>
-    <n v="8310.0284941200007"/>
-    <n v="8313.7364161000005"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <s v="bigjob:bj-6327ea6e-9193-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="800.63245511100001"/>
-    <n v="8312.4067189699999"/>
-    <n v="8313.7364161000005"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="bigjob:bj-b8726e32-91a6-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="30.460361003900001"/>
-    <n v="7255.1056170499996"/>
-    <n v="7749.2488341300004"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="bigjob:bj-be8f4b0a-91a6-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="35.1687569618"/>
-    <n v="7421.4965550899997"/>
-    <n v="7749.2488341300004"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@sierra.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="bigjob:bj-c45aee54-91a6-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="52.7022640705"/>
-    <n v="7684.46806216"/>
-    <n v="7749.2488341300004"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="bigjob:bj-c625fd3c-91a6-11e1-a9eb-bc305b7ee8dc:india.futuregrid.org"/>
-    <n v="32"/>
-    <n v="8"/>
-    <n v="32"/>
-    <n v="119.38696813599999"/>
-    <n v="7747.8027331800004"/>
-    <n v="7749.2488341300004"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
+    <x v="3"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="47" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I54:K65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -21164,93 +21380,7 @@
     <dataField name="STABW - Kraken2" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="9">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="47" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="10">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -21264,7 +21394,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I4:K21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -21363,7 +21493,7 @@
     <dataField name="STABW - Kraken" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="11">
-    <format dxfId="21">
+    <format dxfId="13">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21375,7 +21505,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="12">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -21384,7 +21514,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="11">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21399,10 +21529,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="10">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="9">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -21411,7 +21541,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="8">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -21420,7 +21550,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="7">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21432,7 +21562,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -21441,7 +21571,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="5">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21453,7 +21583,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -21462,7 +21592,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="11">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21485,7 +21615,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="M21:AB31" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -21623,8 +21753,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="M1:Q19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="M1:Q21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -21647,10 +21777,11 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="4">
+      <items count="5">
         <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
         <item x="1"/>
-        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -21659,7 +21790,7 @@
     <field x="9"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="17">
+  <rowItems count="19">
     <i>
       <x/>
     </i>
@@ -21708,6 +21839,12 @@
     <i r="1">
       <x v="5"/>
     </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -21733,7 +21870,7 @@
     <dataField name="Mittelwert - Queuing Time" fld="5" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Mittelwert - BJ Runtime" fld="6" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Queuing Time2" fld="5" subtotal="stdDev" baseField="0" baseItem="0"/>
-    <dataField name="STABW - Queuing Time" fld="5" subtotal="stdDev" baseField="0" baseItem="0"/>
+    <dataField name="STABW - BJ Runtime" fld="6" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -21745,7 +21882,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="M2:O7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -21799,7 +21936,7 @@
     <dataField name="Maximum - BJ Runtime" fld="6" subtotal="max" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="3">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -21813,7 +21950,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="O6:U10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -21888,23 +22025,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-singleresource" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-singleresource" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2bj-results" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1bj_results" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten_1" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2bj-results" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data-interop" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten_1" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data-interop" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22530,16 +22671,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
@@ -51802,13 +51943,13 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="63" t="s">
         <v>202</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
       <c r="F3" s="2" t="s">
         <v>152</v>
       </c>
@@ -52563,11 +52704,11 @@
       <c r="S14" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="T14" s="51" t="s">
+      <c r="T14" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
+      <c r="U14" s="63"/>
+      <c r="V14" s="63"/>
     </row>
     <row r="15" spans="1:22" ht="30">
       <c r="A15">
@@ -56397,10 +56538,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -56419,7 +56560,7 @@
     <col min="14" max="14" width="22.83203125" customWidth="1"/>
     <col min="15" max="15" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="20" customWidth="1"/>
+    <col min="17" max="17" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -56453,6 +56594,9 @@
       <c r="J1" t="s">
         <v>25</v>
       </c>
+      <c r="K1" t="s">
+        <v>118</v>
+      </c>
       <c r="N1" s="6" t="s">
         <v>9</v>
       </c>
@@ -56501,7 +56645,7 @@
         <v>241</v>
       </c>
       <c r="Q2" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -56539,16 +56683,16 @@
         <v>209</v>
       </c>
       <c r="N3" s="7">
-        <v>2816.9436033755601</v>
+        <v>4213.3201519145878</v>
       </c>
       <c r="O3" s="7">
-        <v>5127.0698467406655</v>
+        <v>7103.5192056943743</v>
       </c>
       <c r="P3" s="7">
-        <v>5608.1871896515549</v>
+        <v>7781.5717411190963</v>
       </c>
       <c r="Q3" s="7">
-        <v>5608.1871896515549</v>
+        <v>11737.629932731457</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -56642,7 +56786,7 @@
         <v>1409.4327398100197</v>
       </c>
       <c r="Q5" s="7">
-        <v>1409.4327398100197</v>
+        <v>1391.2524913694263</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -56689,7 +56833,7 @@
         <v>1702.0734024837227</v>
       </c>
       <c r="Q6" s="7">
-        <v>1702.0734024837227</v>
+        <v>1684.9431382495509</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -56736,7 +56880,7 @@
         <v>1409.7868230588144</v>
       </c>
       <c r="Q7" s="7">
-        <v>1409.7868230588144</v>
+        <v>1407.2262046804303</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -56783,7 +56927,7 @@
         <v>905.46192606435238</v>
       </c>
       <c r="Q8" s="7">
-        <v>905.46192606435238</v>
+        <v>760.91632799463173</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -56830,7 +56974,7 @@
         <v>655.47536490629079</v>
       </c>
       <c r="Q9" s="7">
-        <v>655.47536490629079</v>
+        <v>568.90701584762792</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -56868,16 +57012,16 @@
         <v>128</v>
       </c>
       <c r="N10" s="7">
-        <v>22768.135295200002</v>
+        <v>23963.5518376</v>
       </c>
       <c r="O10" s="7">
-        <v>37332.644954199997</v>
-      </c>
-      <c r="P10" s="7" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q10" s="7" t="e">
-        <v>#DIV/0!</v>
+        <v>37041.452272099996</v>
+      </c>
+      <c r="P10" s="7">
+        <v>1690.5742869471997</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>411.80864029044022</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -56915,16 +57059,16 @@
         <v>225</v>
       </c>
       <c r="N11" s="7">
-        <v>22527.895972999999</v>
+        <v>7512.7633737037795</v>
       </c>
       <c r="O11" s="7">
-        <v>47417.862745999999</v>
-      </c>
-      <c r="P11" s="7" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" s="7" t="e">
-        <v>#DIV/0!</v>
+        <v>27702.241021633334</v>
+      </c>
+      <c r="P11" s="7">
+        <v>13003.486282235632</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>17666.539438637141</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -56962,16 +57106,16 @@
         <v>128</v>
       </c>
       <c r="N12" s="7">
-        <v>22527.895972999999</v>
+        <v>7512.7633737037795</v>
       </c>
       <c r="O12" s="7">
-        <v>47417.862745999999</v>
-      </c>
-      <c r="P12" s="7" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" s="7" t="e">
-        <v>#DIV/0!</v>
+        <v>27702.241021633334</v>
+      </c>
+      <c r="P12" s="7">
+        <v>13003.486282235632</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>17666.539438637141</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -57018,7 +57162,7 @@
         <v>835.04325782913259</v>
       </c>
       <c r="Q13" s="7">
-        <v>835.04325782913259</v>
+        <v>964.81053255030292</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -57065,7 +57209,7 @@
         <v>111.92309133969361</v>
       </c>
       <c r="Q14" s="7">
-        <v>111.92309133969361</v>
+        <v>111.54666378357351</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -57112,7 +57256,7 @@
         <v>105.58209255030104</v>
       </c>
       <c r="Q15" s="7">
-        <v>105.58209255030104</v>
+        <v>111.60380077207761</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -57159,39 +57303,39 @@
         <v>934.53259658128707</v>
       </c>
       <c r="Q16" s="7">
-        <v>934.53259658128707</v>
+        <v>867.62424098636143</v>
       </c>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17">
+      <c r="A17" s="13">
         <v>0</v>
       </c>
-      <c r="B17" t="s">
-        <v>224</v>
-      </c>
-      <c r="C17">
-        <v>128</v>
-      </c>
-      <c r="D17">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>128</v>
-      </c>
-      <c r="F17">
-        <v>22527.895972999999</v>
-      </c>
-      <c r="G17">
-        <v>47417.862745999999</v>
-      </c>
-      <c r="H17">
-        <v>47419.311981899999</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="B17" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C17" s="13">
+        <v>128</v>
+      </c>
+      <c r="D17" s="13">
+        <v>16</v>
+      </c>
+      <c r="E17" s="13">
+        <v>128</v>
+      </c>
+      <c r="F17" s="13">
+        <v>25158.968379999998</v>
+      </c>
+      <c r="G17" s="13">
+        <v>36750.259590000001</v>
+      </c>
+      <c r="H17" s="13">
+        <v>36750.694069999998</v>
+      </c>
+      <c r="I17" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="J17" t="s">
-        <v>225</v>
+      <c r="J17" s="13" t="s">
+        <v>209</v>
       </c>
       <c r="M17" s="9">
         <v>16</v>
@@ -57206,7 +57350,7 @@
         <v>1606.2643845303401</v>
       </c>
       <c r="Q17" s="7">
-        <v>1606.2643845303401</v>
+        <v>1609.9533356902239</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -57214,31 +57358,31 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>226</v>
+        <v>271</v>
       </c>
       <c r="C18">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D18">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="F18">
-        <v>300.654438019</v>
+        <v>2217.9745159099998</v>
       </c>
       <c r="G18">
-        <v>934.00202012099999</v>
+        <v>13175.735358</v>
       </c>
       <c r="H18">
-        <v>935.09974002800004</v>
+        <v>13178.010752</v>
       </c>
       <c r="I18" t="s">
         <v>208</v>
       </c>
       <c r="J18" t="s">
-        <v>227</v>
+        <v>272</v>
       </c>
       <c r="M18" s="9">
         <v>32</v>
@@ -57253,126 +57397,156 @@
         <v>246.47106588965303</v>
       </c>
       <c r="Q18" s="7">
-        <v>246.47106588965303</v>
+        <v>363.91520409152037</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C19">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D19">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="F19">
-        <v>113.3769629</v>
+        <v>22527.895972999999</v>
       </c>
       <c r="G19">
-        <v>756.88640379900005</v>
+        <v>47417.862745999999</v>
       </c>
       <c r="H19">
-        <v>758.091012955</v>
+        <v>47419.311981899999</v>
       </c>
       <c r="I19" t="s">
         <v>208</v>
       </c>
       <c r="J19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>8</v>
+        <v>272</v>
       </c>
       <c r="N19" s="7">
-        <v>2382.7539552793528</v>
+        <v>2217.9745159099998</v>
       </c>
       <c r="O19" s="7">
-        <v>4832.0540184732326</v>
-      </c>
-      <c r="P19" s="7">
-        <v>5598.0436865117208</v>
-      </c>
-      <c r="Q19" s="7">
-        <v>5598.0436865117208</v>
+        <v>13175.735358</v>
+      </c>
+      <c r="P19" s="7" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q19" s="7" t="e">
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>229</v>
+        <v>267</v>
       </c>
       <c r="C20">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D20">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="F20">
-        <v>100.828622103</v>
+        <v>5.7084000110600002</v>
       </c>
       <c r="G20">
-        <v>727.96860408800001</v>
+        <v>22380.652238800001</v>
       </c>
       <c r="H20">
-        <v>729.173197985</v>
+        <v>22382.094851999998</v>
       </c>
       <c r="I20" t="s">
         <v>208</v>
       </c>
       <c r="J20" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+      <c r="M20" s="9">
+        <v>128</v>
+      </c>
+      <c r="N20" s="7">
+        <v>2217.9745159099998</v>
+      </c>
+      <c r="O20" s="7">
+        <v>13175.735358</v>
+      </c>
+      <c r="P20" s="7" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q20" s="7" t="e">
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>230</v>
+        <v>268</v>
       </c>
       <c r="C21">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D21">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="F21">
-        <v>252.339545012</v>
+        <v>4.6857481002799997</v>
       </c>
       <c r="G21">
-        <v>927.508314133</v>
+        <v>13308.208080099999</v>
       </c>
       <c r="H21">
-        <v>928.868350029</v>
+        <v>13309.640333200001</v>
       </c>
       <c r="I21" t="s">
         <v>208</v>
       </c>
       <c r="J21" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N21" s="7">
+        <v>2907.9398736000571</v>
+      </c>
+      <c r="O21" s="7">
+        <v>6781.6610535616774</v>
+      </c>
+      <c r="P21" s="7">
+        <v>6581.6905391689634</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>11616.116007390918</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C22">
         <v>12</v>
@@ -57381,16 +57555,16 @@
         <v>12</v>
       </c>
       <c r="E22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F22">
-        <v>220.36070990600001</v>
+        <v>300.654438019</v>
       </c>
       <c r="G22">
-        <v>912.68654990200002</v>
+        <v>934.00202012099999</v>
       </c>
       <c r="H22">
-        <v>913.90338492399997</v>
+        <v>935.09974002800004</v>
       </c>
       <c r="I22" t="s">
         <v>208</v>
@@ -57401,10 +57575,10 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C23">
         <v>12</v>
@@ -57413,16 +57587,16 @@
         <v>12</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F23">
-        <v>55.585777044300002</v>
+        <v>113.3769629</v>
       </c>
       <c r="G23">
-        <v>727.22062802300002</v>
+        <v>756.88640379900005</v>
       </c>
       <c r="H23">
-        <v>728.41032099699999</v>
+        <v>758.091012955</v>
       </c>
       <c r="I23" t="s">
         <v>208</v>
@@ -57433,10 +57607,10 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C24">
         <v>12</v>
@@ -57445,16 +57619,16 @@
         <v>12</v>
       </c>
       <c r="E24">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F24">
-        <v>1703.66234207</v>
+        <v>100.828622103</v>
       </c>
       <c r="G24">
-        <v>2510.5651390600001</v>
+        <v>727.96860408800001</v>
       </c>
       <c r="H24">
-        <v>2511.7870490599998</v>
+        <v>729.173197985</v>
       </c>
       <c r="I24" t="s">
         <v>208</v>
@@ -57465,10 +57639,10 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C25">
         <v>12</v>
@@ -57477,16 +57651,16 @@
         <v>12</v>
       </c>
       <c r="E25">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>90.235594987900001</v>
+        <v>252.339545012</v>
       </c>
       <c r="G25">
-        <v>1207.55374312</v>
+        <v>927.508314133</v>
       </c>
       <c r="H25">
-        <v>1208.7523281599999</v>
+        <v>928.868350029</v>
       </c>
       <c r="I25" t="s">
         <v>208</v>
@@ -57497,10 +57671,10 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C26">
         <v>12</v>
@@ -57509,16 +57683,16 @@
         <v>12</v>
       </c>
       <c r="E26">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F26">
-        <v>79.823445081700001</v>
+        <v>220.36070990600001</v>
       </c>
       <c r="G26">
-        <v>866.61979699100004</v>
+        <v>912.68654990200002</v>
       </c>
       <c r="H26">
-        <v>867.81867504100001</v>
+        <v>913.90338492399997</v>
       </c>
       <c r="I26" t="s">
         <v>208</v>
@@ -57529,28 +57703,28 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C27">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D27">
         <v>12</v>
       </c>
       <c r="E27">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F27">
-        <v>263.91831493400002</v>
+        <v>55.585777044300002</v>
       </c>
       <c r="G27">
-        <v>1318.27436304</v>
+        <v>727.22062802300002</v>
       </c>
       <c r="H27">
-        <v>1319.4774529900001</v>
+        <v>728.41032099699999</v>
       </c>
       <c r="I27" t="s">
         <v>208</v>
@@ -57561,28 +57735,28 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C28">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D28">
         <v>12</v>
       </c>
       <c r="E28">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F28">
-        <v>141.600160837</v>
+        <v>1703.66234207</v>
       </c>
       <c r="G28">
-        <v>1207.09737587</v>
+        <v>2510.5651390600001</v>
       </c>
       <c r="H28">
-        <v>1208.20039296</v>
+        <v>2511.7870490599998</v>
       </c>
       <c r="I28" t="s">
         <v>208</v>
@@ -57593,28 +57767,28 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C29">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D29">
         <v>12</v>
       </c>
       <c r="E29">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F29">
-        <v>2982.8733580100002</v>
+        <v>90.235594987900001</v>
       </c>
       <c r="G29">
-        <v>4049.5441341400001</v>
+        <v>1207.55374312</v>
       </c>
       <c r="H29">
-        <v>4050.7455921199999</v>
+        <v>1208.7523281599999</v>
       </c>
       <c r="I29" t="s">
         <v>208</v>
@@ -57625,28 +57799,28 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C30">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D30">
         <v>12</v>
       </c>
       <c r="E30">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F30">
-        <v>23.373319864300001</v>
+        <v>79.823445081700001</v>
       </c>
       <c r="G30">
-        <v>2503.21842599</v>
+        <v>866.61979699100004</v>
       </c>
       <c r="H30">
-        <v>2504.4764480600002</v>
+        <v>867.81867504100001</v>
       </c>
       <c r="I30" t="s">
         <v>208</v>
@@ -57657,28 +57831,28 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C31">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D31">
         <v>12</v>
       </c>
       <c r="E31">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F31">
-        <v>371.93604397799999</v>
+        <v>263.91831493400002</v>
       </c>
       <c r="G31">
-        <v>1988.56460881</v>
+        <v>1318.27436304</v>
       </c>
       <c r="H31">
-        <v>1989.9456028899999</v>
+        <v>1319.4774529900001</v>
       </c>
       <c r="I31" t="s">
         <v>208</v>
@@ -57687,8 +57861,137 @@
         <v>227</v>
       </c>
     </row>
+    <row r="32" spans="1:17">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>237</v>
+      </c>
+      <c r="C32">
+        <v>24</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>141.600160837</v>
+      </c>
+      <c r="G32">
+        <v>1207.09737587</v>
+      </c>
+      <c r="H32">
+        <v>1208.20039296</v>
+      </c>
+      <c r="I32" t="s">
+        <v>208</v>
+      </c>
+      <c r="J32" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>238</v>
+      </c>
+      <c r="C33">
+        <v>24</v>
+      </c>
+      <c r="D33">
+        <v>12</v>
+      </c>
+      <c r="E33">
+        <v>16</v>
+      </c>
+      <c r="F33">
+        <v>2982.8733580100002</v>
+      </c>
+      <c r="G33">
+        <v>4049.5441341400001</v>
+      </c>
+      <c r="H33">
+        <v>4050.7455921199999</v>
+      </c>
+      <c r="I33" t="s">
+        <v>208</v>
+      </c>
+      <c r="J33" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>239</v>
+      </c>
+      <c r="C34">
+        <v>36</v>
+      </c>
+      <c r="D34">
+        <v>12</v>
+      </c>
+      <c r="E34">
+        <v>32</v>
+      </c>
+      <c r="F34">
+        <v>23.373319864300001</v>
+      </c>
+      <c r="G34">
+        <v>2503.21842599</v>
+      </c>
+      <c r="H34">
+        <v>2504.4764480600002</v>
+      </c>
+      <c r="I34" t="s">
+        <v>208</v>
+      </c>
+      <c r="J34" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>240</v>
+      </c>
+      <c r="C35">
+        <v>36</v>
+      </c>
+      <c r="D35">
+        <v>12</v>
+      </c>
+      <c r="E35">
+        <v>32</v>
+      </c>
+      <c r="F35">
+        <v>371.93604397799999</v>
+      </c>
+      <c r="G35">
+        <v>1988.56460881</v>
+      </c>
+      <c r="H35">
+        <v>1989.9456028899999</v>
+      </c>
+      <c r="I35" t="s">
+        <v>208</v>
+      </c>
+      <c r="J35" t="s">
+        <v>227</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -57702,7 +58005,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -58029,11 +58332,11 @@
       <c r="M8" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="N8" s="59">
+      <c r="N8" s="54">
         <f>AVERAGE(N4:N6)</f>
         <v>330.21324467653335</v>
       </c>
-      <c r="O8" s="59">
+      <c r="O8" s="54">
         <f>AVERAGE(O4:O6)</f>
         <v>8733.732693349999</v>
       </c>
@@ -58258,11 +58561,11 @@
       </c>
     </row>
     <row r="21" spans="13:15" ht="16" thickBot="1">
-      <c r="M21" s="60"/>
-      <c r="N21" s="61">
+      <c r="M21" s="55"/>
+      <c r="N21" s="56">
         <v>6234.875</v>
       </c>
-      <c r="O21" s="61">
+      <c r="O21" s="56">
         <v>1280.515625</v>
       </c>
     </row>
@@ -58270,11 +58573,11 @@
       <c r="M22" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="N22" s="59">
+      <c r="N22" s="54">
         <f>AVERAGE(N16:N21)</f>
         <v>6929.617033333333</v>
       </c>
-      <c r="O22" s="59">
+      <c r="O22" s="54">
         <f>AVERAGE(O16:O21)</f>
         <v>1152.9166666666667</v>
       </c>
@@ -58283,11 +58586,11 @@
       <c r="M23" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N23" s="59">
+      <c r="N23" s="54">
         <f>STDEV(N16:N21)</f>
         <v>1220.3487605097328</v>
       </c>
-      <c r="O23" s="59">
+      <c r="O23" s="54">
         <f>STDEV(O16:O21)</f>
         <v>140.23939620769141</v>
       </c>
@@ -58857,10 +59160,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -58879,11 +59182,16 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2"/>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="51" t="s">
         <v>245</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="F3" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -58932,11 +59240,11 @@
       </c>
       <c r="F5" s="20">
         <f>'BJ w Staging'!N10</f>
-        <v>22768.135295200002</v>
+        <v>23963.5518376</v>
       </c>
       <c r="G5" s="35">
         <f>'BJ w Staging'!N12</f>
-        <v>22527.895972999999</v>
+        <v>7512.7633737037795</v>
       </c>
       <c r="H5" s="20">
         <f>'BJ (FG multi)'!N8</f>
@@ -58961,14 +59269,13 @@
         <f>Condor!C9</f>
         <v>5736.0000000000027</v>
       </c>
-      <c r="F6" s="52">
-        <f>13466.8854166667</f>
-        <v>13466.885416666701</v>
-      </c>
-      <c r="G6" s="55">
-        <v>14727</v>
-      </c>
-      <c r="H6" s="62">
+      <c r="F6" s="47">
+        <v>11460.578475336322</v>
+      </c>
+      <c r="G6" s="50">
+        <v>19192</v>
+      </c>
+      <c r="H6" s="57">
         <f>'BJ (FG multi)'!N22</f>
         <v>6929.617033333333</v>
       </c>
@@ -58994,12 +59301,12 @@
         <v>909.33333333333405</v>
       </c>
       <c r="F7" s="21">
-        <v>911</v>
-      </c>
-      <c r="G7" s="57">
+        <v>906</v>
+      </c>
+      <c r="G7" s="52">
         <v>1069</v>
       </c>
-      <c r="H7" s="63">
+      <c r="H7" s="58">
         <f>'BJ (FG multi)'!O22</f>
         <v>1152.9166666666667</v>
       </c>
@@ -59026,11 +59333,11 @@
       </c>
       <c r="F8" s="21">
         <f>'BJ w Staging'!O10</f>
-        <v>37332.644954199997</v>
+        <v>37041.452272099996</v>
       </c>
       <c r="G8" s="37">
         <f>'BJ w Staging'!O12</f>
-        <v>47417.862745999999</v>
+        <v>27702.241021633334</v>
       </c>
       <c r="H8" s="21">
         <f>'BJ (FG multi)'!O8</f>
@@ -59058,10 +59365,11 @@
         <v>3383.1243449411259</v>
       </c>
       <c r="F9" s="21">
-        <v>0</v>
+        <v>2102.3829270000001</v>
       </c>
       <c r="G9" s="37">
-        <v>0</v>
+        <f>'BJ w Staging'!Q12</f>
+        <v>17666.539438637141</v>
       </c>
       <c r="H9" s="21">
         <f>'BJ (FG multi)'!O9</f>
@@ -59111,11 +59419,11 @@
       </c>
       <c r="F12" s="21">
         <f t="shared" ref="F12:G12" si="1">F5/60</f>
-        <v>379.46892158666668</v>
+        <v>399.39253062666666</v>
       </c>
       <c r="G12" s="37">
         <f t="shared" si="1"/>
-        <v>375.46493288333329</v>
+        <v>125.212722895063</v>
       </c>
       <c r="H12" s="37">
         <f t="shared" ref="H12" si="2">H5/60</f>
@@ -59123,7 +59431,7 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="48" t="s">
         <v>132</v>
       </c>
       <c r="B13" s="21">
@@ -59144,11 +59452,11 @@
       </c>
       <c r="F13" s="30">
         <f t="shared" ref="F13:G13" si="3">F6/60</f>
-        <v>224.44809027777833</v>
+        <v>191.00964125560537</v>
       </c>
       <c r="G13" s="36">
         <f t="shared" si="3"/>
-        <v>245.45</v>
+        <v>319.86666666666667</v>
       </c>
       <c r="H13" s="36">
         <f t="shared" ref="H13" si="4">H6/60</f>
@@ -59160,28 +59468,28 @@
         <v>190</v>
       </c>
       <c r="B14" s="21">
-        <f>B18-B16-B12-B13</f>
+        <f>B19-B16-B12-B13</f>
         <v>4.0070597973667077</v>
       </c>
       <c r="C14" s="16">
-        <f>C18-C16-C12-C13</f>
+        <f>C19-C16-C12-C13</f>
         <v>8.7646148900333287</v>
       </c>
       <c r="D14" s="37">
-        <f>D18-D16-D12-D13</f>
+        <f>D19-D16-D12-D13</f>
         <v>-4.333315928306547E-9</v>
       </c>
       <c r="E14" s="21">
-        <f>E18-E16-E12-E13</f>
+        <f>E19-E16-E12-E13</f>
         <v>-5.5555555555599767E-3</v>
       </c>
       <c r="F14" s="21">
-        <f>F18-F16-F12-F13</f>
-        <v>3.1104040388883334</v>
+        <f>F19-F16-F12-F13</f>
+        <v>11.855365986061173</v>
       </c>
       <c r="G14" s="37">
-        <f t="shared" ref="F14:H14" si="5">G18-G16-G12-G13</f>
-        <v>151.56611288333335</v>
+        <f t="shared" ref="G14:H14" si="5">G19-G16-G12-G13</f>
+        <v>-1.1920392011741114</v>
       </c>
       <c r="H14" s="37">
         <f t="shared" si="5"/>
@@ -59210,11 +59518,11 @@
       </c>
       <c r="F15" s="21">
         <f t="shared" ref="F15:H15" si="6">F12+F14</f>
-        <v>382.57932562555504</v>
+        <v>411.2478966127278</v>
       </c>
       <c r="G15" s="37">
         <f t="shared" si="6"/>
-        <v>527.03104576666669</v>
+        <v>124.02068369388888</v>
       </c>
       <c r="H15" s="37">
         <f t="shared" si="6"/>
@@ -59243,7 +59551,7 @@
       </c>
       <c r="F16" s="21">
         <f t="shared" ref="F16:G16" si="7">F7/60</f>
-        <v>15.183333333333334</v>
+        <v>15.1</v>
       </c>
       <c r="G16" s="37">
         <f t="shared" si="7"/>
@@ -59259,11 +59567,11 @@
         <v>244</v>
       </c>
       <c r="B17" s="21">
-        <f>B18-B12-B13</f>
+        <f>B19-B12-B13</f>
         <v>35.614872297366674</v>
       </c>
       <c r="C17" s="21">
-        <f t="shared" ref="C17:H17" si="9">C18-C12-C13</f>
+        <f t="shared" ref="C17:H17" si="9">C19-C12-C13</f>
         <v>26.579458640033334</v>
       </c>
       <c r="D17" s="21">
@@ -59275,12 +59583,12 @@
         <v>15.150000000000006</v>
       </c>
       <c r="F17" s="21">
-        <f>F18-F12-F13</f>
-        <v>18.293737372221614</v>
+        <f>F19-F12-F13</f>
+        <v>26.955365986061196</v>
       </c>
       <c r="G17" s="37">
         <f t="shared" si="9"/>
-        <v>169.38277955000007</v>
+        <v>16.624627465492551</v>
       </c>
       <c r="H17" s="37">
         <f t="shared" si="9"/>
@@ -59288,199 +59596,208 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>130</v>
+      <c r="A18" s="2" t="s">
+        <v>274</v>
       </c>
       <c r="B18" s="21">
-        <f>B8/60</f>
-        <v>36.901069556666677</v>
-      </c>
-      <c r="C18" s="16">
-        <f>C8/60</f>
-        <v>28.264309130000001</v>
-      </c>
-      <c r="D18" s="37">
-        <f>D8/60</f>
-        <v>144.74436088066668</v>
+        <f>B17-B16</f>
+        <v>4.0070597973667041</v>
+      </c>
+      <c r="C18" s="21">
+        <f t="shared" ref="C18:H18" si="10">C17-C16</f>
+        <v>8.7646148900333287</v>
+      </c>
+      <c r="D18" s="21">
+        <f t="shared" si="10"/>
+        <v>-4.333315928306547E-9</v>
       </c>
       <c r="E18" s="21">
-        <f>E8/60</f>
-        <v>122.62222222222228</v>
+        <f t="shared" si="10"/>
+        <v>-5.5555555555617531E-3</v>
       </c>
       <c r="F18" s="21">
-        <f>F8/60</f>
-        <v>622.21074923666663</v>
-      </c>
-      <c r="G18" s="37">
-        <f>G8/60</f>
-        <v>790.29771243333334</v>
-      </c>
-      <c r="H18" s="37">
-        <f>H8/60</f>
-        <v>145.56221155583333</v>
+        <f t="shared" si="10"/>
+        <v>11.855365986061196</v>
+      </c>
+      <c r="G18" s="21">
+        <f t="shared" si="10"/>
+        <v>-1.192039201174115</v>
+      </c>
+      <c r="H18" s="21">
+        <f t="shared" si="10"/>
+        <v>5.3497624778911117</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="21">
+        <f t="shared" ref="B19:H19" si="11">B8/60</f>
+        <v>36.901069556666677</v>
+      </c>
+      <c r="C19" s="16">
+        <f t="shared" si="11"/>
+        <v>28.264309130000001</v>
+      </c>
+      <c r="D19" s="37">
+        <f t="shared" si="11"/>
+        <v>144.74436088066668</v>
+      </c>
+      <c r="E19" s="21">
+        <f t="shared" si="11"/>
+        <v>122.62222222222228</v>
+      </c>
+      <c r="F19" s="21">
+        <f t="shared" si="11"/>
+        <v>617.35753786833322</v>
+      </c>
+      <c r="G19" s="37">
+        <f t="shared" si="11"/>
+        <v>461.70401702722222</v>
+      </c>
+      <c r="H19" s="37">
+        <f t="shared" si="11"/>
+        <v>145.56221155583333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
         <v>138</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B20" s="21">
         <f>B9/60</f>
         <v>1.1073060889029485</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C20" s="23">
         <f>C9/60</f>
         <v>4.4594062210782148</v>
       </c>
-      <c r="D19" s="37">
+      <c r="D20" s="37">
         <f>D9/60</f>
         <v>23.078721136591266</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E20" s="21">
         <f>E9/60</f>
         <v>56.385405749018766</v>
       </c>
-      <c r="F19" s="21">
-        <f t="shared" ref="F19:G19" si="10">F9/60</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="37">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="37">
-        <f t="shared" ref="H19" si="11">H9/60</f>
+      <c r="F20" s="21">
+        <f t="shared" ref="F20:G20" si="12">F9/60</f>
+        <v>35.039715450000003</v>
+      </c>
+      <c r="G20" s="37">
+        <f t="shared" si="12"/>
+        <v>294.4423239772857</v>
+      </c>
+      <c r="H20" s="37">
+        <f t="shared" ref="H20" si="13">H9/60</f>
         <v>20.849802584910968</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
         <v>194</v>
       </c>
-      <c r="B20" s="37">
+      <c r="B21" s="37">
         <f>B15+B16</f>
         <v>36.901069556666677</v>
       </c>
-      <c r="C20" s="37">
-        <f t="shared" ref="C20:E20" si="12">C15+C16</f>
+      <c r="C21" s="37">
+        <f t="shared" ref="C21:E21" si="14">C15+C16</f>
         <v>28.264309130000001</v>
       </c>
-      <c r="D20" s="37">
-        <f t="shared" si="12"/>
+      <c r="D21" s="37">
+        <f t="shared" si="14"/>
         <v>66.280183530666676</v>
       </c>
-      <c r="E20" s="37">
-        <f t="shared" si="12"/>
+      <c r="E21" s="37">
+        <f t="shared" si="14"/>
         <v>27.022222222222226</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F21" s="37">
         <f>F15+F16</f>
-        <v>397.76265895888838</v>
-      </c>
-      <c r="G20" s="37">
+        <v>426.34789661272782</v>
+      </c>
+      <c r="G21" s="37">
         <f>G15+G16</f>
-        <v>544.84771243333341</v>
-      </c>
-      <c r="H20" s="37">
+        <v>141.83735036055555</v>
+      </c>
+      <c r="H21" s="37">
         <f>H15+H16</f>
         <v>30.06859433361112</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B21" s="37">
-        <f>B18-B12</f>
+      <c r="B22" s="37">
+        <f>B19-B12</f>
         <v>35.614872297366674</v>
       </c>
-      <c r="C21" s="37">
-        <f t="shared" ref="C21:G21" si="13">C18-C12</f>
+      <c r="C22" s="37">
+        <f t="shared" ref="C22:G22" si="15">C19-C12</f>
         <v>26.579458640033334</v>
       </c>
-      <c r="D21" s="37">
-        <f t="shared" si="13"/>
+      <c r="D22" s="37">
+        <f t="shared" si="15"/>
         <v>91.95416284733335</v>
       </c>
-      <c r="E21" s="37">
-        <f t="shared" si="13"/>
+      <c r="E22" s="37">
+        <f t="shared" si="15"/>
         <v>110.75000000000006</v>
       </c>
-      <c r="F21" s="37">
-        <f t="shared" si="13"/>
-        <v>242.74182764999995</v>
-      </c>
-      <c r="G21" s="37">
-        <f t="shared" si="13"/>
-        <v>414.83277955000005</v>
-      </c>
-      <c r="H21" s="37">
-        <f t="shared" ref="H21" si="14">H18-H12</f>
+      <c r="F22" s="37">
+        <f t="shared" si="15"/>
+        <v>217.96500724166657</v>
+      </c>
+      <c r="G22" s="37">
+        <f t="shared" si="15"/>
+        <v>336.49129413215923</v>
+      </c>
+      <c r="H22" s="37">
+        <f t="shared" ref="H22" si="16">H19-H12</f>
         <v>140.0586574778911</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="54"/>
-    </row>
-    <row r="23" spans="1:8" ht="16" thickBot="1">
-      <c r="A23" s="27"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="29"/>
-    </row>
-    <row r="24" spans="1:8" ht="16" thickTop="1">
-      <c r="A24" t="s">
+    <row r="23" spans="1:8">
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="49"/>
+    </row>
+    <row r="24" spans="1:8" ht="16" thickBot="1">
+      <c r="A24" s="27"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="29"/>
+    </row>
+    <row r="25" spans="1:8" ht="16" thickTop="1">
+      <c r="A25" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B25" s="3">
         <f>B8/$C$8</f>
         <v>1.3055712554990258</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C25" s="28">
         <f>C8/$C$8</f>
         <v>1</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D25" s="10">
         <f>D8/$C$8</f>
         <v>5.1211002616382251</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E25" s="28">
         <f>E8/$C$8</f>
         <v>4.3384121528755113</v>
-      </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="28"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>193</v>
-      </c>
-      <c r="B25" s="3">
-        <f>B7/$D$7</f>
-        <v>2.3430575589643796</v>
-      </c>
-      <c r="C25" s="28">
-        <f>C7/$D$7</f>
-        <v>1.3205976943265809</v>
-      </c>
-      <c r="D25" s="10">
-        <f>D7/$D$7</f>
-        <v>1</v>
-      </c>
-      <c r="E25" s="28">
-        <f>E7/$D$7</f>
-        <v>1.1234671492925714</v>
       </c>
       <c r="F25" s="28"/>
       <c r="G25" s="3"/>
@@ -59488,49 +59805,106 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>195</v>
-      </c>
-      <c r="B26" s="28">
-        <f>B20/$C$20</f>
-        <v>1.3055712554990258</v>
+        <v>193</v>
+      </c>
+      <c r="B26" s="3">
+        <f>B7/$D$7</f>
+        <v>2.3430575589643796</v>
       </c>
       <c r="C26" s="28">
-        <f>C20/$C$20</f>
+        <f>C7/$D$7</f>
+        <v>1.3205976943265809</v>
+      </c>
+      <c r="D26" s="10">
+        <f>D7/$D$7</f>
         <v>1</v>
       </c>
-      <c r="D26" s="28">
-        <f t="shared" ref="D26:E26" si="15">D20/$C$20</f>
-        <v>2.3450133957216126</v>
-      </c>
       <c r="E26" s="28">
-        <f t="shared" si="15"/>
-        <v>0.95605458098887641</v>
+        <f>E7/$D$7</f>
+        <v>1.1234671492925714</v>
       </c>
       <c r="F26" s="28"/>
       <c r="G26" s="3"/>
       <c r="H26" s="28"/>
     </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>195</v>
+      </c>
+      <c r="B27" s="28">
+        <f>B21/$C$21</f>
+        <v>1.3055712554990258</v>
+      </c>
+      <c r="C27" s="28">
+        <f>C21/$C$21</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="28">
+        <f t="shared" ref="D27:E27" si="17">D21/$C$21</f>
+        <v>2.3450133957216126</v>
+      </c>
+      <c r="E27" s="28">
+        <f t="shared" si="17"/>
+        <v>0.95605458098887641</v>
+      </c>
+      <c r="F27" s="28"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="28"/>
+    </row>
     <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>269</v>
+      </c>
+      <c r="B28">
+        <f>B14/B19</f>
+        <v>0.10858925894311316</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:H28" si="18">C14/C19</f>
+        <v>0.31009478596207701</v>
+      </c>
       <c r="D28">
-        <f>D20/B20</f>
+        <f t="shared" si="18"/>
+        <v>-2.9937718484792058E-11</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="18"/>
+        <v>-4.5306270387857709E-5</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="18"/>
+        <v>1.9203403633810692E-2</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="18"/>
+        <v>-2.581825492551061E-3</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="18"/>
+        <v>3.6752412736179879E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="D29">
+        <f>D21/B21</f>
         <v>1.7961588736305956</v>
       </c>
     </row>
-    <row r="40" spans="2:11">
-      <c r="B40">
+    <row r="41" spans="2:11">
+      <c r="B41">
         <f>36/34</f>
         <v>1.0588235294117647</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <f>28/34</f>
         <v>0.82352941176470584</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="K41" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="11:11">
-      <c r="K74" s="2" t="s">
+    <row r="75" spans="11:11">
+      <c r="K75" s="2" t="s">
         <v>243</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added Pradeep's FG/XSEDE data
git-svn-id: file://localhost/tmp/svn2git/svn@7188 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15160" yWindow="0" windowWidth="29160" windowHeight="28360" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="2160" yWindow="0" windowWidth="41800" windowHeight="28260" tabRatio="500" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -15,30 +15,33 @@
     <sheet name="Condor" sheetId="11" r:id="rId6"/>
     <sheet name="Total" sheetId="12" r:id="rId7"/>
     <sheet name="Raw (BJ)" sheetId="8" r:id="rId8"/>
-    <sheet name="Interop EGI-FG" sheetId="15" r:id="rId9"/>
-    <sheet name="Interop OSG-XSEDE" sheetId="16" r:id="rId10"/>
-    <sheet name="Interop " sheetId="14" r:id="rId11"/>
+    <sheet name="BJ (FG-XSEDE)" sheetId="19" r:id="rId9"/>
+    <sheet name="Interop EGI-FG" sheetId="15" r:id="rId10"/>
+    <sheet name="Interop OSG-XSEDE" sheetId="16" r:id="rId11"/>
+    <sheet name="Interop " sheetId="14" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="_1bj_results" localSheetId="2">'BJ w Staging'!$A$20:$J$21</definedName>
     <definedName name="_2bj_results" localSheetId="3">'BJ (FG multi)'!$A$1:$J$13</definedName>
+    <definedName name="bj_multi_fg_xsede" localSheetId="8">'BJ (FG-XSEDE)'!$A$1:$J$7</definedName>
     <definedName name="bj_singleresource" localSheetId="2">'BJ w Staging'!$A$1:$J$35</definedName>
-    <definedName name="data_interop" localSheetId="10">'Interop '!$A$1:$J$32</definedName>
+    <definedName name="data_interop" localSheetId="11">'Interop '!$A$1:$J$32</definedName>
     <definedName name="daten" localSheetId="1">BigJob!$A$1:$J$64</definedName>
     <definedName name="daten_1" localSheetId="7">'Raw (BJ)'!$A$1:$J$109</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId13"/>
-    <pivotCache cacheId="22" r:id="rId14"/>
-    <pivotCache cacheId="23" r:id="rId15"/>
-    <pivotCache cacheId="24" r:id="rId16"/>
-    <pivotCache cacheId="25" r:id="rId17"/>
-    <pivotCache cacheId="26" r:id="rId18"/>
-    <pivotCache cacheId="31" r:id="rId19"/>
+    <pivotCache cacheId="12" r:id="rId14"/>
+    <pivotCache cacheId="13" r:id="rId15"/>
+    <pivotCache cacheId="14" r:id="rId16"/>
+    <pivotCache cacheId="15" r:id="rId17"/>
+    <pivotCache cacheId="16" r:id="rId18"/>
+    <pivotCache cacheId="17" r:id="rId19"/>
+    <pivotCache cacheId="18" r:id="rId20"/>
+    <pivotCache cacheId="21" r:id="rId21"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -82,7 +85,23 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="bj-singleresource.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="bj-multi-fg-xsede.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:Dropbox:SAGA:papers:troy:pstar:perf:sc:bj-multi-fg-xsede.txt" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="bj-singleresource.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:Dropbox:SAGA:papers:troy:pstar:perf:sc:bj-singleresource.txt" comma="1">
       <textFields count="10">
         <textField/>
@@ -98,14 +117,14 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="data-interop.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="5" name="data-interop.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:data-interop.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="daten.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" name="daten.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields count="10">
         <textField/>
@@ -121,21 +140,21 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="daten.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="7" name="daten.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="daten.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="8" name="daten.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="daten.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="9" name="daten.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
@@ -146,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="285">
   <si>
     <t>bfast</t>
   </si>
@@ -889,15 +908,6 @@
     <t>to refine</t>
   </si>
   <si>
-    <t>XSEDE (Trestles)</t>
-  </si>
-  <si>
-    <t>FG (India)</t>
-  </si>
-  <si>
-    <t>FG (India/Sierra)</t>
-  </si>
-  <si>
     <t>bigjob:bj-aff746cc-917b-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org</t>
   </si>
   <si>
@@ -974,6 +984,49 @@
   </si>
   <si>
     <t>Overhead</t>
+  </si>
+  <si>
+    <t>DIANE/EGI</t>
+  </si>
+  <si>
+    <t>BigJob/XSEDE (Trestles)</t>
+  </si>
+  <si>
+    <t>BigJob/FG
+ (India)</t>
+  </si>
+  <si>
+    <t>BigJob/FG 
+(India/Sierra)</t>
+  </si>
+  <si>
+    <t>GlideInWMS/
+OSG</t>
+  </si>
+  <si>
+    <t>XSEDE:Trestles/
+FutureGrid</t>
+  </si>
+  <si>
+    <t>bigjob:bj-fd8126ee-9412-11e1-84cd-bc305b7ee8dc:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-013eccd2-9413-11e1-84cd-bc305b7ee8dc:trestles.sdsc.edu</t>
+  </si>
+  <si>
+    <t>bigjob:bj-13857a0e-9430-11e1-84cd-bc305b7ee8dc:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-158cca78-9430-11e1-84cd-bc305b7ee8dc:trestles.sdsc.edu</t>
+  </si>
+  <si>
+    <t>bigjob:bj-22b92086-9442-11e1-84cd-bc305b7ee8dc:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-24c6f574-9442-11e1-84cd-bc305b7ee8dc:trestles.sdsc.edu</t>
+  </si>
+  <si>
+    <t>STABW - Net Runtime2</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1299,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="139">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1386,8 +1439,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1465,6 +1522,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1480,9 +1538,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="139">
+  <cellStyles count="143">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1552,6 +1615,8 @@
     <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1621,6 +1686,8 @@
     <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
@@ -1822,11 +1889,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2141954728"/>
-        <c:axId val="2141957704"/>
+        <c:axId val="2092735608"/>
+        <c:axId val="2085705288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2141954728"/>
+        <c:axId val="2092735608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,7 +1903,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141957704"/>
+        <c:crossAx val="2085705288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1844,7 +1911,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141957704"/>
+        <c:axId val="2085705288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1855,7 +1922,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141954728"/>
+        <c:crossAx val="2092735608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2153,11 +2220,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2141913640"/>
-        <c:axId val="2141895688"/>
+        <c:axId val="2093737544"/>
+        <c:axId val="2093541960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2141913640"/>
+        <c:axId val="2093737544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,7 +2258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141895688"/>
+        <c:crossAx val="2093541960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2199,7 +2266,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141895688"/>
+        <c:axId val="2093541960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2210,7 +2277,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141913640"/>
+        <c:crossAx val="2093737544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2522,11 +2589,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2142818376"/>
-        <c:axId val="2142824088"/>
+        <c:axId val="2090067192"/>
+        <c:axId val="2090144472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142818376"/>
+        <c:axId val="2090067192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2559,7 +2626,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142824088"/>
+        <c:crossAx val="2090144472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2567,7 +2634,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142824088"/>
+        <c:axId val="2090144472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,7 +2663,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142818376"/>
+        <c:crossAx val="2090067192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2662,10 +2729,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>EGI</c:v>
+                  <c:v>DIANE/EGI</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2719,10 +2786,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>EGI</c:v>
+                  <c:v>DIANE/EGI</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2822,10 +2889,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>EGI</c:v>
+                  <c:v>DIANE/EGI</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2862,11 +2929,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2144770296"/>
-        <c:axId val="2144764920"/>
+        <c:axId val="2091238680"/>
+        <c:axId val="2091241720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144770296"/>
+        <c:axId val="2091238680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2888,7 +2955,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144764920"/>
+        <c:crossAx val="2091241720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2896,7 +2963,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144764920"/>
+        <c:axId val="2091241720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -2953,7 +3020,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144770296"/>
+        <c:crossAx val="2091238680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3043,10 +3110,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>EGI</c:v>
+                  <c:v>DIANE/EGI</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3092,10 +3159,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>EGI</c:v>
+                  <c:v>DIANE/EGI</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3141,10 +3208,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>EGI</c:v>
+                  <c:v>DIANE/EGI</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3181,11 +3248,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2141847192"/>
-        <c:axId val="2141825800"/>
+        <c:axId val="2091788904"/>
+        <c:axId val="2091791944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2141847192"/>
+        <c:axId val="2091788904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3199,7 +3266,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="1">
+              <a:defRPr sz="1600" b="1">
                 <a:latin typeface="Times"/>
                 <a:cs typeface="Times"/>
               </a:defRPr>
@@ -3207,7 +3274,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141825800"/>
+        <c:crossAx val="2091791944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3215,7 +3282,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141825800"/>
+        <c:axId val="2091791944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3264,7 +3331,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141847192"/>
+        <c:crossAx val="2091788904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3344,19 +3411,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>XSEDE (Trestles)</c:v>
+                  <c:v>BigJob/XSEDE (Trestles)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FG (India)</c:v>
+                  <c:v>BigJob/FG_x000d_ (India)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FG (India/Sierra)</c:v>
+                  <c:v>BigJob/FG _x000d_(India/Sierra)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>EGI</c:v>
+                  <c:v>DIANE/EGI</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3459,19 +3526,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>XSEDE (Trestles)</c:v>
+                  <c:v>BigJob/XSEDE (Trestles)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>FG (India)</c:v>
+                  <c:v>BigJob/FG_x000d_ (India)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>FG (India/Sierra)</c:v>
+                  <c:v>BigJob/FG _x000d_(India/Sierra)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>EGI</c:v>
+                  <c:v>DIANE/EGI</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3511,11 +3578,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2142950248"/>
-        <c:axId val="2142953224"/>
+        <c:axId val="2091841048"/>
+        <c:axId val="2091844024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142950248"/>
+        <c:axId val="2091841048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3529,7 +3596,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="1">
+              <a:defRPr sz="1600" b="1">
                 <a:latin typeface="Times"/>
                 <a:cs typeface="Times"/>
               </a:defRPr>
@@ -3537,7 +3604,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142953224"/>
+        <c:crossAx val="2091844024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3545,7 +3612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142953224"/>
+        <c:axId val="2091844024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3590,7 +3657,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142950248"/>
+        <c:crossAx val="2091841048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3924,11 +3991,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2144653800"/>
-        <c:axId val="2144639000"/>
+        <c:axId val="2089940760"/>
+        <c:axId val="2089944024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144653800"/>
+        <c:axId val="2089940760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3950,7 +4017,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144639000"/>
+        <c:crossAx val="2089944024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3958,7 +4025,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144639000"/>
+        <c:axId val="2089944024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4013,7 +4080,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144653800"/>
+        <c:crossAx val="2089940760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4025,6 +4092,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4719,6 +4787,57 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41031.942976967592" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="6">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:K7" sheet="BJ (FG-XSEDE)"/>
+  </cacheSource>
+  <cacheFields count="11">
+    <cacheField name="Run" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2"/>
+    </cacheField>
+    <cacheField name="BJ" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="#Nodes" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="64" maxValue="64"/>
+    </cacheField>
+    <cacheField name="#cores/node" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="8" maxValue="32"/>
+    </cacheField>
+    <cacheField name="#jobs" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="64" maxValue="64"/>
+    </cacheField>
+    <cacheField name="Queuing Time" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="10.5786662102" maxValue="9138.7722568499994"/>
+    </cacheField>
+    <cacheField name="BJ Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="5112.9851040800004" maxValue="12486.001956"/>
+    </cacheField>
+    <cacheField name="Total Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="6558.7503042199996" maxValue="12488.289187"/>
+    </cacheField>
+    <cacheField name="Coordination URL" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="LRMS URL" numFmtId="0">
+      <sharedItems count="2">
+        <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
+        <s v="pbs-ssh://pmantha@trestles.sdsc.edu"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Net Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3347.2296991500007" maxValue="7735.1987621791004"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="202">
   <r>
@@ -21219,94 +21338,91 @@
 </pivotCacheRecords>
 </file>
 
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="47" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="1">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
+<file path=xl/pivotCache/pivotCacheRecords8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="6">
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-fd8126ee-9412-11e1-84cd-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="13.372823"/>
+    <n v="5112.9851040800004"/>
+    <n v="12488.289187"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="5099.6122810800007"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-013eccd2-9413-11e1-84cd-bc305b7ee8dc:trestles.sdsc.edu"/>
+    <n v="64"/>
+    <n v="32"/>
+    <n v="64"/>
+    <n v="9138.7722568499994"/>
+    <n v="12486.001956"/>
+    <n v="12488.289187"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="1"/>
+    <n v="3347.2296991500007"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-13857a0e-9430-11e1-84cd-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="11.3641088009"/>
+    <n v="7746.5628709800003"/>
+    <n v="7752.1863899199998"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="7735.1987621791004"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-158cca78-9430-11e1-84cd-bc305b7ee8dc:trestles.sdsc.edu"/>
+    <n v="64"/>
+    <n v="32"/>
+    <n v="64"/>
+    <n v="67.904299020799996"/>
+    <n v="5474.9704988000003"/>
+    <n v="7752.1863899199998"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="1"/>
+    <n v="5407.0661997792004"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-22b92086-9442-11e1-84cd-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="64"/>
+    <n v="8"/>
+    <n v="64"/>
+    <n v="10.5786662102"/>
+    <n v="6553.1529450400003"/>
+    <n v="6558.7503042199996"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="6542.5742788298003"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-24c6f574-9442-11e1-84cd-bc305b7ee8dc:trestles.sdsc.edu"/>
+    <n v="64"/>
+    <n v="32"/>
+    <n v="64"/>
+    <n v="43.676649093599998"/>
+    <n v="5515.1282181699999"/>
+    <n v="6558.7503042199996"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="1"/>
+    <n v="5471.4515690764001"/>
+  </r>
+</pivotCacheRecords>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I54:K65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -21394,6 +21510,92 @@
     <dataField name="STABW - Kraken2" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="47" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
     <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
@@ -21408,7 +21610,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I4:K21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -21629,7 +21831,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="M21:AB31" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -21767,7 +21969,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="M1:Q21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -21896,7 +22098,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="M2:O7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -21964,7 +22166,67 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="M1:O5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="9"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Mittelwert - Net Runtime" fld="10" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - Net Runtime2" fld="10" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="O6:U10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -22039,15 +22301,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-singleresource" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1bj_results" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1bj_results" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-singleresource" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22055,11 +22317,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten_1" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten_1" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data-interop" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-multi-fg-xsede" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data-interop" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22685,16 +22951,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="61" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
@@ -51935,6 +52201,226 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>421.76157190086724</v>
+      </c>
+      <c r="C2">
+        <v>1350.2136189248276</v>
+      </c>
+      <c r="D2">
+        <v>814.09690166110136</v>
+      </c>
+      <c r="E2">
+        <v>2.2251180018750141</v>
+      </c>
+      <c r="F2">
+        <v>2588.2972104886717</v>
+      </c>
+      <c r="H2">
+        <f>F2-E2</f>
+        <v>2586.0720924867965</v>
+      </c>
+      <c r="I2">
+        <f>F2-E2-C2</f>
+        <v>1235.8584735619688</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <f>[1]run1!$O$131</f>
+        <v>4243.4671542812066</v>
+      </c>
+      <c r="Q2">
+        <f>[1]run1!$O$72</f>
+        <v>1212.8018984285716</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <f>[1]run2!$O$131</f>
+        <v>4707.8597792293331</v>
+      </c>
+      <c r="Q3">
+        <f>[1]run2!$O$67</f>
+        <v>1254.3317010400001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <f>[1]run3!$O$131</f>
+        <v>3879.476980005943</v>
+      </c>
+      <c r="Q4">
+        <f>[1]run3!$O$61</f>
+        <v>2148.8040556623728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <f>[1]run4!$O$127</f>
+        <v>4722.518188808127</v>
+      </c>
+      <c r="Q5">
+        <f>[1]run4!$O$62</f>
+        <v>1091.8222408393551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <f>[1]run5!$O$131</f>
+        <v>4306.1173639416338</v>
+      </c>
+      <c r="Q6">
+        <f>[1]run5!$O$68</f>
+        <v>1194.1639064690908</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="B8">
+        <f>AVERAGE(B2:B6)</f>
+        <v>421.76157190086724</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:I8" si="0">AVERAGE(C2:C6)</f>
+        <v>1350.2136189248276</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>814.09690166110136</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2.2251180018750141</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2588.2972104886717</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>2586.0720924867965</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1235.8584735619688</v>
+      </c>
+      <c r="O8" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="P8">
+        <f>AVERAGE(P2:P7)</f>
+        <v>4371.8878932532489</v>
+      </c>
+      <c r="Q8">
+        <f>AVERAGE(Q2:Q7)</f>
+        <v>1380.3847604878779</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="O9" t="s">
+        <v>138</v>
+      </c>
+      <c r="P9">
+        <f>STDEV(P2:P6)</f>
+        <v>353.23677205817961</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ref="Q9" si="1">STDEV(Q2:Q6)</f>
+        <v>433.70154970498379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -51957,13 +52443,13 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="64" t="s">
         <v>202</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="2" t="s">
         <v>152</v>
       </c>
@@ -52143,12 +52629,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView topLeftCell="J2" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -52718,11 +53204,11 @@
       <c r="S14" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="T14" s="63" t="s">
+      <c r="T14" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="U14" s="63"/>
-      <c r="V14" s="63"/>
+      <c r="U14" s="64"/>
+      <c r="V14" s="64"/>
     </row>
     <row r="15" spans="1:22" ht="30">
       <c r="A15">
@@ -52835,7 +53321,7 @@
         <v>5.8872795343029933</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="30">
+    <row r="17" spans="1:21" ht="30">
       <c r="A17">
         <v>8</v>
       </c>
@@ -52884,7 +53370,7 @@
         <v>37.304166666666667</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:21" ht="30">
       <c r="A18">
         <v>8</v>
       </c>
@@ -52915,8 +53401,23 @@
       <c r="J18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:19">
+      <c r="O18" s="44" t="s">
+        <v>277</v>
+      </c>
+      <c r="P18" s="15">
+        <f>'BJ (FG-XSEDE)'!N3/60</f>
+        <v>107.65214067827169</v>
+      </c>
+      <c r="Q18" s="15">
+        <f>'BJ (FG-XSEDE)'!N4/60</f>
+        <v>79.031930377808905</v>
+      </c>
+      <c r="U18" s="15">
+        <f>'BJ (FG-XSEDE)'!O3/60</f>
+        <v>21.99622082922189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
       <c r="A19">
         <v>9</v>
       </c>
@@ -52948,7 +53449,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:21">
       <c r="A20">
         <v>9</v>
       </c>
@@ -52980,7 +53481,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:21">
       <c r="A21">
         <v>10</v>
       </c>
@@ -53012,7 +53513,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:21">
       <c r="A22">
         <v>10</v>
       </c>
@@ -53044,7 +53545,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:21">
       <c r="A23">
         <v>11</v>
       </c>
@@ -53076,7 +53577,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:21">
       <c r="A24">
         <v>11</v>
       </c>
@@ -53108,7 +53609,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:21">
       <c r="A25">
         <v>12</v>
       </c>
@@ -53140,7 +53641,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:21">
       <c r="A26">
         <v>12</v>
       </c>
@@ -53172,7 +53673,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:21">
       <c r="A27">
         <v>13</v>
       </c>
@@ -53204,7 +53705,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:21">
       <c r="A28">
         <v>13</v>
       </c>
@@ -53236,7 +53737,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:21">
       <c r="A29">
         <v>14</v>
       </c>
@@ -53268,7 +53769,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:21">
       <c r="A30">
         <v>14</v>
       </c>
@@ -53300,7 +53801,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:21">
       <c r="A31">
         <v>15</v>
       </c>
@@ -53332,7 +53833,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:21">
       <c r="A32">
         <v>15</v>
       </c>
@@ -56554,8 +57055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -57325,7 +57826,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C17" s="13">
         <v>128</v>
@@ -57372,7 +57873,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C18">
         <v>128</v>
@@ -57396,7 +57897,7 @@
         <v>208</v>
       </c>
       <c r="J18" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="M18" s="9">
         <v>32</v>
@@ -57446,7 +57947,7 @@
         <v>225</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="N19" s="7">
         <v>2217.9745159099998</v>
@@ -57466,7 +57967,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C20">
         <v>128</v>
@@ -57513,7 +58014,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C21">
         <v>128</v>
@@ -58077,7 +58578,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C2">
         <v>32</v>
@@ -58101,7 +58602,7 @@
         <v>208</v>
       </c>
       <c r="J2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>9</v>
@@ -58112,7 +58613,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C3">
         <v>32</v>
@@ -58136,16 +58637,16 @@
         <v>208</v>
       </c>
       <c r="J3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="O3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -58153,7 +58654,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C4">
         <v>32</v>
@@ -58194,7 +58695,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C5">
         <v>32</v>
@@ -58235,7 +58736,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C6">
         <v>32</v>
@@ -58259,7 +58760,7 @@
         <v>208</v>
       </c>
       <c r="J6" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M6" s="8">
         <v>2</v>
@@ -58276,7 +58777,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C7">
         <v>32</v>
@@ -58300,7 +58801,7 @@
         <v>208</v>
       </c>
       <c r="J7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>8</v>
@@ -58317,7 +58818,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C8">
         <v>32</v>
@@ -58344,7 +58845,7 @@
         <v>225</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="N8" s="54">
         <f>AVERAGE(N4:N6)</f>
@@ -58360,7 +58861,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C9">
         <v>32</v>
@@ -58403,7 +58904,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C10">
         <v>32</v>
@@ -58427,7 +58928,7 @@
         <v>208</v>
       </c>
       <c r="J10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -58435,7 +58936,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C11">
         <v>32</v>
@@ -58459,7 +58960,7 @@
         <v>208</v>
       </c>
       <c r="J11" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -58467,7 +58968,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C12">
         <v>32</v>
@@ -58499,7 +59000,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C13">
         <v>32</v>
@@ -58528,10 +59029,10 @@
     </row>
     <row r="15" spans="1:15">
       <c r="N15" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -58585,7 +59086,7 @@
     </row>
     <row r="22" spans="13:15" ht="16" thickTop="1">
       <c r="M22" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="N22" s="54">
         <f>AVERAGE(N16:N21)</f>
@@ -59176,8 +59677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="O112" sqref="O112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -59205,10 +59706,10 @@
     </row>
     <row r="3" spans="1:11">
       <c r="F3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="10"/>
       <c r="B4" s="18" t="s">
         <v>152</v>
@@ -59217,19 +59718,19 @@
         <v>153</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>134</v>
+        <v>272</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>276</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>247</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>248</v>
+        <v>273</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>274</v>
+      </c>
+      <c r="H4" s="66" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -59439,7 +59940,7 @@
         <f t="shared" si="1"/>
         <v>125.212722895063</v>
       </c>
-      <c r="H12" s="64">
+      <c r="H12" s="59">
         <f t="shared" ref="H12" si="2">H5/60</f>
         <v>5.5035540779422227</v>
       </c>
@@ -59611,7 +60112,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B18" s="21">
         <f>B17-B16</f>
@@ -59867,7 +60368,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B28">
         <f>B14/B19</f>
@@ -62849,216 +63350,321 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>118</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2">
+        <v>64</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>64</v>
+      </c>
+      <c r="F2">
+        <v>13.372823</v>
+      </c>
+      <c r="G2">
+        <v>5112.9851040800004</v>
+      </c>
+      <c r="H2">
+        <v>12488.289187</v>
+      </c>
+      <c r="I2" t="s">
+        <v>208</v>
+      </c>
+      <c r="J2" t="s">
+        <v>225</v>
+      </c>
+      <c r="K2">
+        <f>G2-F2</f>
+        <v>5099.6122810800007</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3">
+        <v>64</v>
+      </c>
+      <c r="D3">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+      <c r="F3">
+        <v>9138.7722568499994</v>
+      </c>
+      <c r="G3">
+        <v>12486.001956</v>
+      </c>
+      <c r="H3">
+        <v>12488.289187</v>
+      </c>
+      <c r="I3" t="s">
+        <v>208</v>
+      </c>
+      <c r="J3" t="s">
+        <v>269</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K7" si="0">G3-F3</f>
+        <v>3347.2296991500007</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="N3" s="7">
+        <v>6459.1284406963014</v>
+      </c>
+      <c r="O3" s="7">
+        <v>1319.7732497533134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>421.76157190086724</v>
-      </c>
-      <c r="C2">
-        <v>1350.2136189248276</v>
-      </c>
-      <c r="D2">
-        <v>814.09690166110136</v>
-      </c>
-      <c r="E2">
-        <v>2.2251180018750141</v>
-      </c>
-      <c r="F2">
-        <v>2588.2972104886717</v>
-      </c>
-      <c r="H2">
-        <f>F2-E2</f>
-        <v>2586.0720924867965</v>
-      </c>
-      <c r="I2">
-        <f>F2-E2-C2</f>
-        <v>1235.8584735619688</v>
-      </c>
-      <c r="O2">
+      <c r="B4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4">
+        <v>64</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>64</v>
+      </c>
+      <c r="F4">
+        <v>11.3641088009</v>
+      </c>
+      <c r="G4">
+        <v>7746.5628709800003</v>
+      </c>
+      <c r="H4">
+        <v>7752.1863899199998</v>
+      </c>
+      <c r="I4" t="s">
+        <v>208</v>
+      </c>
+      <c r="J4" t="s">
+        <v>225</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>7735.1987621791004</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="N4" s="7">
+        <v>4741.915822668534</v>
+      </c>
+      <c r="O4" s="7">
+        <v>1208.2625568543642</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5">
         <v>1</v>
       </c>
-      <c r="P2">
-        <f>[1]run1!$O$131</f>
-        <v>4243.4671542812066</v>
-      </c>
-      <c r="Q2">
-        <f>[1]run1!$O$72</f>
-        <v>1212.8018984285716</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3">
+      <c r="B5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5">
+        <v>64</v>
+      </c>
+      <c r="D5">
+        <v>32</v>
+      </c>
+      <c r="E5">
+        <v>64</v>
+      </c>
+      <c r="F5">
+        <v>67.904299020799996</v>
+      </c>
+      <c r="G5">
+        <v>5474.9704988000003</v>
+      </c>
+      <c r="H5">
+        <v>7752.1863899199998</v>
+      </c>
+      <c r="I5" t="s">
+        <v>208</v>
+      </c>
+      <c r="J5" t="s">
+        <v>269</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>5407.0661997792004</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="7">
+        <v>5600.5221316824172</v>
+      </c>
+      <c r="O5" s="7">
+        <v>1471.5045659047066</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6">
         <v>2</v>
       </c>
-      <c r="O3">
+      <c r="B6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6">
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>64</v>
+      </c>
+      <c r="F6">
+        <v>10.5786662102</v>
+      </c>
+      <c r="G6">
+        <v>6553.1529450400003</v>
+      </c>
+      <c r="H6">
+        <v>6558.7503042199996</v>
+      </c>
+      <c r="I6" t="s">
+        <v>208</v>
+      </c>
+      <c r="J6" t="s">
+        <v>225</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>6542.5742788298003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7">
         <v>2</v>
       </c>
-      <c r="P3">
-        <f>[1]run2!$O$131</f>
-        <v>4707.8597792293331</v>
-      </c>
-      <c r="Q3">
-        <f>[1]run2!$O$67</f>
-        <v>1254.3317010400001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="O4">
-        <v>3</v>
-      </c>
-      <c r="P4">
-        <f>[1]run3!$O$131</f>
-        <v>3879.476980005943</v>
-      </c>
-      <c r="Q4">
-        <f>[1]run3!$O$61</f>
-        <v>2148.8040556623728</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="O5">
-        <v>4</v>
-      </c>
-      <c r="P5">
-        <f>[1]run4!$O$127</f>
-        <v>4722.518188808127</v>
-      </c>
-      <c r="Q5">
-        <f>[1]run4!$O$62</f>
-        <v>1091.8222408393551</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="O6">
-        <v>5</v>
-      </c>
-      <c r="P6">
-        <f>[1]run5!$O$131</f>
-        <v>4306.1173639416338</v>
-      </c>
-      <c r="Q6">
-        <f>[1]run5!$O$68</f>
-        <v>1194.1639064690908</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="B8">
-        <f>AVERAGE(B2:B6)</f>
-        <v>421.76157190086724</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ref="C8:I8" si="0">AVERAGE(C2:C6)</f>
-        <v>1350.2136189248276</v>
-      </c>
-      <c r="D8">
+      <c r="B7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7">
+        <v>64</v>
+      </c>
+      <c r="D7">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>64</v>
+      </c>
+      <c r="F7">
+        <v>43.676649093599998</v>
+      </c>
+      <c r="G7">
+        <v>5515.1282181699999</v>
+      </c>
+      <c r="H7">
+        <v>6558.7503042199996</v>
+      </c>
+      <c r="I7" t="s">
+        <v>208</v>
+      </c>
+      <c r="J7" t="s">
+        <v>269</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="0"/>
-        <v>814.09690166110136</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>2.2251180018750141</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>2588.2972104886717</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>2586.0720924867965</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>1235.8584735619688</v>
-      </c>
-      <c r="O8" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="P8">
-        <f>AVERAGE(P2:P7)</f>
-        <v>4371.8878932532489</v>
-      </c>
-      <c r="Q8">
-        <f>AVERAGE(Q2:Q7)</f>
-        <v>1380.3847604878779</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="O9" t="s">
-        <v>138</v>
-      </c>
-      <c r="P9">
-        <f>STDEV(P2:P6)</f>
-        <v>353.23677205817961</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" ref="Q9" si="1">STDEV(Q2:Q6)</f>
-        <v>433.70154970498379</v>
+        <v>5471.4515690764001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated figure 7 with latest india data
git-svn-id: file://localhost/tmp/svn2git/svn@7209 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="0" windowWidth="41800" windowHeight="28260" tabRatio="500" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="20560" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -24,24 +24,26 @@
     <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_1bj_results" localSheetId="2">'BJ w Staging'!$A$20:$J$21</definedName>
+    <definedName name="_1bj_results" localSheetId="2">'BJ w Staging'!$A$19:$J$20</definedName>
     <definedName name="_2bj_results" localSheetId="3">'BJ (FG multi)'!$A$1:$J$13</definedName>
+    <definedName name="bj_india" localSheetId="2">'BJ w Staging'!$A$41:$J$44</definedName>
+    <definedName name="bj_india_1" localSheetId="2">'BJ w Staging'!$A$62:$J$70</definedName>
     <definedName name="bj_multi_fg_xsede" localSheetId="8">'BJ (FG-XSEDE)'!$A$1:$J$7</definedName>
-    <definedName name="bj_singleresource" localSheetId="2">'BJ w Staging'!$A$1:$J$35</definedName>
+    <definedName name="bj_singleresource" localSheetId="2">'BJ w Staging'!$A$1:$J$37</definedName>
     <definedName name="data_interop" localSheetId="11">'Interop '!$A$1:$J$32</definedName>
     <definedName name="daten" localSheetId="1">BigJob!$A$1:$J$64</definedName>
     <definedName name="daten_1" localSheetId="7">'Raw (BJ)'!$A$1:$J$109</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId14"/>
-    <pivotCache cacheId="13" r:id="rId15"/>
-    <pivotCache cacheId="14" r:id="rId16"/>
-    <pivotCache cacheId="15" r:id="rId17"/>
-    <pivotCache cacheId="16" r:id="rId18"/>
-    <pivotCache cacheId="17" r:id="rId19"/>
-    <pivotCache cacheId="18" r:id="rId20"/>
-    <pivotCache cacheId="21" r:id="rId21"/>
+    <pivotCache cacheId="0" r:id="rId14"/>
+    <pivotCache cacheId="1" r:id="rId15"/>
+    <pivotCache cacheId="2" r:id="rId16"/>
+    <pivotCache cacheId="3" r:id="rId17"/>
+    <pivotCache cacheId="4" r:id="rId18"/>
+    <pivotCache cacheId="5" r:id="rId19"/>
+    <pivotCache cacheId="7" r:id="rId20"/>
+    <pivotCache cacheId="28" r:id="rId21"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -85,7 +87,39 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="bj-multi-fg-xsede.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="3" name="bj-india.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:Dropbox:SAGA:papers:troy:pstar:perf:sc:bj-india.txt" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="bj-india.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:Dropbox:SAGA:papers:troy:pstar:perf:sc:bj-india.txt" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="bj-multi-fg-xsede.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:Dropbox:SAGA:papers:troy:pstar:perf:sc:bj-multi-fg-xsede.txt" comma="1">
       <textFields count="10">
         <textField/>
@@ -101,7 +135,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="bj-singleresource.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="6" name="bj-singleresource.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:Dropbox:SAGA:papers:troy:pstar:perf:sc:bj-singleresource.txt" comma="1">
       <textFields count="10">
         <textField/>
@@ -117,14 +151,14 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="data-interop.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="7" name="data-interop.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:data-interop.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="daten.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="8" name="daten.csv" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields count="10">
         <textField/>
@@ -140,21 +174,21 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="daten.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="9" name="daten.csv1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="daten.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="10" name="daten.csv2" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="daten.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="11" name="daten.csv3" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="MacSSD:Users:luckow:workspace-saga:applications:bigjob-performance:fg-xsede:daten.csv" comma="1">
       <textFields>
         <textField/>
@@ -165,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="290">
   <si>
     <t>bfast</t>
   </si>
@@ -905,9 +939,6 @@
     <t>Compute</t>
   </si>
   <si>
-    <t>to refine</t>
-  </si>
-  <si>
     <t>bigjob:bj-aff746cc-917b-11e1-a9eb-bc305b7ee8dc:sierra.futuregrid.org</t>
   </si>
   <si>
@@ -1028,6 +1059,24 @@
   <si>
     <t>STABW - Net Runtime2</t>
   </si>
+  <si>
+    <t>bigjob:bj-5221b9d8-949b-11e1-ba79-bc305b7ee8dc:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-b2611c38-94b1-11e1-ba79-bc305b7ee8dc:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>bigjob:bj-979f66f0-94c7-11e1-ba79-bc305b7ee8dc:india.futuregrid.org</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Download </t>
+  </si>
+  <si>
+    <t>Mittel</t>
+  </si>
 </sst>
 </file>
 
@@ -1036,7 +1085,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1104,6 +1153,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -1299,7 +1359,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="143">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1443,8 +1503,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1513,9 +1587,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
@@ -1523,6 +1595,12 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1538,14 +1616,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="143">
+  <cellStyles count="157">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1617,6 +1692,13 @@
     <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1688,6 +1770,13 @@
     <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
@@ -1889,11 +1978,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2092735608"/>
-        <c:axId val="2085705288"/>
+        <c:axId val="2069539432"/>
+        <c:axId val="2069542392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2092735608"/>
+        <c:axId val="2069539432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1903,7 +1992,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085705288"/>
+        <c:crossAx val="2069542392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1911,7 +2000,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2085705288"/>
+        <c:axId val="2069542392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1922,7 +2011,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092735608"/>
+        <c:crossAx val="2069539432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2220,11 +2309,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2093737544"/>
-        <c:axId val="2093541960"/>
+        <c:axId val="2033532504"/>
+        <c:axId val="2033541304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2093737544"/>
+        <c:axId val="2033532504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2258,7 +2347,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093541960"/>
+        <c:crossAx val="2033541304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2266,7 +2355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2093541960"/>
+        <c:axId val="2033541304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2277,7 +2366,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2093737544"/>
+        <c:crossAx val="2033532504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2589,11 +2678,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2090067192"/>
-        <c:axId val="2090144472"/>
+        <c:axId val="2069652056"/>
+        <c:axId val="2069657784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2090067192"/>
+        <c:axId val="2069652056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2626,7 +2715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090144472"/>
+        <c:crossAx val="2069657784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2634,7 +2723,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090144472"/>
+        <c:axId val="2069657784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2663,7 +2752,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090067192"/>
+        <c:crossAx val="2069652056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2929,11 +3018,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2091238680"/>
-        <c:axId val="2091241720"/>
+        <c:axId val="2070025576"/>
+        <c:axId val="2070019976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2091238680"/>
+        <c:axId val="2070025576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2955,7 +3044,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091241720"/>
+        <c:crossAx val="2070019976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2963,7 +3052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091241720"/>
+        <c:axId val="2070019976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -3020,7 +3109,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091238680"/>
+        <c:crossAx val="2070025576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3248,11 +3337,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2091788904"/>
-        <c:axId val="2091791944"/>
+        <c:axId val="2069970472"/>
+        <c:axId val="2069967416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2091788904"/>
+        <c:axId val="2069970472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3274,7 +3363,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091791944"/>
+        <c:crossAx val="2069967416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3282,7 +3371,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091791944"/>
+        <c:axId val="2069967416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3331,7 +3420,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091788904"/>
+        <c:crossAx val="2069970472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3438,7 +3527,7 @@
                   <c:v>191.0096412556054</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>245.45</c:v>
+                  <c:v>147.6733333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>115.4936172222222</c:v>
@@ -3481,7 +3570,7 @@
                     <c:v>35.03971545</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>294.4423239772857</c:v>
+                    <c:v>94.16504241305603</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>20.84980258491097</c:v>
@@ -3505,7 +3594,7 @@
                     <c:v>35.03971545</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>294.4423239772857</c:v>
+                    <c:v>94.16504241305603</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>20.84980258491097</c:v>
@@ -3550,10 +3639,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>26.9553659860612</c:v>
+                  <c:v>15.17681269489461</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91.04129413215924</c:v>
+                  <c:v>64.78247025965953</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24.56504025566889</c:v>
@@ -3578,11 +3667,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2091841048"/>
-        <c:axId val="2091844024"/>
+        <c:axId val="2069917320"/>
+        <c:axId val="2069914328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2091841048"/>
+        <c:axId val="2069917320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3604,7 +3693,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091844024"/>
+        <c:crossAx val="2069914328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3612,7 +3701,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091844024"/>
+        <c:axId val="2069914328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3657,7 +3746,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2091841048"/>
+        <c:crossAx val="2069917320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3991,11 +4080,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2089940760"/>
-        <c:axId val="2089944024"/>
+        <c:axId val="2076639112"/>
+        <c:axId val="2076635832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2089940760"/>
+        <c:axId val="2076639112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4017,7 +4106,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2089944024"/>
+        <c:crossAx val="2076635832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4025,7 +4114,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2089944024"/>
+        <c:axId val="2076635832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4080,7 +4169,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2089940760"/>
+        <c:crossAx val="2076639112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4730,64 +4819,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41030.902490740744" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="34">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:J35" sheet="BJ w Staging"/>
-  </cacheSource>
-  <cacheFields count="10">
-    <cacheField name="Run" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2"/>
-    </cacheField>
-    <cacheField name="BJ" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="#Nodes" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="128"/>
-    </cacheField>
-    <cacheField name="#cores/node" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="8" maxValue="32"/>
-    </cacheField>
-    <cacheField name="#jobs" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="128" count="7">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="4"/>
-        <n v="8"/>
-        <n v="16"/>
-        <n v="32"/>
-        <n v="128"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Queuing Time" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.6857481002799997" maxValue="25158.968379999998"/>
-    </cacheField>
-    <cacheField name="BJ Runtime" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="727.22062802300002" maxValue="47417.862745999999"/>
-    </cacheField>
-    <cacheField name="Total Runtime" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="728.41032099699999" maxValue="47419.311981899999"/>
-    </cacheField>
-    <cacheField name="Coordination URL" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="LRMS URL" numFmtId="0">
-      <sharedItems count="4">
-        <s v="pbs-ssh://luckow@trestles.sdsc.edu"/>
-        <s v="pbs-ssh://pmantha@trestles.sdsc.edu"/>
-        <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
-        <s v="sge-ssh://login2.ls4.tacc.utexas.edu"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41031.942976967592" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="6">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:K7" sheet="BJ (FG-XSEDE)"/>
@@ -4838,6 +4869,67 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Andre Luckow" refreshedDate="41032.805360995371" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="36">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:K37" sheet="BJ w Staging"/>
+  </cacheSource>
+  <cacheFields count="11">
+    <cacheField name="Run" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2"/>
+    </cacheField>
+    <cacheField name="BJ" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="#Nodes" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="128"/>
+    </cacheField>
+    <cacheField name="#cores/node" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="8" maxValue="32"/>
+    </cacheField>
+    <cacheField name="#jobs" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="128" count="7">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="4"/>
+        <n v="8"/>
+        <n v="16"/>
+        <n v="32"/>
+        <n v="128"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Queuing Time" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.6857481002799997" maxValue="25158.968379999998"/>
+    </cacheField>
+    <cacheField name="BJ Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="727.22062802300002" maxValue="37332.644954199997"/>
+    </cacheField>
+    <cacheField name="Total Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="728.41032099699999" maxValue="37333.205501999997"/>
+    </cacheField>
+    <cacheField name="Coordination URL" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="LRMS URL" numFmtId="0">
+      <sharedItems count="4">
+        <s v="pbs-ssh://luckow@trestles.sdsc.edu"/>
+        <s v="pbs-ssh://pmantha@india.futuregrid.org"/>
+        <s v="sge-ssh://login2.ls4.tacc.utexas.edu"/>
+        <s v="pbs-ssh://pmantha@trestles.sdsc.edu" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Net Runtime" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="627.13998198499996" maxValue="22374.943838788942"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="202">
   <r>
@@ -20926,419 +21018,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="34">
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-887db1c6-910d-11e1-b0d6-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="0"/>
-    <n v="954.949452877"/>
-    <n v="1904.65635991"/>
-    <n v="1905.0930659799999"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-6eaa9054-9115-11e1-98f3-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="1"/>
-    <n v="2756.7323818199998"/>
-    <n v="3690.6159229300001"/>
-    <n v="3691.0615439399999"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-074da80c-911e-11e1-98f3-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="1"/>
-    <n v="763.49348592800004"/>
-    <n v="1723.08778095"/>
-    <n v="1723.5316910700001"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-0e36ce2c-9124-11e1-8878-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="2"/>
-    <n v="926.05387902300004"/>
-    <n v="1960.3043100800001"/>
-    <n v="1960.7434251300001"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-9f8569ac-9128-11e1-8878-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="2"/>
-    <n v="3333.1491689700001"/>
-    <n v="4343.1737480199999"/>
-    <n v="4343.7153339400002"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-7d5abb86-9135-11e1-9521-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="3"/>
-    <n v="37.059126853899997"/>
-    <n v="1116.8879890400001"/>
-    <n v="1117.33498502"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-17ff803e-9138-11e1-9521-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="3"/>
-    <n v="57.486021995500003"/>
-    <n v="1199.46437597"/>
-    <n v="1200.04477"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="bigjob:bj-e3f22442-913a-11e1-9521-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="3"/>
-    <n v="2489.0308990499998"/>
-    <n v="3594.5141370299998"/>
-    <n v="3595.0533909800001"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-77e71942-9144-11e1-a3da-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="4"/>
-    <n v="215.984438896"/>
-    <n v="1851.46343207"/>
-    <n v="1851.9019539400001"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-c9cb5f94-9148-11e1-a3da-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="4"/>
-    <n v="1587.50521493"/>
-    <n v="2996.0286328799998"/>
-    <n v="2996.4767038800001"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="bigjob:bj-c46c6c4e-914f-11e1-a3da-00259019a082:trestles.sdsc.edu"/>
-    <n v="16"/>
-    <n v="16"/>
-    <x v="4"/>
-    <n v="1925.84539294"/>
-    <n v="3292.3419399300001"/>
-    <n v="3292.7900688599998"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-93be4550-9158-11e1-ba03-00259019a082:trestles.sdsc.edu"/>
-    <n v="32"/>
-    <n v="16"/>
-    <x v="5"/>
-    <n v="1001.75782609"/>
-    <n v="4281.8598151200003"/>
-    <n v="4282.3115339300002"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-8ce94fb8-9162-11e1-ba03-00259019a082:trestles.sdsc.edu"/>
-    <n v="32"/>
-    <n v="16"/>
-    <x v="5"/>
-    <n v="1210.1403880099999"/>
-    <n v="3310.2213969200002"/>
-    <n v="3310.6605689500002"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="bigjob:bj-42db75e2-916a-11e1-ba03-00259019a082:trestles.sdsc.edu"/>
-    <n v="32"/>
-    <n v="16"/>
-    <x v="5"/>
-    <n v="2226.8310780500001"/>
-    <n v="4308.7829060599997"/>
-    <n v="4309.21431708"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-ff8c95b8-922d-11e1-8232-00259019a084:trestles.sdsc.edu"/>
-    <n v="128"/>
-    <n v="16"/>
-    <x v="6"/>
-    <n v="22768.135295200002"/>
-    <n v="37332.644954199997"/>
-    <n v="37333.205501999997"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-3ff74b52-935f-11e1-ac66-00259019a084:trestles.sdsc.edu"/>
-    <n v="128"/>
-    <n v="16"/>
-    <x v="6"/>
-    <n v="25158.968379999998"/>
-    <n v="36750.259590000001"/>
-    <n v="36750.694069999998"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-3f8cbd32-93a0-11e1-bbde-bc305b7ee8dc:trestles.sdsc.edu"/>
-    <n v="128"/>
-    <n v="32"/>
-    <x v="6"/>
-    <n v="2217.9745159099998"/>
-    <n v="13175.735358"/>
-    <n v="13178.010752"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-5c9ed678-9259-11e1-83ec-bc305b7ee8dc:india.futuregrid.org"/>
-    <n v="128"/>
-    <n v="8"/>
-    <x v="6"/>
-    <n v="22527.895972999999"/>
-    <n v="47417.862745999999"/>
-    <n v="47419.311981899999"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-ca2a8246-92c7-11e1-83ec-bc305b7ee8dc:india.futuregrid.org"/>
-    <n v="128"/>
-    <n v="8"/>
-    <x v="6"/>
-    <n v="5.7084000110600002"/>
-    <n v="22380.652238800001"/>
-    <n v="22382.094851999998"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="bigjob:bj-e99b42c6-92fb-11e1-83ec-bc305b7ee8dc:india.futuregrid.org"/>
-    <n v="128"/>
-    <n v="8"/>
-    <x v="6"/>
-    <n v="4.6857481002799997"/>
-    <n v="13308.208080099999"/>
-    <n v="13309.640333200001"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-4612a348-9124-11e1-a963-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="12"/>
-    <n v="12"/>
-    <x v="1"/>
-    <n v="300.654438019"/>
-    <n v="934.00202012099999"/>
-    <n v="935.09974002800004"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-747550ee-9126-11e1-a963-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="12"/>
-    <n v="12"/>
-    <x v="1"/>
-    <n v="113.3769629"/>
-    <n v="756.88640379900005"/>
-    <n v="758.091012955"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="bigjob:bj-39586116-9128-11e1-a963-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="12"/>
-    <n v="12"/>
-    <x v="1"/>
-    <n v="100.828622103"/>
-    <n v="727.96860408800001"/>
-    <n v="729.173197985"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-4a0e58e8-9138-11e1-b8c2-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="12"/>
-    <n v="12"/>
-    <x v="2"/>
-    <n v="252.339545012"/>
-    <n v="927.508314133"/>
-    <n v="928.868350029"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-74bdac40-913a-11e1-b8c2-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="12"/>
-    <n v="12"/>
-    <x v="2"/>
-    <n v="220.36070990600001"/>
-    <n v="912.68654990200002"/>
-    <n v="913.90338492399997"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="bigjob:bj-967df9aa-913c-11e1-b8c2-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="12"/>
-    <n v="12"/>
-    <x v="2"/>
-    <n v="55.585777044300002"/>
-    <n v="727.22062802300002"/>
-    <n v="728.41032099699999"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-649d717e-913f-11e1-b681-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="12"/>
-    <n v="12"/>
-    <x v="3"/>
-    <n v="1703.66234207"/>
-    <n v="2510.5651390600001"/>
-    <n v="2511.7870490599998"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-3ec875c4-9145-11e1-b681-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="12"/>
-    <n v="12"/>
-    <x v="3"/>
-    <n v="90.235594987900001"/>
-    <n v="1207.55374312"/>
-    <n v="1208.7523281599999"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="bigjob:bj-104d361e-9148-11e1-b681-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="12"/>
-    <n v="12"/>
-    <x v="3"/>
-    <n v="79.823445081700001"/>
-    <n v="866.61979699100004"/>
-    <n v="867.81867504100001"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-6b6d5e78-914a-11e1-94be-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="24"/>
-    <n v="12"/>
-    <x v="4"/>
-    <n v="263.91831493400002"/>
-    <n v="1318.27436304"/>
-    <n v="1319.4774529900001"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-7ef5a772-914d-11e1-94be-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="24"/>
-    <n v="12"/>
-    <x v="4"/>
-    <n v="141.600160837"/>
-    <n v="1207.09737587"/>
-    <n v="1208.20039296"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <s v="bigjob:bj-503066f4-9150-11e1-94be-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="24"/>
-    <n v="12"/>
-    <x v="4"/>
-    <n v="2982.8733580100002"/>
-    <n v="4049.5441341400001"/>
-    <n v="4050.7455921199999"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="0"/>
-    <s v="bigjob:bj-58acbc06-915a-11e1-88ca-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="36"/>
-    <n v="12"/>
-    <x v="5"/>
-    <n v="23.373319864300001"/>
-    <n v="2503.21842599"/>
-    <n v="2504.4764480600002"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <s v="bigjob:bj-2eac1446-9160-11e1-88ca-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
-    <n v="36"/>
-    <n v="12"/>
-    <x v="5"/>
-    <n v="371.93604397799999"/>
-    <n v="1988.56460881"/>
-    <n v="1989.9456028899999"/>
-    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
-    <x v="3"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords8.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="6">
   <r>
     <n v="0"/>
@@ -21421,8 +21100,567 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="36">
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-887db1c6-910d-11e1-b0d6-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="0"/>
+    <n v="954.949452877"/>
+    <n v="1904.65635991"/>
+    <n v="1905.0930659799999"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="949.70690703299999"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-6eaa9054-9115-11e1-98f3-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="1"/>
+    <n v="2756.7323818199998"/>
+    <n v="3690.6159229300001"/>
+    <n v="3691.0615439399999"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="933.88354111000035"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-074da80c-911e-11e1-98f3-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="1"/>
+    <n v="763.49348592800004"/>
+    <n v="1723.08778095"/>
+    <n v="1723.5316910700001"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="959.59429502199998"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-0e36ce2c-9124-11e1-8878-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="2"/>
+    <n v="926.05387902300004"/>
+    <n v="1960.3043100800001"/>
+    <n v="1960.7434251300001"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="1034.250431057"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-9f8569ac-9128-11e1-8878-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="2"/>
+    <n v="3333.1491689700001"/>
+    <n v="4343.1737480199999"/>
+    <n v="4343.7153339400002"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="1010.0245790499998"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-7d5abb86-9135-11e1-9521-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="3"/>
+    <n v="37.059126853899997"/>
+    <n v="1116.8879890400001"/>
+    <n v="1117.33498502"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="1079.8288621861002"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-17ff803e-9138-11e1-9521-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="3"/>
+    <n v="57.486021995500003"/>
+    <n v="1199.46437597"/>
+    <n v="1200.04477"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="1141.9783539744999"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-e3f22442-913a-11e1-9521-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="3"/>
+    <n v="2489.0308990499998"/>
+    <n v="3594.5141370299998"/>
+    <n v="3595.0533909800001"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="1105.48323798"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-77e71942-9144-11e1-a3da-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="4"/>
+    <n v="215.984438896"/>
+    <n v="1851.46343207"/>
+    <n v="1851.9019539400001"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="1635.4789931739999"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-c9cb5f94-9148-11e1-a3da-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="4"/>
+    <n v="1587.50521493"/>
+    <n v="2996.0286328799998"/>
+    <n v="2996.4767038800001"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="1408.5234179499998"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-c46c6c4e-914f-11e1-a3da-00259019a082:trestles.sdsc.edu"/>
+    <n v="16"/>
+    <n v="16"/>
+    <x v="4"/>
+    <n v="1925.84539294"/>
+    <n v="3292.3419399300001"/>
+    <n v="3292.7900688599998"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="1366.4965469900001"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-93be4550-9158-11e1-ba03-00259019a082:trestles.sdsc.edu"/>
+    <n v="32"/>
+    <n v="16"/>
+    <x v="5"/>
+    <n v="1001.75782609"/>
+    <n v="4281.8598151200003"/>
+    <n v="4282.3115339300002"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="3280.1019890300004"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-8ce94fb8-9162-11e1-ba03-00259019a082:trestles.sdsc.edu"/>
+    <n v="32"/>
+    <n v="16"/>
+    <x v="5"/>
+    <n v="1210.1403880099999"/>
+    <n v="3310.2213969200002"/>
+    <n v="3310.6605689500002"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="2100.0810089100005"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-42db75e2-916a-11e1-ba03-00259019a082:trestles.sdsc.edu"/>
+    <n v="32"/>
+    <n v="16"/>
+    <x v="5"/>
+    <n v="2226.8310780500001"/>
+    <n v="4308.7829060599997"/>
+    <n v="4309.21431708"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="2081.9518280099996"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-ff8c95b8-922d-11e1-8232-00259019a084:trestles.sdsc.edu"/>
+    <n v="128"/>
+    <n v="16"/>
+    <x v="6"/>
+    <n v="22768.135295200002"/>
+    <n v="37332.644954199997"/>
+    <n v="37333.205501999997"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="14564.509658999996"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-3ff74b52-935f-11e1-ac66-00259019a084:trestles.sdsc.edu"/>
+    <n v="128"/>
+    <n v="16"/>
+    <x v="6"/>
+    <n v="25158.968379999998"/>
+    <n v="36750.259590000001"/>
+    <n v="36750.694069999998"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="11591.291210000003"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-3f8cbd32-93a0-11e1-bbde-bc305b7ee8dc:trestles.sdsc.edu"/>
+    <n v="128"/>
+    <n v="32"/>
+    <x v="6"/>
+    <n v="2217.9745159099998"/>
+    <n v="13175.735358"/>
+    <n v="13178.010752"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="0"/>
+    <n v="10957.76084209"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-ca2a8246-92c7-11e1-83ec-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="128"/>
+    <n v="8"/>
+    <x v="6"/>
+    <n v="5.7084000110600002"/>
+    <n v="22380.652238800001"/>
+    <n v="22382.094851999998"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="1"/>
+    <n v="22374.943838788942"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-e99b42c6-92fb-11e1-83ec-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="128"/>
+    <n v="8"/>
+    <x v="6"/>
+    <n v="4.6857481002799997"/>
+    <n v="13308.208080099999"/>
+    <n v="13309.640333200001"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="1"/>
+    <n v="13303.522331999719"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-5221b9d8-949b-11e1-ba79-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="128"/>
+    <n v="8"/>
+    <x v="6"/>
+    <n v="6.1047720909100001"/>
+    <n v="9601.0439431699997"/>
+    <n v="9602.4777331400001"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="1"/>
+    <n v="9594.9391710790896"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-b2611c38-94b1-11e1-ba79-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="128"/>
+    <n v="8"/>
+    <x v="6"/>
+    <n v="48.316945076000003"/>
+    <n v="9398.2399060700009"/>
+    <n v="9399.7276799699994"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="1"/>
+    <n v="9349.9229609940012"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-979f66f0-94c7-11e1-ba79-bc305b7ee8dc:india.futuregrid.org"/>
+    <n v="128"/>
+    <n v="8"/>
+    <x v="6"/>
+    <n v="40.209950923900003"/>
+    <n v="9153.62272596"/>
+    <n v="9154.9730839700005"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="1"/>
+    <n v="9113.4127750361004"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-4612a348-9124-11e1-a963-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="12"/>
+    <n v="12"/>
+    <x v="1"/>
+    <n v="300.654438019"/>
+    <n v="934.00202012099999"/>
+    <n v="935.09974002800004"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="633.34758210199993"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-747550ee-9126-11e1-a963-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="12"/>
+    <n v="12"/>
+    <x v="1"/>
+    <n v="113.3769629"/>
+    <n v="756.88640379900005"/>
+    <n v="758.091012955"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="643.50944089900008"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-39586116-9128-11e1-a963-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="12"/>
+    <n v="12"/>
+    <x v="1"/>
+    <n v="100.828622103"/>
+    <n v="727.96860408800001"/>
+    <n v="729.173197985"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="627.13998198499996"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-4a0e58e8-9138-11e1-b8c2-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="12"/>
+    <n v="12"/>
+    <x v="2"/>
+    <n v="252.339545012"/>
+    <n v="927.508314133"/>
+    <n v="928.868350029"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="675.16876912099997"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-74bdac40-913a-11e1-b8c2-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="12"/>
+    <n v="12"/>
+    <x v="2"/>
+    <n v="220.36070990600001"/>
+    <n v="912.68654990200002"/>
+    <n v="913.90338492399997"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="692.32583999600001"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-967df9aa-913c-11e1-b8c2-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="12"/>
+    <n v="12"/>
+    <x v="2"/>
+    <n v="55.585777044300002"/>
+    <n v="727.22062802300002"/>
+    <n v="728.41032099699999"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="671.6348509787"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-649d717e-913f-11e1-b681-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="12"/>
+    <n v="12"/>
+    <x v="3"/>
+    <n v="1703.66234207"/>
+    <n v="2510.5651390600001"/>
+    <n v="2511.7870490599998"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="806.90279699000007"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-3ec875c4-9145-11e1-b681-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="12"/>
+    <n v="12"/>
+    <x v="3"/>
+    <n v="90.235594987900001"/>
+    <n v="1207.55374312"/>
+    <n v="1208.7523281599999"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="1117.3181481321001"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-104d361e-9148-11e1-b681-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="12"/>
+    <n v="12"/>
+    <x v="3"/>
+    <n v="79.823445081700001"/>
+    <n v="866.61979699100004"/>
+    <n v="867.81867504100001"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="786.79635190930003"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-6b6d5e78-914a-11e1-94be-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="24"/>
+    <n v="12"/>
+    <x v="4"/>
+    <n v="263.91831493400002"/>
+    <n v="1318.27436304"/>
+    <n v="1319.4774529900001"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="1054.3560481059999"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-7ef5a772-914d-11e1-94be-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="24"/>
+    <n v="12"/>
+    <x v="4"/>
+    <n v="141.600160837"/>
+    <n v="1207.09737587"/>
+    <n v="1208.20039296"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="1065.497215033"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <s v="bigjob:bj-503066f4-9150-11e1-94be-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="24"/>
+    <n v="12"/>
+    <x v="4"/>
+    <n v="2982.8733580100002"/>
+    <n v="4049.5441341400001"/>
+    <n v="4050.7455921199999"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="1066.6707761299999"/>
+  </r>
+  <r>
+    <n v="0"/>
+    <s v="bigjob:bj-58acbc06-915a-11e1-88ca-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="36"/>
+    <n v="12"/>
+    <x v="5"/>
+    <n v="23.373319864300001"/>
+    <n v="2503.21842599"/>
+    <n v="2504.4764480600002"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="2479.8451061257001"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <s v="bigjob:bj-2eac1446-9160-11e1-88ca-f04da2004b3c:login2.ls4.tacc.utexas.edu"/>
+    <n v="36"/>
+    <n v="12"/>
+    <x v="5"/>
+    <n v="371.93604397799999"/>
+    <n v="1988.56460881"/>
+    <n v="1989.9456028899999"/>
+    <s v="redis://ILikeBigJob_wITH-REdIS@gw68.quarry.iu.teragrid.org:6379"/>
+    <x v="2"/>
+    <n v="1616.6285648319999"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="47" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I54:K65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -21510,92 +21748,6 @@
     <dataField name="STABW - Kraken2" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="47" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
     <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
@@ -21610,7 +21762,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I4:K21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -21831,7 +21983,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="M21:AB31" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -21969,9 +22121,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="M1:Q21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="M1:Q19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="11">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -21995,18 +22147,19 @@
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
         <item x="0"/>
+        <item x="1"/>
         <item x="2"/>
-        <item x="3"/>
-        <item x="1"/>
+        <item m="1" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
     <field x="9"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="19">
+  <rowItems count="17">
     <i>
       <x/>
     </i>
@@ -22055,12 +22208,6 @@
     <i r="1">
       <x v="5"/>
     </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
@@ -22086,7 +22233,7 @@
     <dataField name="Mittelwert - Queuing Time" fld="5" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Mittelwert - BJ Runtime" fld="6" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Queuing Time2" fld="5" subtotal="stdDev" baseField="0" baseItem="0"/>
-    <dataField name="STABW - BJ Runtime" fld="6" subtotal="stdDev" baseField="0" baseItem="0"/>
+    <dataField name="STABW - Net Runtime" fld="10" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -22098,7 +22245,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="M2:O7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -22166,7 +22313,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="M1:O5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -22226,7 +22373,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="O6:U10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -22301,31 +22448,39 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-india_1" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-india" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-singleresource" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1bj_results" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-singleresource" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="2bj-results" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten_1" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="daten_1" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-multi-fg-xsede" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-multi-fg-xsede" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data-interop" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="data-interop" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -52633,7 +52788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
@@ -53402,7 +53557,7 @@
         <v>47</v>
       </c>
       <c r="O18" s="44" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P18" s="15">
         <f>'BJ (FG-XSEDE)'!N3/60</f>
@@ -57053,16 +57208,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:F21"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.1640625" customWidth="1"/>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
@@ -57073,9 +57228,40 @@
     <col min="10" max="10" width="34.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="36.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.83203125" customWidth="1"/>
-    <col min="15" max="15" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
     <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="17.83203125" customWidth="1"/>
+    <col min="17" max="17" width="19" customWidth="1"/>
+    <col min="18" max="28" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.1640625" customWidth="1"/>
+    <col min="30" max="49" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.1640625" customWidth="1"/>
+    <col min="52" max="52" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.1640625" customWidth="1"/>
+    <col min="54" max="55" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.1640625" customWidth="1"/>
+    <col min="57" max="63" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="65" width="11.1640625" customWidth="1"/>
+    <col min="66" max="69" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.1640625" customWidth="1"/>
+    <col min="71" max="85" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="21" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="12.1640625" customWidth="1"/>
+    <col min="89" max="89" width="11.1640625" customWidth="1"/>
+    <col min="90" max="92" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="12.1640625" customWidth="1"/>
+    <col min="94" max="99" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="100" max="101" width="11.1640625" customWidth="1"/>
+    <col min="102" max="105" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="11.1640625" customWidth="1"/>
+    <col min="107" max="121" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -57147,6 +57333,10 @@
       <c r="J2" t="s">
         <v>209</v>
       </c>
+      <c r="K2">
+        <f>G2-F2</f>
+        <v>949.70690703299999</v>
+      </c>
       <c r="M2" s="6" t="s">
         <v>6</v>
       </c>
@@ -57160,7 +57350,7 @@
         <v>241</v>
       </c>
       <c r="Q2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -57194,20 +57384,24 @@
       <c r="J3" t="s">
         <v>209</v>
       </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K38" si="0">G3-F3</f>
+        <v>933.88354111000035</v>
+      </c>
       <c r="M3" s="8" t="s">
         <v>209</v>
       </c>
       <c r="N3" s="7">
-        <v>4213.3201519145878</v>
+        <v>4095.9468792084353</v>
       </c>
       <c r="O3" s="7">
-        <v>7103.5192056943743</v>
+        <v>7460.708391124117</v>
       </c>
       <c r="P3" s="7">
-        <v>7781.5717411190963</v>
+        <v>7550.0003534453308</v>
       </c>
       <c r="Q3" s="7">
-        <v>11737.629932731457</v>
+        <v>4391.7173146591558</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -57241,6 +57435,10 @@
       <c r="J4" t="s">
         <v>209</v>
       </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>959.59429502199998</v>
+      </c>
       <c r="M4" s="9">
         <v>1</v>
       </c>
@@ -57288,6 +57486,10 @@
       <c r="J5" t="s">
         <v>209</v>
       </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>1034.250431057</v>
+      </c>
       <c r="M5" s="9">
         <v>2</v>
       </c>
@@ -57301,7 +57503,7 @@
         <v>1409.4327398100197</v>
       </c>
       <c r="Q5" s="7">
-        <v>1391.2524913694263</v>
+        <v>18.180248440583544</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -57335,6 +57537,10 @@
       <c r="J6" t="s">
         <v>209</v>
       </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>1010.0245790499998</v>
+      </c>
       <c r="M6" s="9">
         <v>4</v>
       </c>
@@ -57348,7 +57554,7 @@
         <v>1702.0734024837227</v>
       </c>
       <c r="Q6" s="7">
-        <v>1684.9431382495509</v>
+        <v>17.130264234172852</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -57382,6 +57588,10 @@
       <c r="J7" t="s">
         <v>209</v>
       </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>1079.8288621861002</v>
+      </c>
       <c r="M7" s="9">
         <v>8</v>
       </c>
@@ -57395,7 +57605,7 @@
         <v>1409.7868230588144</v>
       </c>
       <c r="Q7" s="7">
-        <v>1407.2262046804303</v>
+        <v>31.231927623246943</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -57429,6 +57639,10 @@
       <c r="J8" t="s">
         <v>209</v>
       </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>1141.9783539744999</v>
+      </c>
       <c r="M8" s="9">
         <v>16</v>
       </c>
@@ -57442,7 +57656,7 @@
         <v>905.46192606435238</v>
       </c>
       <c r="Q8" s="7">
-        <v>760.91632799463173</v>
+        <v>144.69891001839824</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -57476,6 +57690,10 @@
       <c r="J9" t="s">
         <v>209</v>
       </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>1105.48323798</v>
+      </c>
       <c r="M9" s="9">
         <v>32</v>
       </c>
@@ -57489,7 +57707,7 @@
         <v>655.47536490629079</v>
       </c>
       <c r="Q9" s="7">
-        <v>568.90701584762792</v>
+        <v>686.57871472440843</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -57523,20 +57741,24 @@
       <c r="J10" t="s">
         <v>209</v>
       </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>1635.4789931739999</v>
+      </c>
       <c r="M10" s="9">
         <v>128</v>
       </c>
       <c r="N10" s="7">
-        <v>23963.5518376</v>
+        <v>16715.026063703332</v>
       </c>
       <c r="O10" s="7">
-        <v>37041.452272099996</v>
+        <v>29086.213300733332</v>
       </c>
       <c r="P10" s="7">
-        <v>1690.5742869471997</v>
+        <v>12611.597773255229</v>
       </c>
       <c r="Q10" s="7">
-        <v>411.80864029044022</v>
+        <v>1925.7044468981521</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -57570,20 +57792,24 @@
       <c r="J11" t="s">
         <v>209</v>
       </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>1408.5234179499998</v>
+      </c>
       <c r="M11" s="8" t="s">
         <v>225</v>
       </c>
       <c r="N11" s="7">
-        <v>7512.7633737037795</v>
+        <v>21.005163240430001</v>
       </c>
       <c r="O11" s="7">
-        <v>27702.241021633334</v>
+        <v>12768.35337882</v>
       </c>
       <c r="P11" s="7">
-        <v>13003.486282235632</v>
+        <v>21.43066278269054</v>
       </c>
       <c r="Q11" s="7">
-        <v>17666.539438637141</v>
+        <v>5649.9025447833619</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -57617,20 +57843,24 @@
       <c r="J12" t="s">
         <v>209</v>
       </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>1366.4965469900001</v>
+      </c>
       <c r="M12" s="9">
         <v>128</v>
       </c>
       <c r="N12" s="7">
-        <v>7512.7633737037795</v>
+        <v>21.005163240430001</v>
       </c>
       <c r="O12" s="7">
-        <v>27702.241021633334</v>
+        <v>12768.35337882</v>
       </c>
       <c r="P12" s="7">
-        <v>13003.486282235632</v>
+        <v>21.43066278269054</v>
       </c>
       <c r="Q12" s="7">
-        <v>17666.539438637141</v>
+        <v>5649.9025447833619</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -57664,6 +57894,10 @@
       <c r="J13" t="s">
         <v>209</v>
       </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>3280.1019890300004</v>
+      </c>
       <c r="M13" s="8" t="s">
         <v>227</v>
       </c>
@@ -57677,7 +57911,7 @@
         <v>835.04325782913259</v>
       </c>
       <c r="Q13" s="7">
-        <v>964.81053255030292</v>
+        <v>510.40194744237772</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -57711,6 +57945,10 @@
       <c r="J14" t="s">
         <v>209</v>
       </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>2100.0810089100005</v>
+      </c>
       <c r="M14" s="9">
         <v>2</v>
       </c>
@@ -57724,7 +57962,7 @@
         <v>111.92309133969361</v>
       </c>
       <c r="Q14" s="7">
-        <v>111.54666378357351</v>
+        <v>8.2639463793082282</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -57758,6 +57996,10 @@
       <c r="J15" t="s">
         <v>209</v>
       </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>2081.9518280099996</v>
+      </c>
       <c r="M15" s="9">
         <v>4</v>
       </c>
@@ -57771,7 +58013,7 @@
         <v>105.58209255030104</v>
       </c>
       <c r="Q15" s="7">
-        <v>111.60380077207761</v>
+        <v>11.067751088641248</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -57805,6 +58047,10 @@
       <c r="J16" t="s">
         <v>209</v>
       </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>14564.509658999996</v>
+      </c>
       <c r="M16" s="9">
         <v>8</v>
       </c>
@@ -57818,7 +58064,7 @@
         <v>934.53259658128707</v>
       </c>
       <c r="Q16" s="7">
-        <v>867.62424098636143</v>
+        <v>185.29553742458853</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -57826,7 +58072,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C17" s="13">
         <v>128</v>
@@ -57852,6 +58098,10 @@
       <c r="J17" s="13" t="s">
         <v>209</v>
       </c>
+      <c r="K17">
+        <f t="shared" si="0"/>
+        <v>11591.291210000003</v>
+      </c>
       <c r="M17" s="9">
         <v>16</v>
       </c>
@@ -57865,7 +58115,7 @@
         <v>1606.2643845303401</v>
       </c>
       <c r="Q17" s="7">
-        <v>1609.9533356902239</v>
+        <v>6.796511022181404</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -57873,7 +58123,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C18">
         <v>128</v>
@@ -57896,8 +58146,12 @@
       <c r="I18" t="s">
         <v>208</v>
       </c>
-      <c r="J18" t="s">
-        <v>269</v>
+      <c r="J18" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="0"/>
+        <v>10957.76084209</v>
       </c>
       <c r="M18" s="9">
         <v>32</v>
@@ -57912,15 +58166,15 @@
         <v>246.47106588965303</v>
       </c>
       <c r="Q18" s="7">
-        <v>363.91520409152037</v>
+        <v>610.38626998117275</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>224</v>
+        <v>263</v>
       </c>
       <c r="C19">
         <v>128</v>
@@ -57932,13 +58186,13 @@
         <v>128</v>
       </c>
       <c r="F19">
-        <v>22527.895972999999</v>
+        <v>5.7084000110600002</v>
       </c>
       <c r="G19">
-        <v>47417.862745999999</v>
+        <v>22380.652238800001</v>
       </c>
       <c r="H19">
-        <v>47419.311981899999</v>
+        <v>22382.094851999998</v>
       </c>
       <c r="I19" t="s">
         <v>208</v>
@@ -57946,25 +58200,29 @@
       <c r="J19" t="s">
         <v>225</v>
       </c>
+      <c r="K19">
+        <f>G19-F19</f>
+        <v>22374.943838788942</v>
+      </c>
       <c r="M19" s="8" t="s">
-        <v>269</v>
+        <v>8</v>
       </c>
       <c r="N19" s="7">
-        <v>2217.9745159099998</v>
+        <v>2123.2414277081321</v>
       </c>
       <c r="O19" s="7">
-        <v>13175.735358</v>
-      </c>
-      <c r="P19" s="7" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q19" s="7" t="e">
-        <v>#DIV/0!</v>
+        <v>5869.7644347304713</v>
+      </c>
+      <c r="P19" s="7">
+        <v>5469.9900497245644</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>5218.5712707667744</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>264</v>
@@ -57979,13 +58237,13 @@
         <v>128</v>
       </c>
       <c r="F20">
-        <v>5.7084000110600002</v>
+        <v>4.6857481002799997</v>
       </c>
       <c r="G20">
-        <v>22380.652238800001</v>
+        <v>13308.208080099999</v>
       </c>
       <c r="H20">
-        <v>22382.094851999998</v>
+        <v>13309.640333200001</v>
       </c>
       <c r="I20" t="s">
         <v>208</v>
@@ -57993,28 +58251,17 @@
       <c r="J20" t="s">
         <v>225</v>
       </c>
-      <c r="M20" s="9">
-        <v>128</v>
-      </c>
-      <c r="N20" s="7">
-        <v>2217.9745159099998</v>
-      </c>
-      <c r="O20" s="7">
-        <v>13175.735358</v>
-      </c>
-      <c r="P20" s="7" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q20" s="7" t="e">
-        <v>#DIV/0!</v>
+      <c r="K20">
+        <f>G20-F20</f>
+        <v>13303.522331999719</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="C21">
         <v>128</v>
@@ -58026,13 +58273,13 @@
         <v>128</v>
       </c>
       <c r="F21">
-        <v>4.6857481002799997</v>
+        <v>6.1047720909100001</v>
       </c>
       <c r="G21">
-        <v>13308.208080099999</v>
+        <v>9601.0439431699997</v>
       </c>
       <c r="H21">
-        <v>13309.640333200001</v>
+        <v>9602.4777331400001</v>
       </c>
       <c r="I21" t="s">
         <v>208</v>
@@ -58040,92 +58287,89 @@
       <c r="J21" t="s">
         <v>225</v>
       </c>
-      <c r="M21" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="N21" s="7">
-        <v>2907.9398736000571</v>
-      </c>
-      <c r="O21" s="7">
-        <v>6781.6610535616774</v>
-      </c>
-      <c r="P21" s="7">
-        <v>6581.6905391689634</v>
-      </c>
-      <c r="Q21" s="7">
-        <v>11616.116007390918</v>
+      <c r="K21">
+        <f>G21-F21</f>
+        <v>9594.9391710790896</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>226</v>
+        <v>285</v>
       </c>
       <c r="C22">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D22">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="F22">
-        <v>300.654438019</v>
+        <v>48.316945076000003</v>
       </c>
       <c r="G22">
-        <v>934.00202012099999</v>
+        <v>9398.2399060700009</v>
       </c>
       <c r="H22">
-        <v>935.09974002800004</v>
+        <v>9399.7276799699994</v>
       </c>
       <c r="I22" t="s">
         <v>208</v>
       </c>
       <c r="J22" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+      <c r="K22">
+        <f>G22-F22</f>
+        <v>9349.9229609940012</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>286</v>
       </c>
       <c r="C23">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D23">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="F23">
-        <v>113.3769629</v>
+        <v>40.209950923900003</v>
       </c>
       <c r="G23">
-        <v>756.88640379900005</v>
+        <v>9153.62272596</v>
       </c>
       <c r="H23">
-        <v>758.091012955</v>
+        <v>9154.9730839700005</v>
       </c>
       <c r="I23" t="s">
         <v>208</v>
       </c>
       <c r="J23" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+      <c r="K23">
+        <f>G23-F23</f>
+        <v>9113.4127750361004</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C24">
         <v>12</v>
@@ -58137,13 +58381,13 @@
         <v>2</v>
       </c>
       <c r="F24">
-        <v>100.828622103</v>
+        <v>300.654438019</v>
       </c>
       <c r="G24">
-        <v>727.96860408800001</v>
+        <v>934.00202012099999</v>
       </c>
       <c r="H24">
-        <v>729.173197985</v>
+        <v>935.09974002800004</v>
       </c>
       <c r="I24" t="s">
         <v>208</v>
@@ -58151,13 +58395,17 @@
       <c r="J24" t="s">
         <v>227</v>
       </c>
+      <c r="K24">
+        <f>G24-F24</f>
+        <v>633.34758210199993</v>
+      </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C25">
         <v>12</v>
@@ -58166,16 +58414,16 @@
         <v>12</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25">
-        <v>252.339545012</v>
+        <v>113.3769629</v>
       </c>
       <c r="G25">
-        <v>927.508314133</v>
+        <v>756.88640379900005</v>
       </c>
       <c r="H25">
-        <v>928.868350029</v>
+        <v>758.091012955</v>
       </c>
       <c r="I25" t="s">
         <v>208</v>
@@ -58183,13 +58431,17 @@
       <c r="J25" t="s">
         <v>227</v>
       </c>
+      <c r="K25">
+        <f>G25-F25</f>
+        <v>643.50944089900008</v>
+      </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C26">
         <v>12</v>
@@ -58198,16 +58450,16 @@
         <v>12</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F26">
-        <v>220.36070990600001</v>
+        <v>100.828622103</v>
       </c>
       <c r="G26">
-        <v>912.68654990200002</v>
+        <v>727.96860408800001</v>
       </c>
       <c r="H26">
-        <v>913.90338492399997</v>
+        <v>729.173197985</v>
       </c>
       <c r="I26" t="s">
         <v>208</v>
@@ -58215,13 +58467,17 @@
       <c r="J26" t="s">
         <v>227</v>
       </c>
+      <c r="K26">
+        <f>G26-F26</f>
+        <v>627.13998198499996</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C27">
         <v>12</v>
@@ -58233,13 +58489,13 @@
         <v>4</v>
       </c>
       <c r="F27">
-        <v>55.585777044300002</v>
+        <v>252.339545012</v>
       </c>
       <c r="G27">
-        <v>727.22062802300002</v>
+        <v>927.508314133</v>
       </c>
       <c r="H27">
-        <v>728.41032099699999</v>
+        <v>928.868350029</v>
       </c>
       <c r="I27" t="s">
         <v>208</v>
@@ -58247,13 +58503,17 @@
       <c r="J27" t="s">
         <v>227</v>
       </c>
+      <c r="K27">
+        <f>G27-F27</f>
+        <v>675.16876912099997</v>
+      </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C28">
         <v>12</v>
@@ -58262,16 +58522,16 @@
         <v>12</v>
       </c>
       <c r="E28">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F28">
-        <v>1703.66234207</v>
+        <v>220.36070990600001</v>
       </c>
       <c r="G28">
-        <v>2510.5651390600001</v>
+        <v>912.68654990200002</v>
       </c>
       <c r="H28">
-        <v>2511.7870490599998</v>
+        <v>913.90338492399997</v>
       </c>
       <c r="I28" t="s">
         <v>208</v>
@@ -58279,13 +58539,17 @@
       <c r="J28" t="s">
         <v>227</v>
       </c>
+      <c r="K28">
+        <f>G28-F28</f>
+        <v>692.32583999600001</v>
+      </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C29">
         <v>12</v>
@@ -58294,16 +58558,16 @@
         <v>12</v>
       </c>
       <c r="E29">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F29">
-        <v>90.235594987900001</v>
+        <v>55.585777044300002</v>
       </c>
       <c r="G29">
-        <v>1207.55374312</v>
+        <v>727.22062802300002</v>
       </c>
       <c r="H29">
-        <v>1208.7523281599999</v>
+        <v>728.41032099699999</v>
       </c>
       <c r="I29" t="s">
         <v>208</v>
@@ -58311,13 +58575,17 @@
       <c r="J29" t="s">
         <v>227</v>
       </c>
+      <c r="K29">
+        <f>G29-F29</f>
+        <v>671.6348509787</v>
+      </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C30">
         <v>12</v>
@@ -58329,13 +58597,13 @@
         <v>8</v>
       </c>
       <c r="F30">
-        <v>79.823445081700001</v>
+        <v>1703.66234207</v>
       </c>
       <c r="G30">
-        <v>866.61979699100004</v>
+        <v>2510.5651390600001</v>
       </c>
       <c r="H30">
-        <v>867.81867504100001</v>
+        <v>2511.7870490599998</v>
       </c>
       <c r="I30" t="s">
         <v>208</v>
@@ -58343,31 +58611,44 @@
       <c r="J30" t="s">
         <v>227</v>
       </c>
+      <c r="K30">
+        <f>G30-F30</f>
+        <v>806.90279699000007</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C31">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D31">
         <v>12</v>
       </c>
       <c r="E31">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F31">
-        <v>263.91831493400002</v>
+        <v>90.235594987900001</v>
       </c>
       <c r="G31">
-        <v>1318.27436304</v>
+        <v>1207.55374312</v>
       </c>
       <c r="H31">
-        <v>1319.4774529900001</v>
+        <v>1208.7523281599999</v>
       </c>
       <c r="I31" t="s">
         <v>208</v>
@@ -58375,31 +58656,44 @@
       <c r="J31" t="s">
         <v>227</v>
       </c>
+      <c r="K31">
+        <f>G31-F31</f>
+        <v>1117.3181481321001</v>
+      </c>
+      <c r="M31" t="s">
+        <v>5</v>
+      </c>
+      <c r="N31">
+        <v>5192</v>
+      </c>
+      <c r="O31">
+        <v>2879</v>
+      </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C32">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D32">
         <v>12</v>
       </c>
       <c r="E32">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F32">
-        <v>141.600160837</v>
+        <v>79.823445081700001</v>
       </c>
       <c r="G32">
-        <v>1207.09737587</v>
+        <v>866.61979699100004</v>
       </c>
       <c r="H32">
-        <v>1208.20039296</v>
+        <v>867.81867504100001</v>
       </c>
       <c r="I32" t="s">
         <v>208</v>
@@ -58407,13 +58701,26 @@
       <c r="J32" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32">
+        <f>G32-F32</f>
+        <v>786.79635190930003</v>
+      </c>
+      <c r="M32" t="s">
+        <v>5</v>
+      </c>
+      <c r="N32">
+        <v>4844</v>
+      </c>
+      <c r="O32">
+        <v>2864</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C33">
         <v>24</v>
@@ -58425,13 +58732,13 @@
         <v>16</v>
       </c>
       <c r="F33">
-        <v>2982.8733580100002</v>
+        <v>263.91831493400002</v>
       </c>
       <c r="G33">
-        <v>4049.5441341400001</v>
+        <v>1318.27436304</v>
       </c>
       <c r="H33">
-        <v>4050.7455921199999</v>
+        <v>1319.4774529900001</v>
       </c>
       <c r="I33" t="s">
         <v>208</v>
@@ -58439,31 +58746,44 @@
       <c r="J33" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33">
+        <f>G33-F33</f>
+        <v>1054.3560481059999</v>
+      </c>
+      <c r="M33" t="s">
+        <v>5</v>
+      </c>
+      <c r="N33">
+        <v>4812</v>
+      </c>
+      <c r="O33">
+        <v>2784</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C34">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D34">
         <v>12</v>
       </c>
       <c r="E34">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F34">
-        <v>23.373319864300001</v>
+        <v>141.600160837</v>
       </c>
       <c r="G34">
-        <v>2503.21842599</v>
+        <v>1207.09737587</v>
       </c>
       <c r="H34">
-        <v>2504.4764480600002</v>
+        <v>1208.20039296</v>
       </c>
       <c r="I34" t="s">
         <v>208</v>
@@ -58471,37 +58791,381 @@
       <c r="J34" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34">
+        <f>G34-F34</f>
+        <v>1065.497215033</v>
+      </c>
+      <c r="M34" t="s">
+        <v>5</v>
+      </c>
+      <c r="N34" s="65">
+        <v>19192</v>
+      </c>
+      <c r="O34" s="65">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C35">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D35">
         <v>12</v>
       </c>
       <c r="E35">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F35">
-        <v>371.93604397799999</v>
+        <v>2982.8733580100002</v>
       </c>
       <c r="G35">
-        <v>1988.56460881</v>
+        <v>4049.5441341400001</v>
       </c>
       <c r="H35">
-        <v>1989.9456028899999</v>
+        <v>4050.7455921199999</v>
       </c>
       <c r="I35" t="s">
         <v>208</v>
       </c>
       <c r="J35" t="s">
         <v>227</v>
+      </c>
+      <c r="K35">
+        <f>G35-F35</f>
+        <v>1066.6707761299999</v>
+      </c>
+      <c r="M35" t="s">
+        <v>5</v>
+      </c>
+      <c r="N35" s="65">
+        <v>10262</v>
+      </c>
+      <c r="O35" s="65">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>239</v>
+      </c>
+      <c r="C36">
+        <v>36</v>
+      </c>
+      <c r="D36">
+        <v>12</v>
+      </c>
+      <c r="E36">
+        <v>32</v>
+      </c>
+      <c r="F36">
+        <v>23.373319864300001</v>
+      </c>
+      <c r="G36">
+        <v>2503.21842599</v>
+      </c>
+      <c r="H36">
+        <v>2504.4764480600002</v>
+      </c>
+      <c r="I36" t="s">
+        <v>208</v>
+      </c>
+      <c r="J36" t="s">
+        <v>227</v>
+      </c>
+      <c r="K36">
+        <f>G36-F36</f>
+        <v>2479.8451061257001</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="N36" s="2">
+        <f>AVERAGE(N31:N35)</f>
+        <v>8860.4</v>
+      </c>
+      <c r="O36" s="2">
+        <f>AVERAGE(O31:O35)</f>
+        <v>2598.8000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>240</v>
+      </c>
+      <c r="C37">
+        <v>36</v>
+      </c>
+      <c r="D37">
+        <v>12</v>
+      </c>
+      <c r="E37">
+        <v>32</v>
+      </c>
+      <c r="F37">
+        <v>371.93604397799999</v>
+      </c>
+      <c r="G37">
+        <v>1988.56460881</v>
+      </c>
+      <c r="H37">
+        <v>1989.9456028899999</v>
+      </c>
+      <c r="I37" t="s">
+        <v>208</v>
+      </c>
+      <c r="J37" t="s">
+        <v>227</v>
+      </c>
+      <c r="K37">
+        <f>G37-F37</f>
+        <v>1616.6285648319999</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="N37" s="52">
+        <f>STDEV(N31:N35)</f>
+        <v>6218.6134145804563</v>
+      </c>
+      <c r="O37" s="52">
+        <f>STDEV(O31:O35)</f>
+        <v>338.900722926345</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" t="s">
+        <v>20</v>
+      </c>
+      <c r="F62" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" t="s">
+        <v>22</v>
+      </c>
+      <c r="H62" t="s">
+        <v>23</v>
+      </c>
+      <c r="I62" t="s">
+        <v>24</v>
+      </c>
+      <c r="J62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>224</v>
+      </c>
+      <c r="C63">
+        <v>128</v>
+      </c>
+      <c r="D63">
+        <v>8</v>
+      </c>
+      <c r="E63">
+        <v>128</v>
+      </c>
+      <c r="F63">
+        <v>22527.895972999999</v>
+      </c>
+      <c r="G63">
+        <v>47417.862745999999</v>
+      </c>
+      <c r="H63">
+        <v>47419.311981899999</v>
+      </c>
+      <c r="I63" t="s">
+        <v>208</v>
+      </c>
+      <c r="J63" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64">
+        <v>128</v>
+      </c>
+      <c r="D64">
+        <v>8</v>
+      </c>
+      <c r="E64">
+        <v>128</v>
+      </c>
+      <c r="F64">
+        <v>5.7084000110600002</v>
+      </c>
+      <c r="G64">
+        <v>22380.652238800001</v>
+      </c>
+      <c r="H64">
+        <v>22382.094851999998</v>
+      </c>
+      <c r="I64" t="s">
+        <v>208</v>
+      </c>
+      <c r="J64" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>264</v>
+      </c>
+      <c r="C65">
+        <v>128</v>
+      </c>
+      <c r="D65">
+        <v>8</v>
+      </c>
+      <c r="E65">
+        <v>128</v>
+      </c>
+      <c r="F65">
+        <v>4.6857481002799997</v>
+      </c>
+      <c r="G65">
+        <v>13308.208080099999</v>
+      </c>
+      <c r="H65">
+        <v>13309.640333200001</v>
+      </c>
+      <c r="I65" t="s">
+        <v>208</v>
+      </c>
+      <c r="J65" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68">
+        <v>0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>284</v>
+      </c>
+      <c r="C68">
+        <v>128</v>
+      </c>
+      <c r="D68">
+        <v>8</v>
+      </c>
+      <c r="E68">
+        <v>128</v>
+      </c>
+      <c r="F68">
+        <v>6.1047720909100001</v>
+      </c>
+      <c r="G68">
+        <v>9601.0439431699997</v>
+      </c>
+      <c r="H68">
+        <v>9602.4777331400001</v>
+      </c>
+      <c r="I68" t="s">
+        <v>208</v>
+      </c>
+      <c r="J68" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>285</v>
+      </c>
+      <c r="C69">
+        <v>128</v>
+      </c>
+      <c r="D69">
+        <v>8</v>
+      </c>
+      <c r="E69">
+        <v>128</v>
+      </c>
+      <c r="F69">
+        <v>48.316945076000003</v>
+      </c>
+      <c r="G69">
+        <v>9398.2399060700009</v>
+      </c>
+      <c r="H69">
+        <v>9399.7276799699994</v>
+      </c>
+      <c r="I69" t="s">
+        <v>208</v>
+      </c>
+      <c r="J69" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
+        <v>286</v>
+      </c>
+      <c r="C70">
+        <v>128</v>
+      </c>
+      <c r="D70">
+        <v>8</v>
+      </c>
+      <c r="E70">
+        <v>128</v>
+      </c>
+      <c r="F70">
+        <v>40.209950923900003</v>
+      </c>
+      <c r="G70">
+        <v>9153.62272596</v>
+      </c>
+      <c r="H70">
+        <v>9154.9730839700005</v>
+      </c>
+      <c r="I70" t="s">
+        <v>208</v>
+      </c>
+      <c r="J70" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -58578,7 +59242,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C2">
         <v>32</v>
@@ -58602,7 +59266,7 @@
         <v>208</v>
       </c>
       <c r="J2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>9</v>
@@ -58613,7 +59277,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C3">
         <v>32</v>
@@ -58637,16 +59301,16 @@
         <v>208</v>
       </c>
       <c r="J3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="N3" t="s">
+        <v>258</v>
+      </c>
+      <c r="O3" t="s">
         <v>259</v>
-      </c>
-      <c r="O3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -58654,7 +59318,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C4">
         <v>32</v>
@@ -58695,7 +59359,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C5">
         <v>32</v>
@@ -58736,7 +59400,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C6">
         <v>32</v>
@@ -58760,7 +59424,7 @@
         <v>208</v>
       </c>
       <c r="J6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M6" s="8">
         <v>2</v>
@@ -58777,7 +59441,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C7">
         <v>32</v>
@@ -58801,7 +59465,7 @@
         <v>208</v>
       </c>
       <c r="J7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>8</v>
@@ -58818,7 +59482,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C8">
         <v>32</v>
@@ -58845,13 +59509,13 @@
         <v>225</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="N8" s="54">
+        <v>260</v>
+      </c>
+      <c r="N8" s="52">
         <f>AVERAGE(N4:N6)</f>
         <v>330.21324467653335</v>
       </c>
-      <c r="O8" s="54">
+      <c r="O8" s="52">
         <f>AVERAGE(O4:O6)</f>
         <v>8733.732693349999</v>
       </c>
@@ -58861,7 +59525,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C9">
         <v>32</v>
@@ -58904,7 +59568,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C10">
         <v>32</v>
@@ -58928,7 +59592,7 @@
         <v>208</v>
       </c>
       <c r="J10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -58936,7 +59600,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C11">
         <v>32</v>
@@ -58960,7 +59624,7 @@
         <v>208</v>
       </c>
       <c r="J11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -58968,7 +59632,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C12">
         <v>32</v>
@@ -59000,7 +59664,7 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C13">
         <v>32</v>
@@ -59029,10 +59693,10 @@
     </row>
     <row r="15" spans="1:15">
       <c r="N15" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -59076,23 +59740,23 @@
       </c>
     </row>
     <row r="21" spans="13:15" ht="16" thickBot="1">
-      <c r="M21" s="55"/>
-      <c r="N21" s="56">
+      <c r="M21" s="53"/>
+      <c r="N21" s="54">
         <v>6234.875</v>
       </c>
-      <c r="O21" s="56">
+      <c r="O21" s="54">
         <v>1280.515625</v>
       </c>
     </row>
     <row r="22" spans="13:15" ht="16" thickTop="1">
       <c r="M22" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="N22" s="54">
+        <v>260</v>
+      </c>
+      <c r="N22" s="52">
         <f>AVERAGE(N16:N21)</f>
         <v>6929.617033333333</v>
       </c>
-      <c r="O22" s="54">
+      <c r="O22" s="52">
         <f>AVERAGE(O16:O21)</f>
         <v>1152.9166666666667</v>
       </c>
@@ -59101,11 +59765,11 @@
       <c r="M23" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N23" s="54">
+      <c r="N23" s="52">
         <f>STDEV(N16:N21)</f>
         <v>1220.3487605097328</v>
       </c>
-      <c r="O23" s="54">
+      <c r="O23" s="52">
         <f>STDEV(O16:O21)</f>
         <v>140.23939620769141</v>
       </c>
@@ -59677,8 +60341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="O112" sqref="O112"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -59697,16 +60361,14 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2"/>
-      <c r="G2" s="51" t="s">
-        <v>245</v>
-      </c>
+      <c r="G2" s="50"/>
       <c r="K2" s="2" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="F3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="30">
@@ -59718,19 +60380,19 @@
         <v>153</v>
       </c>
       <c r="D4" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>275</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>276</v>
-      </c>
-      <c r="F4" s="18" t="s">
+      <c r="G4" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="H4" s="59" t="s">
         <v>274</v>
-      </c>
-      <c r="H4" s="66" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -59755,11 +60417,11 @@
       </c>
       <c r="F5" s="20">
         <f>'BJ w Staging'!N10</f>
-        <v>23963.5518376</v>
+        <v>16715.026063703332</v>
       </c>
       <c r="G5" s="35">
         <f>'BJ w Staging'!N12</f>
-        <v>7512.7633737037795</v>
+        <v>21.005163240430001</v>
       </c>
       <c r="H5" s="20">
         <f>'BJ (FG multi)'!N8</f>
@@ -59787,10 +60449,11 @@
       <c r="F6" s="47">
         <v>11460.578475336322</v>
       </c>
-      <c r="G6" s="50">
-        <v>14727</v>
-      </c>
-      <c r="H6" s="57">
+      <c r="G6" s="67">
+        <f>'BJ w Staging'!N36</f>
+        <v>8860.4</v>
+      </c>
+      <c r="H6" s="55">
         <f>'BJ (FG multi)'!N22</f>
         <v>6929.617033333333</v>
       </c>
@@ -59818,10 +60481,11 @@
       <c r="F7" s="21">
         <v>906</v>
       </c>
-      <c r="G7" s="52">
-        <v>2233.5</v>
-      </c>
-      <c r="H7" s="58">
+      <c r="G7" s="66">
+        <f>'BJ w Staging'!O36</f>
+        <v>2598.8000000000002</v>
+      </c>
+      <c r="H7" s="56">
         <f>'BJ (FG multi)'!O22</f>
         <v>1152.9166666666667</v>
       </c>
@@ -59848,11 +60512,11 @@
       </c>
       <c r="F8" s="21">
         <f>'BJ w Staging'!O10</f>
-        <v>37041.452272099996</v>
+        <v>29086.213300733332</v>
       </c>
       <c r="G8" s="37">
         <f>'BJ w Staging'!O12</f>
-        <v>27702.241021633334</v>
+        <v>12768.35337882</v>
       </c>
       <c r="H8" s="21">
         <f>'BJ (FG multi)'!O8</f>
@@ -59884,7 +60548,7 @@
       </c>
       <c r="G9" s="37">
         <f>'BJ w Staging'!Q12</f>
-        <v>17666.539438637141</v>
+        <v>5649.9025447833619</v>
       </c>
       <c r="H9" s="21">
         <f>'BJ (FG multi)'!O9</f>
@@ -59934,13 +60598,13 @@
       </c>
       <c r="F12" s="21">
         <f t="shared" ref="F12:G12" si="1">F5/60</f>
-        <v>399.39253062666666</v>
+        <v>278.58376772838886</v>
       </c>
       <c r="G12" s="37">
         <f t="shared" si="1"/>
-        <v>125.212722895063</v>
-      </c>
-      <c r="H12" s="59">
+        <v>0.35008605400716669</v>
+      </c>
+      <c r="H12" s="57">
         <f t="shared" ref="H12" si="2">H5/60</f>
         <v>5.5035540779422227</v>
       </c>
@@ -59971,7 +60635,7 @@
       </c>
       <c r="G13" s="36">
         <f t="shared" si="3"/>
-        <v>245.45</v>
+        <v>147.67333333333332</v>
       </c>
       <c r="H13" s="30">
         <f t="shared" ref="H13" si="4">H6/60</f>
@@ -60000,11 +60664,11 @@
       </c>
       <c r="F14" s="21">
         <f>F19-F16-F12-F13</f>
-        <v>11.855365986061173</v>
+        <v>7.6812694894584865E-2</v>
       </c>
       <c r="G14" s="37">
         <f t="shared" ref="G14:H14" si="5">G19-G16-G12-G13</f>
-        <v>53.816294132159214</v>
+        <v>21.4691369263262</v>
       </c>
       <c r="H14" s="21">
         <f t="shared" si="5"/>
@@ -60033,11 +60697,11 @@
       </c>
       <c r="F15" s="21">
         <f t="shared" ref="F15:H15" si="6">F12+F14</f>
-        <v>411.2478966127278</v>
+        <v>278.66058042328348</v>
       </c>
       <c r="G15" s="37">
         <f t="shared" si="6"/>
-        <v>179.02901702722221</v>
+        <v>21.819222980333368</v>
       </c>
       <c r="H15" s="21">
         <f t="shared" si="6"/>
@@ -60070,7 +60734,7 @@
       </c>
       <c r="G16" s="37">
         <f t="shared" si="7"/>
-        <v>37.225000000000001</v>
+        <v>43.31333333333334</v>
       </c>
       <c r="H16" s="21">
         <f t="shared" ref="H16" si="8">H7/60</f>
@@ -60099,11 +60763,11 @@
       </c>
       <c r="F17" s="21">
         <f>F19-F12-F13</f>
-        <v>26.955365986061196</v>
+        <v>15.176812694894608</v>
       </c>
       <c r="G17" s="37">
         <f t="shared" si="9"/>
-        <v>91.041294132159237</v>
+        <v>64.782470259659533</v>
       </c>
       <c r="H17" s="21">
         <f t="shared" si="9"/>
@@ -60112,7 +60776,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B18" s="21">
         <f>B17-B16</f>
@@ -60132,11 +60796,11 @@
       </c>
       <c r="F18" s="21">
         <f t="shared" si="10"/>
-        <v>11.855365986061196</v>
+        <v>7.6812694894607958E-2</v>
       </c>
       <c r="G18" s="21">
         <f t="shared" si="10"/>
-        <v>53.816294132159236</v>
+        <v>21.469136926326193</v>
       </c>
       <c r="H18" s="21">
         <f t="shared" si="10"/>
@@ -60165,11 +60829,11 @@
       </c>
       <c r="F19" s="21">
         <f t="shared" si="11"/>
-        <v>617.35753786833322</v>
+        <v>484.77022167888884</v>
       </c>
       <c r="G19" s="37">
         <f t="shared" si="11"/>
-        <v>461.70401702722222</v>
+        <v>212.80588964700001</v>
       </c>
       <c r="H19" s="21">
         <f t="shared" si="11"/>
@@ -60202,7 +60866,7 @@
       </c>
       <c r="G20" s="37">
         <f t="shared" si="12"/>
-        <v>294.4423239772857</v>
+        <v>94.165042413056028</v>
       </c>
       <c r="H20" s="21">
         <f t="shared" ref="H20" si="13">H9/60</f>
@@ -60231,11 +60895,11 @@
       </c>
       <c r="F21" s="37">
         <f>F15+F16</f>
-        <v>426.34789661272782</v>
+        <v>293.7605804232835</v>
       </c>
       <c r="G21" s="37">
         <f>G15+G16</f>
-        <v>216.2540170272222</v>
+        <v>65.132556313666711</v>
       </c>
       <c r="H21" s="21">
         <f>H15+H16</f>
@@ -60264,11 +60928,11 @@
       </c>
       <c r="F22" s="37">
         <f t="shared" si="15"/>
-        <v>217.96500724166657</v>
+        <v>206.18645395049998</v>
       </c>
       <c r="G22" s="37">
         <f t="shared" si="15"/>
-        <v>336.49129413215923</v>
+        <v>212.45580359299285</v>
       </c>
       <c r="H22" s="21">
         <f t="shared" ref="H22" si="16">H19-H12</f>
@@ -60281,7 +60945,7 @@
       <c r="D23" s="31"/>
       <c r="E23" s="32"/>
       <c r="F23" s="32"/>
-      <c r="G23" s="53"/>
+      <c r="G23" s="51"/>
       <c r="H23" s="49"/>
     </row>
     <row r="24" spans="1:8" ht="16" thickBot="1">
@@ -60368,7 +61032,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B28">
         <f>B14/B19</f>
@@ -60388,11 +61052,11 @@
       </c>
       <c r="F28">
         <f t="shared" si="18"/>
-        <v>1.9203403633810692E-2</v>
+        <v>1.584517601525976E-4</v>
       </c>
       <c r="G28">
         <f t="shared" si="18"/>
-        <v>0.11656016007542379</v>
+        <v>0.10088600913226115</v>
       </c>
       <c r="H28">
         <f t="shared" si="18"/>
@@ -63416,7 +64080,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C2">
         <v>64</v>
@@ -63453,7 +64117,7 @@
         <v>119</v>
       </c>
       <c r="O2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -63461,7 +64125,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C3">
         <v>64</v>
@@ -63485,7 +64149,7 @@
         <v>208</v>
       </c>
       <c r="J3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K7" si="0">G3-F3</f>
@@ -63506,7 +64170,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C4">
         <v>64</v>
@@ -63537,7 +64201,7 @@
         <v>7735.1987621791004</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N4" s="7">
         <v>4741.915822668534</v>
@@ -63551,7 +64215,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C5">
         <v>64</v>
@@ -63575,7 +64239,7 @@
         <v>208</v>
       </c>
       <c r="J5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
@@ -63596,7 +64260,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C6">
         <v>64</v>
@@ -63632,7 +64296,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C7">
         <v>64</v>
@@ -63656,7 +64320,7 @@
         <v>208</v>
       </c>
       <c r="J7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
going through performance section making discussed changes
git-svn-id: file://localhost/tmp/svn2git/svn@7218 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="20560" tabRatio="500" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="50380" windowHeight="28360" tabRatio="500" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="299">
   <si>
     <t>bfast</t>
   </si>
@@ -1077,6 +1077,33 @@
   <si>
     <t>Mittel</t>
   </si>
+  <si>
+    <t>Time 1</t>
+  </si>
+  <si>
+    <t>Time 2</t>
+  </si>
+  <si>
+    <t>XSEDE:Trestles/FG</t>
+  </si>
+  <si>
+    <t>EGI/FG</t>
+  </si>
+  <si>
+    <t>XSEDE:QB/OSG</t>
+  </si>
+  <si>
+    <t>Stddev 1</t>
+  </si>
+  <si>
+    <t>Stddev 2</t>
+  </si>
+  <si>
+    <t>adjusted with staging 100 min (EU-US)</t>
+  </si>
+  <si>
+    <t>adjusted with staging 80 min (OSG-QB)</t>
+  </si>
 </sst>
 </file>
 
@@ -1359,8 +1386,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="157">
+  <cellStyleXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1620,7 +1677,7 @@
     <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="157">
+  <cellStyles count="187">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1699,6 +1756,21 @@
     <cellStyle name="Besuchter Link" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1777,6 +1849,21 @@
     <cellStyle name="Link" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
@@ -4061,7 +4148,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72.86479822088748</c:v>
+                  <c:v>49.85838554608952</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
                   <c:v>0.0</c:v>
@@ -4194,6 +4281,339 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="117"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="17"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Interop '!$P$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Interop '!$R$63:$R$65</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>20.13770928090607</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.887279534302993</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.983319421247957</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Interop '!$R$63:$R$65</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>20.13770928090607</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.887279534302993</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.983319421247957</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Interop '!$O$63:$O$65</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE:Trestles/FG</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EGI/FG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>XSEDE:QB/OSG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Interop '!$P$63:$P$65</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>79.03193037780891</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.86479822088748</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Interop '!$Q$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Interop '!$S$63:$S$65</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>21.99622082922189</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.22835916174973</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>21.8339710466664</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Interop '!$S$63:$S$65</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>21.99622082922189</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.22835916174973</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>21.8339710466664</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Interop '!$O$63:$O$65</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>XSEDE:Trestles/FG</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>EGI/FG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>XSEDE:QB/OSG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Interop '!$Q$63:$Q$65</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>107.6521406782717</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>123.006412674798</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117.3041666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2083983672"/>
+        <c:axId val="2081339752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2083983672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1">
+                <a:latin typeface="Times"/>
+                <a:cs typeface="Times"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2081339752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2081339752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800">
+                    <a:latin typeface="Times"/>
+                    <a:cs typeface="Times"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1800">
+                    <a:latin typeface="Times"/>
+                    <a:cs typeface="Times"/>
+                  </a:rPr>
+                  <a:t>Runtime (in min)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800">
+                <a:latin typeface="Times"/>
+                <a:cs typeface="Times"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2083983672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4435,6 +4855,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>1612900</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -52359,7 +52809,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -52579,7 +53029,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -52786,10 +53236,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="T66" sqref="T66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -53464,8 +53914,8 @@
         <v>0</v>
       </c>
       <c r="R16" s="38">
-        <f>'Interop EGI-FG'!P8/60</f>
-        <v>72.864798220887479</v>
+        <f>'Interop EGI-FG'!P8/60-P16</f>
+        <v>49.858385546089515</v>
       </c>
       <c r="S16">
         <v>0</v>
@@ -54019,6 +54469,99 @@
       <c r="J32" t="s">
         <v>47</v>
       </c>
+    </row>
+    <row r="62" spans="15:20">
+      <c r="P62" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>291</v>
+      </c>
+      <c r="R62" t="s">
+        <v>295</v>
+      </c>
+      <c r="S62" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="63" spans="15:20">
+      <c r="O63" t="s">
+        <v>292</v>
+      </c>
+      <c r="P63" s="16">
+        <f>'BJ (FG-XSEDE)'!N4/60</f>
+        <v>79.031930377808905</v>
+      </c>
+      <c r="Q63" s="47">
+        <f>'BJ (FG-XSEDE)'!N3/60</f>
+        <v>107.65214067827169</v>
+      </c>
+      <c r="R63" s="16">
+        <f>'BJ (FG-XSEDE)'!O4/60</f>
+        <v>20.137709280906069</v>
+      </c>
+      <c r="S63" s="16">
+        <f>'BJ (FG-XSEDE)'!O3/60</f>
+        <v>21.99622082922189</v>
+      </c>
+    </row>
+    <row r="64" spans="15:20">
+      <c r="O64" t="s">
+        <v>293</v>
+      </c>
+      <c r="P64" s="16">
+        <f>'Interop EGI-FG'!P8/60</f>
+        <v>72.864798220887479</v>
+      </c>
+      <c r="Q64" s="16">
+        <f>'Interop EGI-FG'!Q8/60+100</f>
+        <v>123.00641267479796</v>
+      </c>
+      <c r="R64" s="16">
+        <f>'Interop EGI-FG'!P9/60</f>
+        <v>5.8872795343029933</v>
+      </c>
+      <c r="S64" s="16">
+        <f>'Interop EGI-FG'!Q9/60</f>
+        <v>7.2283591617497303</v>
+      </c>
+      <c r="T64" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="65" spans="15:20">
+      <c r="O65" t="s">
+        <v>294</v>
+      </c>
+      <c r="P65" s="16">
+        <f>'Interop OSG-XSEDE'!F11/60</f>
+        <v>86.5</v>
+      </c>
+      <c r="Q65" s="16">
+        <f>'Interop OSG-XSEDE'!B11/60+80</f>
+        <v>117.30416666666667</v>
+      </c>
+      <c r="R65" s="16">
+        <f>'Interop OSG-XSEDE'!F12/60</f>
+        <v>9.9833194212479572</v>
+      </c>
+      <c r="S65" s="16">
+        <f>'Interop OSG-XSEDE'!B12/60</f>
+        <v>21.833971046666402</v>
+      </c>
+      <c r="T65" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="68" spans="15:20">
+      <c r="P68" s="15"/>
+      <c r="S68" s="16"/>
+    </row>
+    <row r="69" spans="15:20">
+      <c r="P69" s="15"/>
+    </row>
+    <row r="70" spans="15:20">
+      <c r="P70" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -60341,7 +60884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
typos and final data spreadsheets
git-svn-id: file://localhost/tmp/svn2git/svn@7301 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -42,8 +42,8 @@
     <pivotCache cacheId="3" r:id="rId17"/>
     <pivotCache cacheId="4" r:id="rId18"/>
     <pivotCache cacheId="5" r:id="rId19"/>
-    <pivotCache cacheId="7" r:id="rId20"/>
-    <pivotCache cacheId="28" r:id="rId21"/>
+    <pivotCache cacheId="6" r:id="rId20"/>
+    <pivotCache cacheId="7" r:id="rId21"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1658,6 +1658,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1673,9 +1676,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="187">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -1949,7 +1949,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2065,11 +2064,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2069539432"/>
-        <c:axId val="2069542392"/>
+        <c:axId val="2047437864"/>
+        <c:axId val="2047440888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2069539432"/>
+        <c:axId val="2047437864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2079,7 +2078,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069542392"/>
+        <c:crossAx val="2047440888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2087,7 +2086,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2069542392"/>
+        <c:axId val="2047440888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2098,7 +2097,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069539432"/>
+        <c:crossAx val="2047437864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2396,11 +2395,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2033532504"/>
-        <c:axId val="2033541304"/>
+        <c:axId val="2084449544"/>
+        <c:axId val="2083475400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2033532504"/>
+        <c:axId val="2084449544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2427,14 +2426,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2033541304"/>
+        <c:crossAx val="2083475400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2442,7 +2440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2033541304"/>
+        <c:axId val="2083475400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2453,7 +2451,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2033532504"/>
+        <c:crossAx val="2084449544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2765,11 +2763,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2069652056"/>
-        <c:axId val="2069657784"/>
+        <c:axId val="2082443384"/>
+        <c:axId val="2082449112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2069652056"/>
+        <c:axId val="2082443384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2802,7 +2800,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069657784"/>
+        <c:crossAx val="2082449112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2810,7 +2808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2069657784"/>
+        <c:axId val="2082449112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2839,7 +2837,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2069652056"/>
+        <c:crossAx val="2082443384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3105,11 +3103,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2070025576"/>
-        <c:axId val="2070019976"/>
+        <c:axId val="2076227000"/>
+        <c:axId val="2076893672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2070025576"/>
+        <c:axId val="2076227000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3131,7 +3129,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2070019976"/>
+        <c:crossAx val="2076893672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3139,7 +3137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2070019976"/>
+        <c:axId val="2076893672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -3196,7 +3194,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2070025576"/>
+        <c:crossAx val="2076227000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3424,11 +3422,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2069970472"/>
-        <c:axId val="2069967416"/>
+        <c:axId val="2047683912"/>
+        <c:axId val="2047065464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2069970472"/>
+        <c:axId val="2047683912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3450,7 +3448,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2069967416"/>
+        <c:crossAx val="2047065464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3458,7 +3456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2069967416"/>
+        <c:axId val="2047065464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3507,7 +3505,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2069970472"/>
+        <c:crossAx val="2047683912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3754,11 +3752,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2069917320"/>
-        <c:axId val="2069914328"/>
+        <c:axId val="2082363800"/>
+        <c:axId val="2047694616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2069917320"/>
+        <c:axId val="2082363800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3780,7 +3778,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2069914328"/>
+        <c:crossAx val="2047694616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3788,7 +3786,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2069914328"/>
+        <c:axId val="2047694616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3833,7 +3831,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2069917320"/>
+        <c:crossAx val="2082363800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4167,11 +4165,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2076639112"/>
-        <c:axId val="2076635832"/>
+        <c:axId val="2087055976"/>
+        <c:axId val="2087059240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2076639112"/>
+        <c:axId val="2087055976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4193,7 +4191,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2076635832"/>
+        <c:crossAx val="2087059240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4201,7 +4199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2076635832"/>
+        <c:axId val="2087059240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4256,7 +4254,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2076639112"/>
+        <c:crossAx val="2087055976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4527,11 +4525,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2083983672"/>
-        <c:axId val="2081339752"/>
+        <c:axId val="2087000808"/>
+        <c:axId val="2086941048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2083983672"/>
+        <c:axId val="2087000808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4553,7 +4551,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081339752"/>
+        <c:crossAx val="2086941048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4561,7 +4559,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081339752"/>
+        <c:axId val="2086941048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4616,7 +4614,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2083983672"/>
+        <c:crossAx val="2087000808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22031,92 +22029,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="47" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="1">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I54:K65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
@@ -22203,6 +22115,92 @@
   <dataFields count="2">
     <dataField name="Mittelwert - Kraken" fld="2" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Kraken2" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="47" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
     <format dxfId="2">
@@ -22578,7 +22576,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="M1:Q19" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -22770,7 +22768,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="M1:O5" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -22913,7 +22911,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-india" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1bj_results" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22921,7 +22919,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1bj_results" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-india" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23563,16 +23561,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="62" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
@@ -53036,7 +53034,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -53055,13 +53053,13 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="67" t="s">
         <v>202</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="2" t="s">
         <v>152</v>
       </c>
@@ -53245,8 +53243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="P66" sqref="P66"/>
+    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
+      <selection activeCell="P65" sqref="P65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -53816,11 +53814,11 @@
       <c r="S14" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="T14" s="64" t="s">
+      <c r="T14" s="67" t="s">
         <v>138</v>
       </c>
-      <c r="U14" s="64"/>
-      <c r="V14" s="64"/>
+      <c r="U14" s="67"/>
+      <c r="V14" s="67"/>
     </row>
     <row r="15" spans="1:22" ht="30">
       <c r="A15">
@@ -57761,7 +57759,7 @@
   <dimension ref="A1:Q70"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -57935,7 +57933,7 @@
         <v>209</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K38" si="0">G3-F3</f>
+        <f t="shared" ref="K3:K18" si="0">G3-F3</f>
         <v>933.88354111000035</v>
       </c>
       <c r="M3" s="8" t="s">
@@ -58751,7 +58749,7 @@
         <v>225</v>
       </c>
       <c r="K19">
-        <f>G19-F19</f>
+        <f t="shared" ref="K19:K37" si="1">G19-F19</f>
         <v>22374.943838788942</v>
       </c>
       <c r="M19" s="8" t="s">
@@ -58802,7 +58800,7 @@
         <v>225</v>
       </c>
       <c r="K20">
-        <f>G20-F20</f>
+        <f t="shared" si="1"/>
         <v>13303.522331999719</v>
       </c>
     </row>
@@ -58838,7 +58836,7 @@
         <v>225</v>
       </c>
       <c r="K21">
-        <f>G21-F21</f>
+        <f t="shared" si="1"/>
         <v>9594.9391710790896</v>
       </c>
     </row>
@@ -58874,7 +58872,7 @@
         <v>225</v>
       </c>
       <c r="K22">
-        <f>G22-F22</f>
+        <f t="shared" si="1"/>
         <v>9349.9229609940012</v>
       </c>
     </row>
@@ -58910,7 +58908,7 @@
         <v>225</v>
       </c>
       <c r="K23">
-        <f>G23-F23</f>
+        <f t="shared" si="1"/>
         <v>9113.4127750361004</v>
       </c>
     </row>
@@ -58946,7 +58944,7 @@
         <v>227</v>
       </c>
       <c r="K24">
-        <f>G24-F24</f>
+        <f t="shared" si="1"/>
         <v>633.34758210199993</v>
       </c>
     </row>
@@ -58982,7 +58980,7 @@
         <v>227</v>
       </c>
       <c r="K25">
-        <f>G25-F25</f>
+        <f t="shared" si="1"/>
         <v>643.50944089900008</v>
       </c>
     </row>
@@ -59018,7 +59016,7 @@
         <v>227</v>
       </c>
       <c r="K26">
-        <f>G26-F26</f>
+        <f t="shared" si="1"/>
         <v>627.13998198499996</v>
       </c>
     </row>
@@ -59054,7 +59052,7 @@
         <v>227</v>
       </c>
       <c r="K27">
-        <f>G27-F27</f>
+        <f t="shared" si="1"/>
         <v>675.16876912099997</v>
       </c>
     </row>
@@ -59090,7 +59088,7 @@
         <v>227</v>
       </c>
       <c r="K28">
-        <f>G28-F28</f>
+        <f t="shared" si="1"/>
         <v>692.32583999600001</v>
       </c>
     </row>
@@ -59126,7 +59124,7 @@
         <v>227</v>
       </c>
       <c r="K29">
-        <f>G29-F29</f>
+        <f t="shared" si="1"/>
         <v>671.6348509787</v>
       </c>
     </row>
@@ -59162,7 +59160,7 @@
         <v>227</v>
       </c>
       <c r="K30">
-        <f>G30-F30</f>
+        <f t="shared" si="1"/>
         <v>806.90279699000007</v>
       </c>
       <c r="M30" s="2" t="s">
@@ -59207,7 +59205,7 @@
         <v>227</v>
       </c>
       <c r="K31">
-        <f>G31-F31</f>
+        <f t="shared" si="1"/>
         <v>1117.3181481321001</v>
       </c>
       <c r="M31" t="s">
@@ -59252,7 +59250,7 @@
         <v>227</v>
       </c>
       <c r="K32">
-        <f>G32-F32</f>
+        <f t="shared" si="1"/>
         <v>786.79635190930003</v>
       </c>
       <c r="M32" t="s">
@@ -59297,7 +59295,7 @@
         <v>227</v>
       </c>
       <c r="K33">
-        <f>G33-F33</f>
+        <f t="shared" si="1"/>
         <v>1054.3560481059999</v>
       </c>
       <c r="M33" t="s">
@@ -59342,16 +59340,16 @@
         <v>227</v>
       </c>
       <c r="K34">
-        <f>G34-F34</f>
+        <f t="shared" si="1"/>
         <v>1065.497215033</v>
       </c>
       <c r="M34" t="s">
         <v>5</v>
       </c>
-      <c r="N34" s="65">
+      <c r="N34" s="60">
         <v>19192</v>
       </c>
-      <c r="O34" s="65">
+      <c r="O34" s="60">
         <v>2302</v>
       </c>
     </row>
@@ -59387,16 +59385,16 @@
         <v>227</v>
       </c>
       <c r="K35">
-        <f>G35-F35</f>
+        <f t="shared" si="1"/>
         <v>1066.6707761299999</v>
       </c>
       <c r="M35" t="s">
         <v>5</v>
       </c>
-      <c r="N35" s="65">
+      <c r="N35" s="60">
         <v>10262</v>
       </c>
-      <c r="O35" s="65">
+      <c r="O35" s="60">
         <v>2165</v>
       </c>
     </row>
@@ -59432,7 +59430,7 @@
         <v>227</v>
       </c>
       <c r="K36">
-        <f>G36-F36</f>
+        <f t="shared" si="1"/>
         <v>2479.8451061257001</v>
       </c>
       <c r="M36" s="2" t="s">
@@ -59479,7 +59477,7 @@
         <v>227</v>
       </c>
       <c r="K37">
-        <f>G37-F37</f>
+        <f t="shared" si="1"/>
         <v>1616.6285648319999</v>
       </c>
       <c r="M37" s="2" t="s">
@@ -60889,10 +60887,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:Z75"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="Z31" sqref="Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -60999,7 +60997,7 @@
       <c r="F6" s="47">
         <v>11460.578475336322</v>
       </c>
-      <c r="G6" s="67">
+      <c r="G6" s="62">
         <f>'BJ w Staging'!N36</f>
         <v>8860.4</v>
       </c>
@@ -61031,7 +61029,7 @@
       <c r="F7" s="21">
         <v>906</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="61">
         <f>'BJ w Staging'!O36</f>
         <v>2598.8000000000002</v>
       </c>
@@ -61291,7 +61289,7 @@
         <v>19.215277777777779</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:26">
       <c r="A17" s="2" t="s">
         <v>244</v>
       </c>
@@ -61324,7 +61322,7 @@
         <v>24.56504025566889</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:26">
       <c r="A18" s="2" t="s">
         <v>270</v>
       </c>
@@ -61357,7 +61355,7 @@
         <v>5.3497624778911117</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:26">
       <c r="A19" t="s">
         <v>130</v>
       </c>
@@ -61390,7 +61388,7 @@
         <v>145.56221155583333</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:26">
       <c r="A20" t="s">
         <v>138</v>
       </c>
@@ -61423,7 +61421,7 @@
         <v>20.849802584910968</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:26">
       <c r="A21" t="s">
         <v>194</v>
       </c>
@@ -61456,7 +61454,7 @@
         <v>30.06859433361112</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:26">
       <c r="A22" s="2" t="s">
         <v>242</v>
       </c>
@@ -61489,7 +61487,7 @@
         <v>140.0586574778911</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:26">
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
       <c r="D23" s="31"/>
@@ -61498,7 +61496,7 @@
       <c r="G23" s="51"/>
       <c r="H23" s="49"/>
     </row>
-    <row r="24" spans="1:8" ht="16" thickBot="1">
+    <row r="24" spans="1:26" ht="16" thickBot="1">
       <c r="A24" s="27"/>
       <c r="B24" s="33"/>
       <c r="C24" s="29"/>
@@ -61508,7 +61506,7 @@
       <c r="G24" s="33"/>
       <c r="H24" s="29"/>
     </row>
-    <row r="25" spans="1:8" ht="16" thickTop="1">
+    <row r="25" spans="1:26" ht="16" thickTop="1">
       <c r="A25" t="s">
         <v>192</v>
       </c>
@@ -61532,7 +61530,7 @@
       <c r="G25" s="3"/>
       <c r="H25" s="28"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:26">
       <c r="A26" t="s">
         <v>193</v>
       </c>
@@ -61556,7 +61554,7 @@
       <c r="G26" s="3"/>
       <c r="H26" s="28"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:26">
       <c r="A27" t="s">
         <v>195</v>
       </c>
@@ -61580,7 +61578,7 @@
       <c r="G27" s="3"/>
       <c r="H27" s="28"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:26">
       <c r="A28" t="s">
         <v>265</v>
       </c>
@@ -61613,10 +61611,16 @@
         <v>3.6752412736179879E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:26">
       <c r="D29">
         <f>D21/B21</f>
         <v>1.7961588736305956</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="Z30">
+        <f>108/212</f>
+        <v>0.50943396226415094</v>
       </c>
     </row>
     <row r="41" spans="2:11">

</xml_diff>

<commit_message>
added scenarios Bx and Cx to figure captions
git-svn-id: file://localhost/tmp/svn2git/svn@7544 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="50380" windowHeight="28360" tabRatio="500" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="50380" windowHeight="28000" tabRatio="500" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -1084,15 +1084,6 @@
     <t>Time 2</t>
   </si>
   <si>
-    <t>XSEDE:Trestles/FG</t>
-  </si>
-  <si>
-    <t>EGI/FG</t>
-  </si>
-  <si>
-    <t>XSEDE:QB/OSG</t>
-  </si>
-  <si>
     <t>Stddev 1</t>
   </si>
   <si>
@@ -1103,6 +1094,18 @@
   </si>
   <si>
     <t>adjusted with staging 80 min (OSG-QB)</t>
+  </si>
+  <si>
+    <t>XSEDE:QB/OSG
+(C3)</t>
+  </si>
+  <si>
+    <t>EGI/FG 
+(C2)</t>
+  </si>
+  <si>
+    <t>XSEDE:Trestles/FG
+(C1)</t>
   </si>
 </sst>
 </file>
@@ -2064,11 +2067,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2047437864"/>
-        <c:axId val="2047440888"/>
+        <c:axId val="2120557016"/>
+        <c:axId val="2120559928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2047437864"/>
+        <c:axId val="2120557016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2078,7 +2081,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047440888"/>
+        <c:crossAx val="2120559928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2086,7 +2089,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2047440888"/>
+        <c:axId val="2120559928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2097,7 +2100,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2047437864"/>
+        <c:crossAx val="2120557016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2395,11 +2398,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2084449544"/>
-        <c:axId val="2083475400"/>
+        <c:axId val="2120644680"/>
+        <c:axId val="2120650440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2084449544"/>
+        <c:axId val="2120644680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2432,7 +2435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083475400"/>
+        <c:crossAx val="2120650440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2440,7 +2443,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083475400"/>
+        <c:axId val="2120650440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,7 +2454,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2084449544"/>
+        <c:crossAx val="2120644680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2763,11 +2766,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2082443384"/>
-        <c:axId val="2082449112"/>
+        <c:axId val="2085741896"/>
+        <c:axId val="2085736168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2082443384"/>
+        <c:axId val="2085741896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2800,7 +2803,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082449112"/>
+        <c:crossAx val="2085736168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2808,7 +2811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2082449112"/>
+        <c:axId val="2085736168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2837,7 +2840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2082443384"/>
+        <c:crossAx val="2085741896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3103,11 +3106,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2076227000"/>
-        <c:axId val="2076893672"/>
+        <c:axId val="2120751560"/>
+        <c:axId val="2120754248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2076227000"/>
+        <c:axId val="2120751560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3129,7 +3132,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2076893672"/>
+        <c:crossAx val="2120754248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3137,7 +3140,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2076893672"/>
+        <c:axId val="2120754248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180.0"/>
@@ -3174,7 +3177,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3194,7 +3196,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2076227000"/>
+        <c:crossAx val="2120751560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3206,7 +3208,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3422,11 +3423,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2047683912"/>
-        <c:axId val="2047065464"/>
+        <c:axId val="2120788520"/>
+        <c:axId val="2120791560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2047683912"/>
+        <c:axId val="2120788520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3448,7 +3449,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2047065464"/>
+        <c:crossAx val="2120791560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3456,7 +3457,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2047065464"/>
+        <c:axId val="2120791560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -3485,7 +3486,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3505,14 +3505,13 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2047683912"/>
+        <c:crossAx val="2120788520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3752,11 +3751,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2082363800"/>
-        <c:axId val="2047694616"/>
+        <c:axId val="2120841208"/>
+        <c:axId val="2120844184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2082363800"/>
+        <c:axId val="2120841208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3778,7 +3777,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2047694616"/>
+        <c:crossAx val="2120844184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3786,7 +3785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2047694616"/>
+        <c:axId val="2120844184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3811,7 +3810,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
@@ -3831,14 +3829,13 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2082363800"/>
+        <c:crossAx val="2120841208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -4165,11 +4162,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2087055976"/>
-        <c:axId val="2087059240"/>
+        <c:axId val="2120926840"/>
+        <c:axId val="2120930104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087055976"/>
+        <c:axId val="2120926840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4191,7 +4188,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2087059240"/>
+        <c:crossAx val="2120930104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4199,7 +4196,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2087059240"/>
+        <c:axId val="2120930104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4254,7 +4251,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2087055976"/>
+        <c:crossAx val="2120926840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4387,13 +4384,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>XSEDE:Trestles/FG</c:v>
+                  <c:v>XSEDE:Trestles/FG_x000d_(C1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>EGI/FG</c:v>
+                  <c:v>EGI/FG _x000d_(C2)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>XSEDE:QB/OSG</c:v>
+                  <c:v>XSEDE:QB/OSG_x000d_(C3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4486,13 +4483,13 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>XSEDE:Trestles/FG</c:v>
+                  <c:v>XSEDE:Trestles/FG_x000d_(C1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>EGI/FG</c:v>
+                  <c:v>EGI/FG _x000d_(C2)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>XSEDE:QB/OSG</c:v>
+                  <c:v>XSEDE:QB/OSG_x000d_(C3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4525,11 +4522,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2087000808"/>
-        <c:axId val="2086941048"/>
+        <c:axId val="2120966056"/>
+        <c:axId val="2120968920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2087000808"/>
+        <c:axId val="2120966056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4551,7 +4548,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2086941048"/>
+        <c:crossAx val="2120968920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4559,7 +4556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2086941048"/>
+        <c:axId val="2120968920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4614,7 +4611,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2087000808"/>
+        <c:crossAx val="2120966056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22029,6 +22026,92 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="5"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="47" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="1">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="I54:K65" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="3">
@@ -22115,92 +22198,6 @@
   <dataFields count="2">
     <dataField name="Mittelwert - Kraken" fld="2" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Kraken2" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="1">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="I33:K41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="7">
-        <item x="5"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="47" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Mittelwert - India" fld="2" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - India" fld="2" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
     <format dxfId="2">
@@ -22911,7 +22908,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1bj_results" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-india" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22919,7 +22916,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bj-india" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1bj_results" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53243,8 +53240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
-      <selection activeCell="P65" sqref="P65"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="O64" sqref="O64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -54483,15 +54480,15 @@
         <v>291</v>
       </c>
       <c r="R62" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="S62" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="63" spans="15:20">
-      <c r="O63" t="s">
-        <v>292</v>
+        <v>293</v>
+      </c>
+    </row>
+    <row r="63" spans="15:20" ht="30">
+      <c r="O63" s="44" t="s">
+        <v>298</v>
       </c>
       <c r="P63" s="16">
         <f>'BJ (FG-XSEDE)'!N4/60</f>
@@ -54510,9 +54507,9 @@
         <v>21.99622082922189</v>
       </c>
     </row>
-    <row r="64" spans="15:20">
-      <c r="O64" t="s">
-        <v>293</v>
+    <row r="64" spans="15:20" ht="30">
+      <c r="O64" s="44" t="s">
+        <v>297</v>
       </c>
       <c r="P64" s="16">
         <f>'Interop EGI-FG'!P8/60</f>
@@ -54531,12 +54528,12 @@
         <v>7.2283591617497303</v>
       </c>
       <c r="T64" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="65" spans="15:20">
-      <c r="O65" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="65" spans="15:20" ht="30">
+      <c r="O65" s="44" t="s">
+        <v>296</v>
       </c>
       <c r="P65" s="16">
         <f>'Interop OSG-XSEDE'!F11/60+80</f>
@@ -54555,7 +54552,7 @@
         <v>21.833971046666402</v>
       </c>
       <c r="T65" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" spans="15:20">

</xml_diff>

<commit_message>
added some description and reference to Venus C
git-svn-id: file://localhost/tmp/svn2git/svn@7547 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/troy/pstar/perf/interop/pj-interop.xlsx
+++ b/papers/troy/pstar/perf/interop/pj-interop.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="50380" windowHeight="28000" tabRatio="500" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="50380" windowHeight="28000" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BFAST" sheetId="1" r:id="rId1"/>
@@ -1017,24 +1017,6 @@
     <t>Overhead</t>
   </si>
   <si>
-    <t>DIANE/EGI</t>
-  </si>
-  <si>
-    <t>BigJob/XSEDE (Trestles)</t>
-  </si>
-  <si>
-    <t>BigJob/FG
- (India)</t>
-  </si>
-  <si>
-    <t>BigJob/FG 
-(India/Sierra)</t>
-  </si>
-  <si>
-    <t>GlideInWMS/
-OSG</t>
-  </si>
-  <si>
     <t>XSEDE:Trestles/
 FutureGrid</t>
   </si>
@@ -1106,6 +1088,28 @@
   <si>
     <t>XSEDE:Trestles/FG
 (C1)</t>
+  </si>
+  <si>
+    <t>BigJob/FG 
+(India/Sierra) (B3)</t>
+  </si>
+  <si>
+    <t>GlideInWMS/
+OSG 
+(B5)</t>
+  </si>
+  <si>
+    <t>BigJob/FG
+ (India)
+(B2)</t>
+  </si>
+  <si>
+    <t>BigJob/XSEDE (Trestles) 
+(B1)</t>
+  </si>
+  <si>
+    <t>DIANE/EGI 
+(B4)</t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1582,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1623,9 +1627,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1952,6 +1953,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2429,6 +2431,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2906,10 +2909,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DIANE/EGI</c:v>
+                  <c:v>DIANE/EGI _x000d_(B4)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>GlideInWMS/_x000d_OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG _x000d_(B5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2963,10 +2966,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DIANE/EGI</c:v>
+                  <c:v>DIANE/EGI _x000d_(B4)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>GlideInWMS/_x000d_OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG _x000d_(B5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3066,10 +3069,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DIANE/EGI</c:v>
+                  <c:v>DIANE/EGI _x000d_(B4)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>GlideInWMS/_x000d_OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG _x000d_(B5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3177,6 +3180,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3208,6 +3212,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3285,10 +3290,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DIANE/EGI</c:v>
+                  <c:v>DIANE/EGI _x000d_(B4)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>GlideInWMS/_x000d_OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG _x000d_(B5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3334,10 +3339,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DIANE/EGI</c:v>
+                  <c:v>DIANE/EGI _x000d_(B4)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>GlideInWMS/_x000d_OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG _x000d_(B5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3383,10 +3388,10 @@
                   <c:v>FutureGrid</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>DIANE/EGI</c:v>
+                  <c:v>DIANE/EGI _x000d_(B4)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>GlideInWMS/_x000d_OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG _x000d_(B5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3486,6 +3491,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3512,6 +3518,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3584,19 +3591,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>BigJob/XSEDE (Trestles)</c:v>
+                  <c:v>BigJob/XSEDE (Trestles) _x000d_(B1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BigJob/FG_x000d_ (India)</c:v>
+                  <c:v>BigJob/FG_x000d_ (India)_x000d_(B2)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BigJob/FG _x000d_(India/Sierra)</c:v>
+                  <c:v>BigJob/FG _x000d_(India/Sierra) (B3)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>DIANE/EGI</c:v>
+                  <c:v>DIANE/EGI _x000d_(B4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>GlideInWMS/_x000d_OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG _x000d_(B5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3699,19 +3706,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>BigJob/XSEDE (Trestles)</c:v>
+                  <c:v>BigJob/XSEDE (Trestles) _x000d_(B1)</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BigJob/FG_x000d_ (India)</c:v>
+                  <c:v>BigJob/FG_x000d_ (India)_x000d_(B2)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>BigJob/FG _x000d_(India/Sierra)</c:v>
+                  <c:v>BigJob/FG _x000d_(India/Sierra) (B3)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>DIANE/EGI</c:v>
+                  <c:v>DIANE/EGI _x000d_(B4)</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>GlideInWMS/_x000d_OSG</c:v>
+                  <c:v>GlideInWMS/_x000d_OSG _x000d_(B5)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3810,6 +3817,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
@@ -3836,6 +3844,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -23558,16 +23567,16 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="28">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
@@ -52990,7 +52999,7 @@
         <f t="shared" si="0"/>
         <v>1235.8584735619688</v>
       </c>
-      <c r="O8" s="42" t="s">
+      <c r="O8" s="41" t="s">
         <v>131</v>
       </c>
       <c r="P8">
@@ -53050,13 +53059,13 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="66" t="s">
         <v>202</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
       <c r="F3" s="2" t="s">
         <v>152</v>
       </c>
@@ -53085,13 +53094,13 @@
       <c r="A5">
         <v>748</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="42">
         <v>4202</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="42">
         <v>2475</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="42">
         <v>2991</v>
       </c>
       <c r="E5">
@@ -53106,10 +53115,10 @@
       <c r="A6">
         <v>854</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="42">
         <v>1582</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="42">
         <v>1218</v>
       </c>
       <c r="D6">
@@ -53127,10 +53136,10 @@
       <c r="A7">
         <v>880</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="42">
         <v>1526</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="42">
         <v>1203</v>
       </c>
       <c r="D7">
@@ -53148,10 +53157,10 @@
       <c r="A8">
         <v>763</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="42">
         <v>1643</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="42">
         <v>1203</v>
       </c>
       <c r="D8">
@@ -53170,7 +53179,7 @@
         <f>AVERAGE(A5:A9)</f>
         <v>811.25</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <f t="shared" ref="B11:F11" si="0">AVERAGE(B5:B9)</f>
         <v>2238.25</v>
       </c>
@@ -53186,7 +53195,7 @@
         <f t="shared" si="0"/>
         <v>446.75</v>
       </c>
-      <c r="F11" s="46">
+      <c r="F11" s="45">
         <f t="shared" si="0"/>
         <v>5190</v>
       </c>
@@ -53240,7 +53249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="O64" sqref="O64"/>
     </sheetView>
   </sheetViews>
@@ -53799,10 +53808,10 @@
       <c r="J14" t="s">
         <v>47</v>
       </c>
-      <c r="P14" s="45" t="s">
+      <c r="P14" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="Q14" s="45" t="s">
+      <c r="Q14" s="44" t="s">
         <v>152</v>
       </c>
       <c r="R14" s="2" t="s">
@@ -53811,11 +53820,11 @@
       <c r="S14" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="T14" s="67" t="s">
+      <c r="T14" s="66" t="s">
         <v>138</v>
       </c>
-      <c r="U14" s="67"/>
-      <c r="V14" s="67"/>
+      <c r="U14" s="66"/>
+      <c r="V14" s="66"/>
     </row>
     <row r="15" spans="1:22" ht="30">
       <c r="A15">
@@ -53848,24 +53857,24 @@
       <c r="J15" t="s">
         <v>28</v>
       </c>
-      <c r="O15" s="41" t="s">
+      <c r="O15" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="P15" s="39">
+      <c r="P15" s="38">
         <f>Q8/60</f>
         <v>15.752848429242707</v>
       </c>
-      <c r="Q15" s="39">
+      <c r="Q15" s="38">
         <f>Q9/60-P15</f>
         <v>7.5963283108795174</v>
       </c>
-      <c r="R15" s="40">
+      <c r="R15" s="39">
         <v>0</v>
       </c>
       <c r="S15">
         <v>0</v>
       </c>
-      <c r="T15" s="40">
+      <c r="T15" s="39">
         <f>T9/60</f>
         <v>1.3298815950546723</v>
       </c>
@@ -53905,7 +53914,7 @@
       <c r="J16" t="s">
         <v>47</v>
       </c>
-      <c r="O16" s="41" t="s">
+      <c r="O16" s="40" t="s">
         <v>197</v>
       </c>
       <c r="P16" s="15">
@@ -53915,14 +53924,14 @@
       <c r="Q16">
         <v>0</v>
       </c>
-      <c r="R16" s="38">
+      <c r="R16" s="37">
         <f>'Interop EGI-FG'!P8/60-P16</f>
         <v>49.858385546089515</v>
       </c>
       <c r="S16">
         <v>0</v>
       </c>
-      <c r="T16" s="40"/>
+      <c r="T16" s="39"/>
       <c r="U16">
         <f>'Interop EGI-FG'!P9/60</f>
         <v>5.8872795343029933</v>
@@ -53959,7 +53968,7 @@
       <c r="J17" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="44" t="s">
+      <c r="O17" s="43" t="s">
         <v>206</v>
       </c>
       <c r="P17">
@@ -54008,8 +54017,8 @@
       <c r="J18" t="s">
         <v>47</v>
       </c>
-      <c r="O18" s="44" t="s">
-        <v>276</v>
+      <c r="O18" s="43" t="s">
+        <v>271</v>
       </c>
       <c r="P18" s="15">
         <f>'BJ (FG-XSEDE)'!N3/60</f>
@@ -54474,27 +54483,27 @@
     </row>
     <row r="62" spans="15:20">
       <c r="P62" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="Q62" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="R62" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="S62" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="63" spans="15:20" ht="30">
+      <c r="O63" s="43" t="s">
         <v>293</v>
-      </c>
-    </row>
-    <row r="63" spans="15:20" ht="30">
-      <c r="O63" s="44" t="s">
-        <v>298</v>
       </c>
       <c r="P63" s="16">
         <f>'BJ (FG-XSEDE)'!N4/60</f>
         <v>79.031930377808905</v>
       </c>
-      <c r="Q63" s="47">
+      <c r="Q63" s="46">
         <f>'BJ (FG-XSEDE)'!N3/60</f>
         <v>107.65214067827169</v>
       </c>
@@ -54508,8 +54517,8 @@
       </c>
     </row>
     <row r="64" spans="15:20" ht="30">
-      <c r="O64" s="44" t="s">
-        <v>297</v>
+      <c r="O64" s="43" t="s">
+        <v>292</v>
       </c>
       <c r="P64" s="16">
         <f>'Interop EGI-FG'!P8/60</f>
@@ -54528,12 +54537,12 @@
         <v>7.2283591617497303</v>
       </c>
       <c r="T64" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" spans="15:20" ht="30">
-      <c r="O65" s="44" t="s">
-        <v>296</v>
+      <c r="O65" s="43" t="s">
+        <v>291</v>
       </c>
       <c r="P65" s="16">
         <f>'Interop OSG-XSEDE'!F11/60+80</f>
@@ -54552,7 +54561,7 @@
         <v>21.833971046666402</v>
       </c>
       <c r="T65" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="68" spans="15:20">
@@ -58806,7 +58815,7 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C21">
         <v>128</v>
@@ -58842,7 +58851,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C22">
         <v>128</v>
@@ -58878,7 +58887,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C23">
         <v>128</v>
@@ -59161,10 +59170,10 @@
         <v>806.90279699000007</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="O30" s="2" t="s">
         <v>262</v>
@@ -59343,10 +59352,10 @@
       <c r="M34" t="s">
         <v>5</v>
       </c>
-      <c r="N34" s="60">
+      <c r="N34" s="59">
         <v>19192</v>
       </c>
-      <c r="O34" s="60">
+      <c r="O34" s="59">
         <v>2302</v>
       </c>
     </row>
@@ -59388,10 +59397,10 @@
       <c r="M35" t="s">
         <v>5</v>
       </c>
-      <c r="N35" s="60">
+      <c r="N35" s="59">
         <v>10262</v>
       </c>
-      <c r="O35" s="60">
+      <c r="O35" s="59">
         <v>2165</v>
       </c>
     </row>
@@ -59431,7 +59440,7 @@
         <v>2479.8451061257001</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="N36" s="2">
         <f>AVERAGE(N31:N35)</f>
@@ -59480,11 +59489,11 @@
       <c r="M37" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="N37" s="52">
+      <c r="N37" s="51">
         <f>STDEV(N31:N35)</f>
         <v>6218.6134145804563</v>
       </c>
-      <c r="O37" s="52">
+      <c r="O37" s="51">
         <f>STDEV(O31:O35)</f>
         <v>338.900722926345</v>
       </c>
@@ -59622,7 +59631,7 @@
         <v>0</v>
       </c>
       <c r="B68" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C68">
         <v>128</v>
@@ -59654,7 +59663,7 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C69">
         <v>128</v>
@@ -59686,7 +59695,7 @@
         <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C70">
         <v>128</v>
@@ -60056,11 +60065,11 @@
       <c r="M8" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="N8" s="52">
+      <c r="N8" s="51">
         <f>AVERAGE(N4:N6)</f>
         <v>330.21324467653335</v>
       </c>
-      <c r="O8" s="52">
+      <c r="O8" s="51">
         <f>AVERAGE(O4:O6)</f>
         <v>8733.732693349999</v>
       </c>
@@ -60285,11 +60294,11 @@
       </c>
     </row>
     <row r="21" spans="13:15" ht="16" thickBot="1">
-      <c r="M21" s="53"/>
-      <c r="N21" s="54">
+      <c r="M21" s="52"/>
+      <c r="N21" s="53">
         <v>6234.875</v>
       </c>
-      <c r="O21" s="54">
+      <c r="O21" s="53">
         <v>1280.515625</v>
       </c>
     </row>
@@ -60297,11 +60306,11 @@
       <c r="M22" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="N22" s="52">
+      <c r="N22" s="51">
         <f>AVERAGE(N16:N21)</f>
         <v>6929.617033333333</v>
       </c>
-      <c r="O22" s="52">
+      <c r="O22" s="51">
         <f>AVERAGE(O16:O21)</f>
         <v>1152.9166666666667</v>
       </c>
@@ -60310,11 +60319,11 @@
       <c r="M23" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="N23" s="52">
+      <c r="N23" s="51">
         <f>STDEV(N16:N21)</f>
         <v>1220.3487605097328</v>
       </c>
-      <c r="O23" s="52">
+      <c r="O23" s="51">
         <f>STDEV(O16:O21)</f>
         <v>140.23939620769141</v>
       </c>
@@ -60715,16 +60724,16 @@
       <c r="A7">
         <v>962</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="42">
         <v>2830</v>
       </c>
       <c r="C7">
         <v>872</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="42">
         <v>2711</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="42">
         <v>4697</v>
       </c>
       <c r="F7" s="15">
@@ -60739,16 +60748,16 @@
       <c r="A8">
         <v>826</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="42">
         <v>1978</v>
       </c>
       <c r="C8">
         <v>190</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="42">
         <v>1994</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="42">
         <v>3129</v>
       </c>
       <c r="F8" s="15">
@@ -60841,13 +60850,13 @@
       <c r="A18">
         <v>962</v>
       </c>
-      <c r="B18" s="43">
+      <c r="B18" s="42">
         <v>4697</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="42">
         <v>2830</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="42">
         <v>2711</v>
       </c>
       <c r="E18">
@@ -60858,13 +60867,13 @@
       <c r="A19">
         <v>826</v>
       </c>
-      <c r="B19" s="43">
+      <c r="B19" s="42">
         <v>3129</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19" s="42">
         <v>1978</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="42">
         <v>1994</v>
       </c>
       <c r="E19">
@@ -60886,8 +60895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z75"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="Z31" sqref="Z31"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="T120" sqref="T120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -60906,7 +60915,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2"/>
-      <c r="G2" s="50"/>
+      <c r="G2" s="49"/>
       <c r="K2" s="2" t="s">
         <v>155</v>
       </c>
@@ -60916,7 +60925,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30">
+    <row r="4" spans="1:11" ht="45">
       <c r="A4" s="10"/>
       <c r="B4" s="18" t="s">
         <v>152</v>
@@ -60924,20 +60933,20 @@
       <c r="C4" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="34" t="s">
-        <v>271</v>
-      </c>
-      <c r="E4" s="59" t="s">
-        <v>275</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="G4" s="58" t="s">
-        <v>273</v>
-      </c>
-      <c r="H4" s="59" t="s">
-        <v>274</v>
+      <c r="D4" s="57" t="s">
+        <v>298</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>295</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>297</v>
+      </c>
+      <c r="G4" s="57" t="s">
+        <v>296</v>
+      </c>
+      <c r="H4" s="58" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -60952,7 +60961,7 @@
         <f>BigJob!N28</f>
         <v>101.09102939799999</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="34">
         <f>Diane!B10</f>
         <v>3167.4118819999999</v>
       </c>
@@ -60964,7 +60973,7 @@
         <f>'BJ w Staging'!N10</f>
         <v>16715.026063703332</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="34">
         <f>'BJ w Staging'!N12</f>
         <v>21.005163240430001</v>
       </c>
@@ -60983,7 +60992,7 @@
       <c r="C6" s="10">
         <v>0</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="35">
         <f>Diane!C10</f>
         <v>4707.850641</v>
       </c>
@@ -60991,14 +61000,14 @@
         <f>Condor!C9</f>
         <v>5736.0000000000027</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="46">
         <v>11460.578475336322</v>
       </c>
-      <c r="G6" s="62">
+      <c r="G6" s="61">
         <f>'BJ w Staging'!N36</f>
         <v>8860.4</v>
       </c>
-      <c r="H6" s="55">
+      <c r="H6" s="54">
         <f>'BJ (FG multi)'!N22</f>
         <v>6929.617033333333</v>
       </c>
@@ -61015,7 +61024,7 @@
         <f>BFAST!J39*60*60*24</f>
         <v>1068.8906250000002</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="36">
         <f>Diane!D10</f>
         <v>809.39913009999998</v>
       </c>
@@ -61026,11 +61035,11 @@
       <c r="F7" s="21">
         <v>906</v>
       </c>
-      <c r="G7" s="61">
+      <c r="G7" s="60">
         <f>'BJ w Staging'!O36</f>
         <v>2598.8000000000002</v>
       </c>
-      <c r="H7" s="56">
+      <c r="H7" s="55">
         <f>'BJ (FG multi)'!O22</f>
         <v>1152.9166666666667</v>
       </c>
@@ -61047,7 +61056,7 @@
         <f>BigJob!Q28</f>
         <v>1695.8585478</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="36">
         <f>Diane!F10-Diane!E10</f>
         <v>8684.6616528400009</v>
       </c>
@@ -61059,7 +61068,7 @@
         <f>'BJ w Staging'!O10</f>
         <v>29086.213300733332</v>
       </c>
-      <c r="G8" s="37">
+      <c r="G8" s="36">
         <f>'BJ w Staging'!O12</f>
         <v>12768.35337882</v>
       </c>
@@ -61080,7 +61089,7 @@
         <f>BigJob!Z28</f>
         <v>267.5643732646929</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="36">
         <f>Diane!H11</f>
         <v>1384.7232681954761</v>
       </c>
@@ -61091,7 +61100,7 @@
       <c r="F9" s="21">
         <v>2102.3829270000001</v>
       </c>
-      <c r="G9" s="37">
+      <c r="G9" s="36">
         <f>'BJ w Staging'!Q12</f>
         <v>5649.9025447833619</v>
       </c>
@@ -61103,10 +61112,10 @@
     <row r="10" spans="1:11">
       <c r="B10" s="21"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="37"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="21"/>
       <c r="F10" s="21"/>
-      <c r="G10" s="37"/>
+      <c r="G10" s="36"/>
       <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:11" ht="16" thickBot="1">
@@ -61133,7 +61142,7 @@
         <f t="shared" si="0"/>
         <v>1.6848504899666665</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="36">
         <f t="shared" si="0"/>
         <v>52.790198033333333</v>
       </c>
@@ -61145,17 +61154,17 @@
         <f t="shared" ref="F12:G12" si="1">F5/60</f>
         <v>278.58376772838886</v>
       </c>
-      <c r="G12" s="37">
+      <c r="G12" s="36">
         <f t="shared" si="1"/>
         <v>0.35008605400716669</v>
       </c>
-      <c r="H12" s="57">
+      <c r="H12" s="56">
         <f t="shared" ref="H12" si="2">H5/60</f>
         <v>5.5035540779422227</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="47" t="s">
         <v>132</v>
       </c>
       <c r="B13" s="21">
@@ -61166,7 +61175,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="35">
         <f t="shared" si="0"/>
         <v>78.46417735</v>
       </c>
@@ -61178,7 +61187,7 @@
         <f t="shared" ref="F13:G13" si="3">F6/60</f>
         <v>191.00964125560537</v>
       </c>
-      <c r="G13" s="36">
+      <c r="G13" s="35">
         <f t="shared" si="3"/>
         <v>147.67333333333332</v>
       </c>
@@ -61199,7 +61208,7 @@
         <f>C19-C16-C12-C13</f>
         <v>8.7646148900333287</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="36">
         <f>D19-D16-D12-D13</f>
         <v>-4.333315928306547E-9</v>
       </c>
@@ -61211,7 +61220,7 @@
         <f>F19-F16-F12-F13</f>
         <v>7.6812694894584865E-2</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G14" s="36">
         <f t="shared" ref="G14:H14" si="5">G19-G16-G12-G13</f>
         <v>21.4691369263262</v>
       </c>
@@ -61232,7 +61241,7 @@
         <f>C12+C14</f>
         <v>10.449465379999996</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="36">
         <f>D12+D14</f>
         <v>52.790198029000017</v>
       </c>
@@ -61244,7 +61253,7 @@
         <f t="shared" ref="F15:H15" si="6">F12+F14</f>
         <v>278.66058042328348</v>
       </c>
-      <c r="G15" s="37">
+      <c r="G15" s="36">
         <f t="shared" si="6"/>
         <v>21.819222980333368</v>
       </c>
@@ -61265,7 +61274,7 @@
         <f>C7/60</f>
         <v>17.814843750000005</v>
       </c>
-      <c r="D16" s="37">
+      <c r="D16" s="36">
         <f>D7/60</f>
         <v>13.489985501666666</v>
       </c>
@@ -61277,7 +61286,7 @@
         <f t="shared" ref="F16:G16" si="7">F7/60</f>
         <v>15.1</v>
       </c>
-      <c r="G16" s="37">
+      <c r="G16" s="36">
         <f t="shared" si="7"/>
         <v>43.31333333333334</v>
       </c>
@@ -61310,7 +61319,7 @@
         <f>F19-F12-F13</f>
         <v>15.176812694894608</v>
       </c>
-      <c r="G17" s="37">
+      <c r="G17" s="36">
         <f t="shared" si="9"/>
         <v>64.782470259659533</v>
       </c>
@@ -61364,7 +61373,7 @@
         <f t="shared" si="11"/>
         <v>28.264309130000001</v>
       </c>
-      <c r="D19" s="37">
+      <c r="D19" s="36">
         <f t="shared" si="11"/>
         <v>144.74436088066668</v>
       </c>
@@ -61376,7 +61385,7 @@
         <f t="shared" si="11"/>
         <v>484.77022167888884</v>
       </c>
-      <c r="G19" s="37">
+      <c r="G19" s="36">
         <f t="shared" si="11"/>
         <v>212.80588964700001</v>
       </c>
@@ -61397,7 +61406,7 @@
         <f>C9/60</f>
         <v>4.4594062210782148</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D20" s="36">
         <f>D9/60</f>
         <v>23.078721136591266</v>
       </c>
@@ -61409,7 +61418,7 @@
         <f t="shared" ref="F20:G20" si="12">F9/60</f>
         <v>35.039715450000003</v>
       </c>
-      <c r="G20" s="37">
+      <c r="G20" s="36">
         <f t="shared" si="12"/>
         <v>94.165042413056028</v>
       </c>
@@ -61422,27 +61431,27 @@
       <c r="A21" t="s">
         <v>194</v>
       </c>
-      <c r="B21" s="37">
+      <c r="B21" s="36">
         <f>B15+B16</f>
         <v>36.901069556666677</v>
       </c>
-      <c r="C21" s="37">
+      <c r="C21" s="36">
         <f t="shared" ref="C21:E21" si="14">C15+C16</f>
         <v>28.264309130000001</v>
       </c>
-      <c r="D21" s="37">
+      <c r="D21" s="36">
         <f t="shared" si="14"/>
         <v>66.280183530666676</v>
       </c>
-      <c r="E21" s="37">
+      <c r="E21" s="36">
         <f t="shared" si="14"/>
         <v>27.022222222222226</v>
       </c>
-      <c r="F21" s="37">
+      <c r="F21" s="36">
         <f>F15+F16</f>
         <v>293.7605804232835</v>
       </c>
-      <c r="G21" s="37">
+      <c r="G21" s="36">
         <f>G15+G16</f>
         <v>65.132556313666711</v>
       </c>
@@ -61455,27 +61464,27 @@
       <c r="A22" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B22" s="37">
+      <c r="B22" s="36">
         <f>B19-B12</f>
         <v>35.614872297366674</v>
       </c>
-      <c r="C22" s="37">
+      <c r="C22" s="36">
         <f t="shared" ref="C22:G22" si="15">C19-C12</f>
         <v>26.579458640033334</v>
       </c>
-      <c r="D22" s="37">
+      <c r="D22" s="36">
         <f t="shared" si="15"/>
         <v>91.95416284733335</v>
       </c>
-      <c r="E22" s="37">
+      <c r="E22" s="36">
         <f t="shared" si="15"/>
         <v>110.75000000000006</v>
       </c>
-      <c r="F22" s="37">
+      <c r="F22" s="36">
         <f t="shared" si="15"/>
         <v>206.18645395049998</v>
       </c>
-      <c r="G22" s="37">
+      <c r="G22" s="36">
         <f t="shared" si="15"/>
         <v>212.45580359299285</v>
       </c>
@@ -61490,8 +61499,8 @@
       <c r="D23" s="31"/>
       <c r="E23" s="32"/>
       <c r="F23" s="32"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="49"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="1:26" ht="16" thickBot="1">
       <c r="A24" s="27"/>
@@ -64631,7 +64640,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C2">
         <v>64</v>
@@ -64668,7 +64677,7 @@
         <v>119</v>
       </c>
       <c r="O2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -64676,7 +64685,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C3">
         <v>64</v>
@@ -64721,7 +64730,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C4">
         <v>64</v>
@@ -64766,7 +64775,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C5">
         <v>64</v>
@@ -64811,7 +64820,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C6">
         <v>64</v>
@@ -64847,7 +64856,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C7">
         <v>64</v>

</xml_diff>